<commit_message>
-fixed an issue, where regulated taxonomy v2.1.0 had property keys missplaced for criterion #21. (GES-80 Jira issue)
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andreas Schmitz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Documents\NetBeansProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85F7FF5C-11DE-4202-9323-C550ED885A05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DF1B9A-FB26-4FD3-B969-01380062C794}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="588" firstSheet="29" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="588" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12447" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12443" uniqueCount="613">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3188,80 +3188,64 @@
     </xf>
   </cellXfs>
   <cellStyles count="112">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent1 2" xfId="54" xr:uid="{58EA2EC2-B9C9-47AD-9424-4145847963D4}"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2 2" xfId="55" xr:uid="{3D09D290-71F3-4E6E-A3A4-6E0D7E595C74}"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3 2" xfId="56" xr:uid="{33A4B671-0486-4AA5-AD35-1DE337A4D196}"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent4 2" xfId="57" xr:uid="{0CED6BA4-60EF-4640-ACAC-5491EFAA41B6}"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent5 2" xfId="58" xr:uid="{9711E678-D35B-4FDE-A1A2-62A8AD2BA356}"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent6 2" xfId="59" xr:uid="{7CA7835D-FCB7-402D-AC01-33C1572D9E8D}"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση6" xfId="39" builtinId="50" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent1 2" xfId="60" xr:uid="{F156E56A-1EB1-4208-BC29-CF6B998EA7A3}"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent2 2" xfId="61" xr:uid="{278057DE-C374-4BCB-BFCD-8FC15D932AF8}"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent3 2" xfId="62" xr:uid="{A54EAA7B-E320-4400-9E82-FA6F6AEFE3AC}"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent4 2" xfId="63" xr:uid="{CC5AD9F6-BA87-4F3F-A56B-CDCDACABDA15}"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent5 2" xfId="64" xr:uid="{207787DD-36B8-45D1-8027-AE3F706CF8B6}"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent6 2" xfId="65" xr:uid="{17547E8C-9F29-4A3C-9ED2-715309027EBC}"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent1 2" xfId="66" xr:uid="{40B95E25-5021-4D50-BD78-EF739646E98A}"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent2 2" xfId="67" xr:uid="{6E273BEA-D51E-4B50-8CF4-C2833969CE90}"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent3 2" xfId="68" xr:uid="{D51BC707-3D8B-4DDD-AE79-8DC5AB0B42C5}"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent4 2" xfId="69" xr:uid="{4A56C24B-3685-4CD1-A574-E40817E12F78}"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent5 2" xfId="70" xr:uid="{CCE7CC06-0A99-4475-96EE-A84CB6F4A3A5}"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent6 2" xfId="71" xr:uid="{3289F5EB-86A3-4274-AFFF-FD4F68731930}"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Akzent1 2" xfId="72" xr:uid="{5D4AEBF1-0A7C-4BFB-B180-EAF44EA9B0A0}"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Akzent2 2" xfId="73" xr:uid="{85CC1BEF-51DC-4570-B4A5-B17C34C9B97A}"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Akzent3 2" xfId="74" xr:uid="{B9E858DA-8B8C-4D0C-B338-C45F23F9086A}"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Akzent4 2" xfId="75" xr:uid="{457566C8-88EC-4A83-9182-F048E0B22D5B}"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Akzent5 2" xfId="76" xr:uid="{CF7F8E61-0EB1-4992-B9F6-7E1DE473F1D5}"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Akzent6 2" xfId="77" xr:uid="{CF8B57BC-427C-49FA-B00F-9FDC4AE226A3}"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Ausgabe 2" xfId="78" xr:uid="{A0801910-C56D-41DB-AA5B-D7B9CEA5154B}"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Berechnung 2" xfId="79" xr:uid="{41BDA43A-1ABB-4CE8-B9C1-27E91F26BF6C}"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Eingabe 2" xfId="80" xr:uid="{4E63FB11-C380-4C78-9E5D-ECEC7E1F665D}"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Ergebnis 2" xfId="81" xr:uid="{DD805113-7B66-4F6A-AC81-26589BA0D384}"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Erklärender Text 2" xfId="82" xr:uid="{A194B96E-6874-44FD-B943-01939BDA0BD2}"/>
     <cellStyle name="Erklärender Text 3" xfId="44" xr:uid="{3688BAA7-06B9-4333-8C0D-984DFDD1B2A1}"/>
     <cellStyle name="Excel Built-in Normal" xfId="50" xr:uid="{56DB3A1F-9D76-48AF-827F-04CDE3DA5590}"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Gut 2" xfId="83" xr:uid="{36A99347-B94D-4690-83AC-8C6CBD65002F}"/>
     <cellStyle name="Hipervínculo" xfId="42" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
     <cellStyle name="Hipervínculo visitado" xfId="103" xr:uid="{9051DEEC-FC84-4591-A8B5-638DE46C05EC}"/>
     <cellStyle name="Link 2" xfId="46" xr:uid="{74412CD5-81A4-4040-B22F-ED1B046355CD}"/>
     <cellStyle name="Link 2 2" xfId="51" xr:uid="{D14BD33F-0DCB-4F85-85A5-9BB7DDF8AB8C}"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Neutral 2" xfId="84" xr:uid="{1AD55C52-8BBF-476B-B40D-9E1715BBCCDF}"/>
     <cellStyle name="Normal 2" xfId="96" xr:uid="{A0210B32-A716-4DA1-8921-79BD6474A84A}"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Notiz 2" xfId="85" xr:uid="{96F7E845-1C7B-4930-A81D-0C72B5CBD2E5}"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Schlecht 2" xfId="86" xr:uid="{4CC925FC-A91B-432E-96A0-54E0F7C70564}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Standard 2" xfId="45" xr:uid="{4E059FDF-05CD-4388-BF86-76C2B6B0C261}"/>
     <cellStyle name="Standard 2 2" xfId="47" xr:uid="{E963BC3A-6088-4583-83FD-9423FD1ED1E0}"/>
     <cellStyle name="Standard 2 2 2" xfId="48" xr:uid="{B3E35E68-087C-47B8-B9C1-FA1C4CA6C8FA}"/>
@@ -3284,22 +3268,38 @@
     <cellStyle name="Standard 7" xfId="102" xr:uid="{744AB2FD-CA4D-461B-ABDD-66032D974148}"/>
     <cellStyle name="Standard 7 2" xfId="111" xr:uid="{E5E883CA-4D25-4EE5-AF23-D5DFF53989E9}"/>
     <cellStyle name="Style 1" xfId="52" xr:uid="{DF55E41B-F785-4866-85CE-BBB64E7F0959}"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 1 2" xfId="87" xr:uid="{22C91833-F9B6-4CA7-8F5F-BC0057EEF790}"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Überschrift 2 2" xfId="88" xr:uid="{CEF7EE81-7675-40F5-B163-07B4049BC735}"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Überschrift 3 2" xfId="89" xr:uid="{31D47085-7A55-424D-9C36-8209503C4B54}"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Überschrift 4 2" xfId="90" xr:uid="{FC1EF9AA-1E48-4C68-A18A-465057A10BD0}"/>
     <cellStyle name="Überschrift 5" xfId="91" xr:uid="{77E8198C-A64B-454E-9437-C7F654B906EC}"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Verknüpfte Zelle 2" xfId="92" xr:uid="{75D6E79A-C9C3-4688-BF38-48D65D7888B4}"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Warnender Text 2" xfId="93" xr:uid="{B95B2F27-4BD2-47FB-BFB4-0373AACBC00D}"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen 2" xfId="94" xr:uid="{CC6AF966-5680-457A-B96D-078ED43C1691}"/>
+    <cellStyle name="Εισαγωγή" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Έλεγχος κελιού" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Έμφαση1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Έμφαση2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Έμφαση3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Έμφαση4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Έμφαση5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Έμφαση6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Έξοδος" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Επεξηγηματικό κείμενο" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Κακό" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Καλό" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Ουδέτερο" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Προειδοποιητικό κείμενο" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Σημείωση" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Συνδεδεμένο κελί" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Σύνολο" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Τίτλος" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Υπολογισμός" xfId="11" builtinId="22" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -5366,7 +5366,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5693,23 +5693,23 @@
       <selection activeCell="AA123" sqref="AA123:AB123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.7109375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="3.85546875" style="25" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="3.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="17.140625" style="25" customWidth="1"/>
-    <col min="21" max="21" width="13.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="17.140625" style="87" customWidth="1"/>
-    <col min="24" max="25" width="17.140625" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="2.83984375" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.68359375" style="25" customWidth="1"/>
+    <col min="8" max="8" width="2.83984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.83984375" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="3.83984375" style="25" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="3.83984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="17.15625" style="25" customWidth="1"/>
+    <col min="21" max="21" width="13.83984375" style="54" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="17.15625" style="87" customWidth="1"/>
+    <col min="24" max="25" width="17.15625" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.41796875" style="25" customWidth="1"/>
     <col min="27" max="27" width="24" style="25" customWidth="1"/>
-    <col min="28" max="28" width="22.7109375" style="25" customWidth="1"/>
-    <col min="29" max="29" width="22.85546875" style="25" customWidth="1"/>
-    <col min="30" max="16384" width="11.42578125" style="25"/>
+    <col min="28" max="28" width="22.68359375" style="25" customWidth="1"/>
+    <col min="29" max="29" width="22.83984375" style="25" customWidth="1"/>
+    <col min="30" max="16384" width="11.41796875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -5870,7 +5870,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="30">
+    <row r="3" spans="1:29" ht="28.8">
       <c r="A3" s="55">
         <v>1</v>
       </c>
@@ -6155,7 +6155,7 @@
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
     </row>
-    <row r="8" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="8" spans="1:29" s="56" customFormat="1">
       <c r="A8" s="55" t="s">
         <v>0</v>
       </c>
@@ -6326,7 +6326,7 @@
       <c r="AB10" s="89"/>
       <c r="AC10" s="89"/>
     </row>
-    <row r="11" spans="1:29" s="56" customFormat="1" ht="26.25">
+    <row r="11" spans="1:29" s="56" customFormat="1" ht="25.5">
       <c r="A11" s="55" t="s">
         <v>0</v>
       </c>
@@ -6438,7 +6438,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="13" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -6554,7 +6554,7 @@
       <c r="AB14" s="89"/>
       <c r="AC14" s="89"/>
     </row>
-    <row r="15" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="15" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A15" s="55" t="s">
         <v>0</v>
       </c>
@@ -6888,7 +6888,7 @@
       <c r="AB20" s="89"/>
       <c r="AC20" s="89"/>
     </row>
-    <row r="21" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="21" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -7206,7 +7206,7 @@
       <c r="AB26" s="163"/>
       <c r="AC26" s="163"/>
     </row>
-    <row r="27" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="27" spans="1:29" s="56" customFormat="1">
       <c r="A27" s="55">
         <v>2</v>
       </c>
@@ -7485,7 +7485,7 @@
       <c r="AB31" s="89"/>
       <c r="AC31" s="89"/>
     </row>
-    <row r="32" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="32" spans="1:29" s="56" customFormat="1">
       <c r="A32" s="55" t="s">
         <v>0</v>
       </c>
@@ -7656,7 +7656,7 @@
       <c r="AB34" s="89"/>
       <c r="AC34" s="89"/>
     </row>
-    <row r="35" spans="1:29" s="56" customFormat="1" ht="26.25">
+    <row r="35" spans="1:29" s="56" customFormat="1" ht="25.5">
       <c r="A35" s="55" t="s">
         <v>0</v>
       </c>
@@ -7768,7 +7768,7 @@
       <c r="AB36" s="89"/>
       <c r="AC36" s="89"/>
     </row>
-    <row r="37" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="37" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A37" s="55" t="s">
         <v>0</v>
       </c>
@@ -7884,7 +7884,7 @@
       <c r="AB38" s="89"/>
       <c r="AC38" s="89"/>
     </row>
-    <row r="39" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="39" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A39" s="55" t="s">
         <v>0</v>
       </c>
@@ -8218,7 +8218,7 @@
       <c r="AB44" s="89"/>
       <c r="AC44" s="89"/>
     </row>
-    <row r="45" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="45" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A45" s="55" t="s">
         <v>0</v>
       </c>
@@ -8825,7 +8825,7 @@
       <c r="AB55" s="89"/>
       <c r="AC55" s="89"/>
     </row>
-    <row r="56" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="56" spans="1:29" s="56" customFormat="1">
       <c r="A56" s="55" t="s">
         <v>0</v>
       </c>
@@ -8996,7 +8996,7 @@
       <c r="AB58" s="89"/>
       <c r="AC58" s="89"/>
     </row>
-    <row r="59" spans="1:29" s="56" customFormat="1" ht="26.25">
+    <row r="59" spans="1:29" s="56" customFormat="1" ht="25.5">
       <c r="A59" s="55" t="s">
         <v>0</v>
       </c>
@@ -9108,7 +9108,7 @@
       <c r="AB60" s="89"/>
       <c r="AC60" s="89"/>
     </row>
-    <row r="61" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="61" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A61" s="55" t="s">
         <v>0</v>
       </c>
@@ -9224,7 +9224,7 @@
       <c r="AB62" s="89"/>
       <c r="AC62" s="89"/>
     </row>
-    <row r="63" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="63" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A63" s="55" t="s">
         <v>0</v>
       </c>
@@ -9558,7 +9558,7 @@
       <c r="AB68" s="89"/>
       <c r="AC68" s="89"/>
     </row>
-    <row r="69" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="69" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A69" s="55" t="s">
         <v>0</v>
       </c>
@@ -9876,7 +9876,7 @@
       <c r="AB74" s="163"/>
       <c r="AC74" s="163"/>
     </row>
-    <row r="75" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="75" spans="1:29" s="56" customFormat="1">
       <c r="A75" s="55">
         <v>4</v>
       </c>
@@ -10165,7 +10165,7 @@
       <c r="AB79" s="89"/>
       <c r="AC79" s="89"/>
     </row>
-    <row r="80" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="80" spans="1:29" s="56" customFormat="1">
       <c r="A80" s="55" t="s">
         <v>0</v>
       </c>
@@ -10336,7 +10336,7 @@
       <c r="AB82" s="89"/>
       <c r="AC82" s="89"/>
     </row>
-    <row r="83" spans="1:29" s="56" customFormat="1" ht="26.25">
+    <row r="83" spans="1:29" s="56" customFormat="1" ht="25.5">
       <c r="A83" s="55" t="s">
         <v>0</v>
       </c>
@@ -10448,7 +10448,7 @@
       <c r="AB84" s="89"/>
       <c r="AC84" s="89"/>
     </row>
-    <row r="85" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="85" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A85" s="55" t="s">
         <v>0</v>
       </c>
@@ -10564,7 +10564,7 @@
       <c r="AB86" s="89"/>
       <c r="AC86" s="89"/>
     </row>
-    <row r="87" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="87" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A87" s="55" t="s">
         <v>0</v>
       </c>
@@ -10898,7 +10898,7 @@
       <c r="AB92" s="89"/>
       <c r="AC92" s="89"/>
     </row>
-    <row r="93" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="93" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A93" s="55" t="s">
         <v>0</v>
       </c>
@@ -11216,7 +11216,7 @@
       <c r="AB98" s="163"/>
       <c r="AC98" s="163"/>
     </row>
-    <row r="99" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="99" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A99" s="55">
         <v>5</v>
       </c>
@@ -11505,7 +11505,7 @@
       <c r="AB103" s="89"/>
       <c r="AC103" s="89"/>
     </row>
-    <row r="104" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="104" spans="1:29" s="56" customFormat="1">
       <c r="A104" s="55" t="s">
         <v>0</v>
       </c>
@@ -11676,7 +11676,7 @@
       <c r="AB106" s="89"/>
       <c r="AC106" s="89"/>
     </row>
-    <row r="107" spans="1:29" s="56" customFormat="1" ht="26.25">
+    <row r="107" spans="1:29" s="56" customFormat="1" ht="25.5">
       <c r="A107" s="55" t="s">
         <v>0</v>
       </c>
@@ -11788,7 +11788,7 @@
       <c r="AB108" s="89"/>
       <c r="AC108" s="89"/>
     </row>
-    <row r="109" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="109" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A109" s="55" t="s">
         <v>0</v>
       </c>
@@ -11904,7 +11904,7 @@
       <c r="AB110" s="89"/>
       <c r="AC110" s="89"/>
     </row>
-    <row r="111" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="111" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A111" s="55" t="s">
         <v>0</v>
       </c>
@@ -12238,7 +12238,7 @@
       <c r="AB116" s="89"/>
       <c r="AC116" s="89"/>
     </row>
-    <row r="117" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="117" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A117" s="55" t="s">
         <v>0</v>
       </c>
@@ -12556,7 +12556,7 @@
       <c r="AB122" s="163"/>
       <c r="AC122" s="163"/>
     </row>
-    <row r="123" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="123" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A123" s="55">
         <v>6</v>
       </c>
@@ -12843,7 +12843,7 @@
       <c r="AB127" s="89"/>
       <c r="AC127" s="89"/>
     </row>
-    <row r="128" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="128" spans="1:29" s="56" customFormat="1">
       <c r="A128" s="55" t="s">
         <v>0</v>
       </c>
@@ -13014,7 +13014,7 @@
       <c r="AB130" s="89"/>
       <c r="AC130" s="89"/>
     </row>
-    <row r="131" spans="1:29" s="56" customFormat="1" ht="26.25">
+    <row r="131" spans="1:29" s="56" customFormat="1" ht="25.5">
       <c r="A131" s="55" t="s">
         <v>0</v>
       </c>
@@ -13126,7 +13126,7 @@
       <c r="AB132" s="89"/>
       <c r="AC132" s="89"/>
     </row>
-    <row r="133" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="133" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A133" s="55" t="s">
         <v>0</v>
       </c>
@@ -13242,7 +13242,7 @@
       <c r="AB134" s="89"/>
       <c r="AC134" s="89"/>
     </row>
-    <row r="135" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="135" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A135" s="55" t="s">
         <v>0</v>
       </c>
@@ -13576,7 +13576,7 @@
       <c r="AB140" s="89"/>
       <c r="AC140" s="89"/>
     </row>
-    <row r="141" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="141" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A141" s="55" t="s">
         <v>0</v>
       </c>
@@ -13917,24 +13917,24 @@
       <selection activeCell="AA15" sqref="AA15:AB15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="2" customWidth="1"/>
-    <col min="3" max="5" width="10.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.68359375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.68359375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="1.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="12.68359375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="11.41796875" style="2" customWidth="1"/>
     <col min="21" max="21" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="24" width="11.42578125" style="2"/>
-    <col min="25" max="25" width="11.42578125" style="113"/>
-    <col min="26" max="26" width="11.42578125" style="2"/>
-    <col min="27" max="29" width="23.140625" style="2" customWidth="1"/>
-    <col min="30" max="16384" width="11.42578125" style="2"/>
+    <col min="22" max="24" width="11.41796875" style="2"/>
+    <col min="25" max="25" width="11.41796875" style="113"/>
+    <col min="26" max="26" width="11.41796875" style="2"/>
+    <col min="27" max="29" width="23.15625" style="2" customWidth="1"/>
+    <col min="30" max="16384" width="11.41796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" s="142" customFormat="1">
@@ -14115,7 +14115,7 @@
       <c r="AV2" s="203"/>
       <c r="AW2" s="203"/>
     </row>
-    <row r="3" spans="1:55" customFormat="1" ht="60">
+    <row r="3" spans="1:55" customFormat="1" ht="43.2">
       <c r="A3" s="29">
         <v>25</v>
       </c>
@@ -14597,7 +14597,7 @@
       <c r="BB8" s="202"/>
       <c r="BC8" s="202"/>
     </row>
-    <row r="9" spans="1:55" s="56" customFormat="1" ht="30">
+    <row r="9" spans="1:55" s="56" customFormat="1" ht="28.8">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -15069,7 +15069,7 @@
       <c r="BB14" s="202"/>
       <c r="BC14" s="202"/>
     </row>
-    <row r="15" spans="1:55" customFormat="1" ht="45">
+    <row r="15" spans="1:55" customFormat="1" ht="43.2">
       <c r="A15" s="29">
         <v>26</v>
       </c>
@@ -15523,7 +15523,7 @@
       <c r="AV20" s="202"/>
       <c r="AW20" s="202"/>
     </row>
-    <row r="21" spans="1:49" s="56" customFormat="1" ht="30">
+    <row r="21" spans="1:49" s="56" customFormat="1" ht="28.8">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -16263,13 +16263,13 @@
       <selection activeCell="AB18" sqref="AA18:AB18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
     <col min="6" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" style="111"/>
-    <col min="27" max="29" width="23.5703125" customWidth="1"/>
+    <col min="25" max="25" width="11.578125" style="111"/>
+    <col min="27" max="29" width="23.578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -16430,7 +16430,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="45">
+    <row r="3" spans="1:50" ht="43.2">
       <c r="A3" s="29">
         <v>27</v>
       </c>
@@ -16722,7 +16722,7 @@
       <c r="AW7"/>
       <c r="AX7"/>
     </row>
-    <row r="8" spans="1:50" s="111" customFormat="1" ht="30">
+    <row r="8" spans="1:50" s="111" customFormat="1" ht="28.8">
       <c r="A8" s="29"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -16976,7 +16976,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="12" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -17294,7 +17294,7 @@
       <c r="AB17" s="163"/>
       <c r="AC17" s="163"/>
     </row>
-    <row r="18" spans="1:50" ht="45">
+    <row r="18" spans="1:50" ht="43.2">
       <c r="A18" s="29">
         <v>28</v>
       </c>
@@ -17647,7 +17647,7 @@
       <c r="AW22"/>
       <c r="AX22"/>
     </row>
-    <row r="23" spans="1:50" s="111" customFormat="1" ht="30">
+    <row r="23" spans="1:50" s="111" customFormat="1" ht="28.8">
       <c r="A23" s="29"/>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
@@ -17922,7 +17922,7 @@
       <c r="AB26" s="89"/>
       <c r="AC26" s="89"/>
     </row>
-    <row r="27" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="27" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A27" s="55" t="s">
         <v>0</v>
       </c>
@@ -18279,23 +18279,23 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="68" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="66" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="66" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="66" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" style="66" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.85546875" style="66" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="66" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="66" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="66" customWidth="1"/>
-    <col min="19" max="19" width="27.5703125" style="66" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="66" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="73" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="66" customWidth="1"/>
-    <col min="23" max="26" width="11.42578125" style="66"/>
-    <col min="27" max="29" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.15625" style="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.26171875" style="66" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.578125" style="66" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.83984375" style="66" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.83984375" style="66" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="66" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="66" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" style="66" customWidth="1"/>
+    <col min="19" max="19" width="27.578125" style="66" customWidth="1"/>
+    <col min="20" max="20" width="11.41796875" style="66" customWidth="1"/>
+    <col min="21" max="21" width="11.41796875" style="73" customWidth="1"/>
+    <col min="22" max="22" width="11.41796875" style="66" customWidth="1"/>
+    <col min="23" max="26" width="11.41796875" style="66"/>
+    <col min="27" max="29" width="23.41796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -18456,7 +18456,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="45">
+    <row r="3" spans="1:29" ht="43.2">
       <c r="A3" s="65">
         <v>29</v>
       </c>
@@ -18861,7 +18861,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="10" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -19187,18 +19187,18 @@
       <selection activeCell="AA6" sqref="AA6:AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" style="111"/>
-    <col min="27" max="29" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.83984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.68359375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.578125" style="111"/>
+    <col min="27" max="29" width="23.578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -19359,7 +19359,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="45">
+    <row r="3" spans="1:50" ht="43.2">
       <c r="A3" s="4">
         <v>30</v>
       </c>
@@ -19530,7 +19530,7 @@
       <c r="AB5" s="89"/>
       <c r="AC5" s="89"/>
     </row>
-    <row r="6" spans="1:50" ht="30">
+    <row r="6" spans="1:50">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -19591,7 +19591,7 @@
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
     </row>
-    <row r="7" spans="1:50" ht="30">
+    <row r="7" spans="1:50">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -19758,7 +19758,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="10" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -20110,25 +20110,25 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="7" customWidth="1"/>
-    <col min="3" max="5" width="10.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="7" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="7" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="7" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="7"/>
-    <col min="19" max="19" width="25.140625" style="7" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="7" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="69" customWidth="1"/>
-    <col min="22" max="22" width="18.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" style="7"/>
-    <col min="24" max="25" width="11.42578125" style="69"/>
-    <col min="26" max="26" width="11.42578125" style="7"/>
-    <col min="27" max="29" width="23.42578125" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="7"/>
+    <col min="2" max="2" width="7.41796875" style="7" customWidth="1"/>
+    <col min="3" max="5" width="10.68359375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="1.83984375" style="7" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="7" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" style="7"/>
+    <col min="19" max="19" width="25.15625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="11.41796875" style="7" customWidth="1"/>
+    <col min="21" max="21" width="11.41796875" style="69" customWidth="1"/>
+    <col min="22" max="22" width="18.578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.41796875" style="7"/>
+    <col min="24" max="25" width="11.41796875" style="69"/>
+    <col min="26" max="26" width="11.41796875" style="7"/>
+    <col min="27" max="29" width="23.41796875" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -20289,7 +20289,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="45">
+    <row r="3" spans="1:29" ht="43.2">
       <c r="A3" s="4">
         <v>31</v>
       </c>
@@ -20460,7 +20460,7 @@
       <c r="AB5" s="89"/>
       <c r="AC5" s="89"/>
     </row>
-    <row r="6" spans="1:29" ht="30">
+    <row r="6" spans="1:29">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -20521,7 +20521,7 @@
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
     </row>
-    <row r="7" spans="1:29" ht="30">
+    <row r="7" spans="1:29">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -20688,7 +20688,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="10" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -21019,17 +21019,17 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="1.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="1.41796875" bestFit="1" customWidth="1"/>
     <col min="8" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" style="111"/>
-    <col min="27" max="29" width="23.7109375" customWidth="1"/>
+    <col min="25" max="25" width="11.578125" style="111"/>
+    <col min="27" max="29" width="23.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -21190,7 +21190,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="15" customFormat="1" ht="45">
+    <row r="3" spans="1:29" s="15" customFormat="1" ht="43.2">
       <c r="A3" s="65">
         <v>32</v>
       </c>
@@ -21609,7 +21609,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="10" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -21945,21 +21945,21 @@
       <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="54" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.85546875" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.7109375" style="54" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.42578125" style="54"/>
-    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="54" customWidth="1"/>
-    <col min="22" max="26" width="11.42578125" style="54"/>
-    <col min="27" max="29" width="23.42578125" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="54"/>
+    <col min="2" max="2" width="11.15625" style="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.26171875" style="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.578125" style="54" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.83984375" style="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.83984375" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.68359375" style="54" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.41796875" style="54"/>
+    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.41796875" style="54" customWidth="1"/>
+    <col min="22" max="26" width="11.41796875" style="54"/>
+    <col min="27" max="29" width="23.41796875" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -22120,7 +22120,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="56" customFormat="1" ht="45">
+    <row r="3" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A3" s="55">
         <v>33</v>
       </c>
@@ -22575,7 +22575,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -22922,25 +22922,25 @@
       <selection activeCell="AA6" sqref="AA6:AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="80" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="15" customWidth="1"/>
-    <col min="3" max="5" width="10.7109375" style="15" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="15" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="15" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" style="15" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="73" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" style="15"/>
-    <col min="24" max="25" width="11.42578125" style="73"/>
-    <col min="26" max="26" width="11.42578125" style="15"/>
-    <col min="27" max="29" width="23.5703125" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="15"/>
+    <col min="1" max="1" width="3.41796875" style="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83984375" style="15" customWidth="1"/>
+    <col min="3" max="5" width="10.68359375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="1.83984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="15" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="15" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.41796875" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.68359375" style="15" customWidth="1"/>
+    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.41796875" style="73" customWidth="1"/>
+    <col min="22" max="22" width="17.15625" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.41796875" style="15"/>
+    <col min="24" max="25" width="11.41796875" style="73"/>
+    <col min="26" max="26" width="11.41796875" style="15"/>
+    <col min="27" max="29" width="23.578125" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -23101,7 +23101,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="45">
+    <row r="3" spans="1:50" ht="28.8">
       <c r="A3" s="55">
         <v>34</v>
       </c>
@@ -23546,7 +23546,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="10" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -23903,20 +23903,20 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="54" customWidth="1"/>
-    <col min="3" max="5" width="10.7109375" style="54" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="54" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.42578125" style="54"/>
-    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="11.42578125" style="54"/>
-    <col min="27" max="29" width="23.28515625" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="54"/>
+    <col min="1" max="1" width="3.15625" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.68359375" style="54" customWidth="1"/>
+    <col min="3" max="5" width="10.68359375" style="54" customWidth="1"/>
+    <col min="6" max="6" width="1.83984375" style="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="54" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="54" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.41796875" style="54"/>
+    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="11.41796875" style="54"/>
+    <col min="27" max="29" width="23.26171875" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -24077,7 +24077,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="56" customFormat="1" ht="45">
+    <row r="3" spans="1:50" s="56" customFormat="1" ht="43.2">
       <c r="A3" s="55">
         <v>35</v>
       </c>
@@ -24516,7 +24516,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -24873,22 +24873,22 @@
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.7109375" style="54" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.85546875" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="54" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="54"/>
-    <col min="19" max="19" width="41.42578125" style="54" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="54"/>
-    <col min="22" max="22" width="17.140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="11.42578125" style="54"/>
-    <col min="27" max="29" width="23.5703125" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="54"/>
+    <col min="1" max="1" width="3.83984375" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.68359375" style="54" customWidth="1"/>
+    <col min="5" max="5" width="1.83984375" style="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.83984375" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="54" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="54" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" style="54"/>
+    <col min="19" max="19" width="41.41796875" style="54" customWidth="1"/>
+    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.41796875" style="54"/>
+    <col min="22" max="22" width="17.15625" style="54" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="11.41796875" style="54"/>
+    <col min="27" max="29" width="23.578125" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -25049,7 +25049,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="56" customFormat="1" ht="45">
+    <row r="3" spans="1:50" s="56" customFormat="1" ht="43.2">
       <c r="A3" s="55">
         <v>36</v>
       </c>
@@ -25361,7 +25361,7 @@
       <c r="AW6"/>
       <c r="AX6"/>
     </row>
-    <row r="7" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="7" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A7" s="55" t="s">
         <v>0</v>
       </c>
@@ -25535,7 +25535,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="10" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -25834,26 +25834,26 @@
       <selection activeCell="AA15" sqref="AA15:AA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="10.7109375" style="15" customWidth="1"/>
-    <col min="9" max="9" width="2.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="16" width="3.7109375" style="15" customWidth="1"/>
-    <col min="17" max="17" width="3.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="15" customWidth="1"/>
+    <col min="1" max="1" width="2.68359375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="10.68359375" style="15" customWidth="1"/>
+    <col min="9" max="9" width="2.68359375" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="16" width="3.68359375" style="15" customWidth="1"/>
+    <col min="17" max="17" width="3.68359375" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" style="15" customWidth="1"/>
     <col min="19" max="19" width="23" style="15" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="15" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="73" customWidth="1"/>
-    <col min="22" max="22" width="24.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.28515625" style="15" customWidth="1"/>
+    <col min="20" max="20" width="11.41796875" style="15" customWidth="1"/>
+    <col min="21" max="21" width="11.41796875" style="73" customWidth="1"/>
+    <col min="22" max="22" width="24.15625" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.26171875" style="15" customWidth="1"/>
     <col min="24" max="24" width="17" style="15" customWidth="1"/>
     <col min="25" max="25" width="22" style="15" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="15"/>
+    <col min="26" max="26" width="11.41796875" style="15"/>
     <col min="27" max="27" width="23" style="15" customWidth="1"/>
-    <col min="28" max="28" width="22.5703125" style="15" customWidth="1"/>
+    <col min="28" max="28" width="22.578125" style="15" customWidth="1"/>
     <col min="29" max="29" width="23" style="15" customWidth="1"/>
-    <col min="30" max="16384" width="11.42578125" style="15"/>
+    <col min="30" max="16384" width="11.41796875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -26014,7 +26014,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="21" customFormat="1" ht="30">
+    <row r="3" spans="1:29" s="21" customFormat="1" ht="28.8">
       <c r="A3" s="58">
         <v>7</v>
       </c>
@@ -29668,23 +29668,23 @@
       <selection activeCell="AA36" sqref="AA36:AA39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.7109375" style="25" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="2.85546875" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="3.85546875" style="25" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" style="25" customWidth="1"/>
+    <col min="1" max="1" width="3.83984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.68359375" style="25" customWidth="1"/>
+    <col min="6" max="6" width="2.83984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="2.83984375" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="3.83984375" style="25" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9.68359375" style="25" customWidth="1"/>
     <col min="19" max="19" width="37" style="25" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" style="87" customWidth="1"/>
-    <col min="23" max="23" width="43.42578125" style="87" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="95.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.28515625" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="25"/>
-    <col min="27" max="29" width="23.85546875" customWidth="1"/>
+    <col min="20" max="20" width="8.26171875" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.83984375" style="54" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.41796875" style="87" customWidth="1"/>
+    <col min="23" max="23" width="43.41796875" style="87" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="95.578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.26171875" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.41796875" style="25"/>
+    <col min="27" max="29" width="23.83984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -29845,7 +29845,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="45">
+    <row r="3" spans="1:29" ht="43.2">
       <c r="A3" s="56">
         <v>37</v>
       </c>
@@ -30372,7 +30372,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="12" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -30664,7 +30664,7 @@
       <c r="AB17" s="163"/>
       <c r="AC17" s="163"/>
     </row>
-    <row r="18" spans="1:29" ht="60">
+    <row r="18" spans="1:29" ht="43.2">
       <c r="A18" s="56">
         <v>38</v>
       </c>
@@ -31189,7 +31189,7 @@
       <c r="AB26" s="89"/>
       <c r="AC26" s="89"/>
     </row>
-    <row r="27" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="27" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A27" s="55" t="s">
         <v>0</v>
       </c>
@@ -31481,7 +31481,7 @@
       <c r="AB32" s="163"/>
       <c r="AC32" s="163"/>
     </row>
-    <row r="33" spans="1:29" ht="60">
+    <row r="33" spans="1:29" ht="43.2">
       <c r="A33" s="83">
         <v>39</v>
       </c>
@@ -32008,7 +32008,7 @@
       <c r="AB41" s="89"/>
       <c r="AC41" s="89"/>
     </row>
-    <row r="42" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="42" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A42" s="55" t="s">
         <v>0</v>
       </c>
@@ -32323,18 +32323,18 @@
       <selection activeCell="AA87" sqref="AA87:AB87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.7109375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="10" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="11.42578125" style="10"/>
-    <col min="24" max="24" width="13.7109375" style="10" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="4.26171875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.68359375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="10" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="11.41796875" style="10"/>
+    <col min="24" max="24" width="13.68359375" style="10" customWidth="1"/>
+    <col min="25" max="25" width="11.83984375" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.41796875" style="10"/>
     <col min="27" max="29" width="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -32496,7 +32496,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="45">
+    <row r="3" spans="1:29" ht="43.2">
       <c r="A3" s="1">
         <v>40</v>
       </c>
@@ -32657,7 +32657,7 @@
       <c r="AB5" s="89"/>
       <c r="AC5" s="89"/>
     </row>
-    <row r="6" spans="1:29" ht="30">
+    <row r="6" spans="1:29" ht="28.8">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -32816,7 +32816,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="9" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -33126,7 +33126,7 @@
       <c r="AB14" s="163"/>
       <c r="AC14" s="163"/>
     </row>
-    <row r="15" spans="1:29" ht="45">
+    <row r="15" spans="1:29" ht="43.2">
       <c r="A15" s="1">
         <v>41</v>
       </c>
@@ -33289,7 +33289,7 @@
       <c r="AB17" s="89"/>
       <c r="AC17" s="89"/>
     </row>
-    <row r="18" spans="1:29" ht="30">
+    <row r="18" spans="1:29" ht="28.8">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -33448,7 +33448,7 @@
       <c r="AB20" s="89"/>
       <c r="AC20" s="89"/>
     </row>
-    <row r="21" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="21" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -33766,7 +33766,7 @@
       <c r="AB26" s="163"/>
       <c r="AC26" s="163"/>
     </row>
-    <row r="27" spans="1:29" ht="45">
+    <row r="27" spans="1:29" ht="43.2">
       <c r="A27" s="1">
         <v>42</v>
       </c>
@@ -33931,7 +33931,7 @@
       <c r="AB29" s="89"/>
       <c r="AC29" s="89"/>
     </row>
-    <row r="30" spans="1:29" ht="30">
+    <row r="30" spans="1:29" ht="28.8">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -34090,7 +34090,7 @@
       <c r="AB32" s="89"/>
       <c r="AC32" s="89"/>
     </row>
-    <row r="33" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="33" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A33" s="55" t="s">
         <v>0</v>
       </c>
@@ -34408,7 +34408,7 @@
       <c r="AB38" s="163"/>
       <c r="AC38" s="163"/>
     </row>
-    <row r="39" spans="1:29" ht="45">
+    <row r="39" spans="1:29" ht="43.2">
       <c r="A39" s="1">
         <v>43</v>
       </c>
@@ -34573,7 +34573,7 @@
       <c r="AB41" s="89"/>
       <c r="AC41" s="89"/>
     </row>
-    <row r="42" spans="1:29" ht="30">
+    <row r="42" spans="1:29" ht="28.8">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -34732,7 +34732,7 @@
       <c r="AB44" s="89"/>
       <c r="AC44" s="89"/>
     </row>
-    <row r="45" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="45" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A45" s="55" t="s">
         <v>0</v>
       </c>
@@ -35050,7 +35050,7 @@
       <c r="AB50" s="163"/>
       <c r="AC50" s="163"/>
     </row>
-    <row r="51" spans="1:29" ht="45">
+    <row r="51" spans="1:29" ht="43.2">
       <c r="A51" s="1">
         <v>44</v>
       </c>
@@ -35215,7 +35215,7 @@
       <c r="AB53" s="89"/>
       <c r="AC53" s="89"/>
     </row>
-    <row r="54" spans="1:29" ht="30">
+    <row r="54" spans="1:29" ht="28.8">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -35374,7 +35374,7 @@
       <c r="AB56" s="89"/>
       <c r="AC56" s="89"/>
     </row>
-    <row r="57" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="57" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A57" s="55" t="s">
         <v>0</v>
       </c>
@@ -35692,7 +35692,7 @@
       <c r="AB62" s="163"/>
       <c r="AC62" s="163"/>
     </row>
-    <row r="63" spans="1:29" ht="60">
+    <row r="63" spans="1:29" ht="43.2">
       <c r="A63" s="1">
         <v>45</v>
       </c>
@@ -35857,7 +35857,7 @@
       <c r="AB65" s="89"/>
       <c r="AC65" s="89"/>
     </row>
-    <row r="66" spans="1:29" ht="30">
+    <row r="66" spans="1:29" ht="28.8">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -36016,7 +36016,7 @@
       <c r="AB68" s="89"/>
       <c r="AC68" s="89"/>
     </row>
-    <row r="69" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="69" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A69" s="55" t="s">
         <v>0</v>
       </c>
@@ -36334,7 +36334,7 @@
       <c r="AB74" s="163"/>
       <c r="AC74" s="163"/>
     </row>
-    <row r="75" spans="1:29" ht="60">
+    <row r="75" spans="1:29" ht="43.2">
       <c r="A75" s="1">
         <v>46</v>
       </c>
@@ -36499,7 +36499,7 @@
       <c r="AB77" s="89"/>
       <c r="AC77" s="89"/>
     </row>
-    <row r="78" spans="1:29" ht="30">
+    <row r="78" spans="1:29" ht="28.8">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -36658,7 +36658,7 @@
       <c r="AB80" s="89"/>
       <c r="AC80" s="89"/>
     </row>
-    <row r="81" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="81" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A81" s="55" t="s">
         <v>0</v>
       </c>
@@ -36976,7 +36976,7 @@
       <c r="AB86" s="199"/>
       <c r="AC86" s="199"/>
     </row>
-    <row r="87" spans="1:29" ht="45">
+    <row r="87" spans="1:29" ht="28.8">
       <c r="A87" s="1">
         <v>47</v>
       </c>
@@ -37141,7 +37141,7 @@
       <c r="AB89" s="89"/>
       <c r="AC89" s="89"/>
     </row>
-    <row r="90" spans="1:29" ht="30">
+    <row r="90" spans="1:29" ht="28.8">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
@@ -37300,7 +37300,7 @@
       <c r="AB92" s="89"/>
       <c r="AC92" s="89"/>
     </row>
-    <row r="93" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="93" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A93" s="55" t="s">
         <v>0</v>
       </c>
@@ -37642,22 +37642,22 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="10" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.68359375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="10" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" style="10" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.42578125" style="10"/>
-    <col min="24" max="25" width="13.85546875" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="10"/>
+    <col min="19" max="19" width="16.83984375" style="10" customWidth="1"/>
+    <col min="20" max="20" width="6.15625" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11.41796875" style="10"/>
+    <col min="24" max="25" width="13.83984375" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.41796875" style="10"/>
     <col min="27" max="29" width="23" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="10"/>
+    <col min="51" max="16384" width="11.41796875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -37818,7 +37818,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" customFormat="1" ht="45">
+    <row r="3" spans="1:50" customFormat="1" ht="43.2">
       <c r="A3" s="1">
         <v>48</v>
       </c>
@@ -38504,23 +38504,23 @@
       <selection activeCell="AA43" sqref="AA43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="7.41796875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="10.26171875" style="10" customWidth="1"/>
     <col min="4" max="4" width="10" style="10" customWidth="1"/>
-    <col min="5" max="6" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.7109375" style="10" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.42578125" style="10"/>
-    <col min="20" max="20" width="9.140625" style="10" customWidth="1"/>
-    <col min="21" max="23" width="11.42578125" style="10"/>
-    <col min="24" max="24" width="17.5703125" style="10" customWidth="1"/>
+    <col min="5" max="6" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.68359375" style="10" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.41796875" style="10"/>
+    <col min="20" max="20" width="9.15625" style="10" customWidth="1"/>
+    <col min="21" max="23" width="11.41796875" style="10"/>
+    <col min="24" max="24" width="17.578125" style="10" customWidth="1"/>
     <col min="25" max="25" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="10"/>
-    <col min="27" max="29" width="24.7109375" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="10"/>
+    <col min="26" max="26" width="11.41796875" style="10"/>
+    <col min="27" max="29" width="24.68359375" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -38681,7 +38681,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" customFormat="1" ht="45">
+    <row r="3" spans="1:29" customFormat="1" ht="43.2">
       <c r="A3" s="1">
         <v>49</v>
       </c>
@@ -39462,7 +39462,7 @@
       <c r="AB17" s="89"/>
       <c r="AC17" s="89"/>
     </row>
-    <row r="18" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="18" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A18" s="55" t="s">
         <v>0</v>
       </c>
@@ -39791,7 +39791,7 @@
       <c r="AW23"/>
       <c r="AX23"/>
     </row>
-    <row r="24" spans="1:50" customFormat="1" ht="45">
+    <row r="24" spans="1:50" customFormat="1" ht="43.2">
       <c r="A24" s="1">
         <v>50</v>
       </c>
@@ -40572,7 +40572,7 @@
       <c r="AB38" s="89"/>
       <c r="AC38" s="89"/>
     </row>
-    <row r="39" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="39" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A39" s="55" t="s">
         <v>0</v>
       </c>
@@ -40920,19 +40920,19 @@
       <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.83984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.83984375" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.68359375" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="6.15625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14" customWidth="1"/>
     <col min="25" max="25" width="14" style="111" customWidth="1"/>
-    <col min="27" max="29" width="23.140625" customWidth="1"/>
+    <col min="27" max="29" width="23.15625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -41093,7 +41093,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="10" customFormat="1" ht="45">
+    <row r="3" spans="1:50" s="10" customFormat="1" ht="43.2">
       <c r="A3" s="1">
         <v>51</v>
       </c>
@@ -41531,7 +41531,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -41879,23 +41879,23 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.7109375" style="10" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.42578125" style="10"/>
-    <col min="20" max="20" width="6.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.42578125" style="10"/>
-    <col min="24" max="25" width="9.42578125" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="10"/>
-    <col min="27" max="29" width="23.7109375" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="3.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83984375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.15625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.83984375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.68359375" style="10" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.41796875" style="10"/>
+    <col min="20" max="20" width="6.15625" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11.41796875" style="10"/>
+    <col min="24" max="25" width="9.41796875" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.41796875" style="10"/>
+    <col min="27" max="29" width="23.68359375" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -42056,7 +42056,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" customFormat="1" ht="45">
+    <row r="3" spans="1:50" customFormat="1" ht="43.2">
       <c r="A3" s="1">
         <v>52</v>
       </c>
@@ -42388,7 +42388,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -42717,7 +42717,7 @@
       <c r="AW14"/>
       <c r="AX14"/>
     </row>
-    <row r="15" spans="1:50" customFormat="1" ht="45">
+    <row r="15" spans="1:50" customFormat="1" ht="43.2">
       <c r="A15" s="1">
         <v>53</v>
       </c>
@@ -43046,7 +43046,7 @@
       <c r="AB20" s="89"/>
       <c r="AC20" s="89"/>
     </row>
-    <row r="21" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="21" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -43390,22 +43390,22 @@
       <selection activeCell="AB26" sqref="AB26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.41796875" customWidth="1"/>
+    <col min="3" max="3" width="13.26171875" customWidth="1"/>
+    <col min="4" max="4" width="8.15625" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="1.85546875" customWidth="1"/>
-    <col min="9" max="9" width="1.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" customWidth="1"/>
-    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="10.140625" style="10" customWidth="1"/>
-    <col min="27" max="29" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="1.83984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="1.83984375" customWidth="1"/>
+    <col min="9" max="9" width="1.83984375" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" customWidth="1"/>
+    <col min="20" max="20" width="6.15625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.15625" style="10" customWidth="1"/>
+    <col min="27" max="29" width="23.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -43566,7 +43566,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="10" customFormat="1" ht="60">
+    <row r="3" spans="1:50" s="10" customFormat="1" ht="43.2">
       <c r="A3" s="1">
         <v>54</v>
       </c>
@@ -43888,7 +43888,7 @@
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
     </row>
-    <row r="8" spans="1:50" ht="45">
+    <row r="8" spans="1:50" ht="43.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -44096,7 +44096,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="12" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -44425,7 +44425,7 @@
       <c r="AW17"/>
       <c r="AX17"/>
     </row>
-    <row r="18" spans="1:50" s="10" customFormat="1" ht="60">
+    <row r="18" spans="1:50" s="10" customFormat="1" ht="43.2">
       <c r="A18" s="1">
         <v>55</v>
       </c>
@@ -44745,7 +44745,7 @@
       <c r="AB22" s="89"/>
       <c r="AC22" s="89"/>
     </row>
-    <row r="23" spans="1:50" ht="45">
+    <row r="23" spans="1:50" ht="43.2">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -44951,7 +44951,7 @@
       <c r="AB26" s="89"/>
       <c r="AC26" s="89"/>
     </row>
-    <row r="27" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="27" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A27" s="55" t="s">
         <v>0</v>
       </c>
@@ -45280,7 +45280,7 @@
       <c r="AW32"/>
       <c r="AX32"/>
     </row>
-    <row r="33" spans="1:50" s="10" customFormat="1" ht="60">
+    <row r="33" spans="1:50" s="10" customFormat="1" ht="43.2">
       <c r="A33" s="1">
         <v>56</v>
       </c>
@@ -45602,7 +45602,7 @@
       <c r="AB37" s="89"/>
       <c r="AC37" s="89"/>
     </row>
-    <row r="38" spans="1:50" ht="45">
+    <row r="38" spans="1:50" ht="43.2">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -45810,7 +45810,7 @@
       <c r="AB41" s="89"/>
       <c r="AC41" s="89"/>
     </row>
-    <row r="42" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="42" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A42" s="55" t="s">
         <v>0</v>
       </c>
@@ -46163,24 +46163,24 @@
       <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="39" customWidth="1"/>
+    <col min="1" max="1" width="3.83984375" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.41796875" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.26171875" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.15625" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
-    <col min="19" max="23" width="11.42578125" style="39"/>
-    <col min="24" max="24" width="46.28515625" style="97" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
+    <col min="19" max="23" width="11.41796875" style="39"/>
+    <col min="24" max="24" width="46.26171875" style="97" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="39"/>
-    <col min="27" max="29" width="24.42578125" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="39"/>
+    <col min="26" max="26" width="11.41796875" style="39"/>
+    <col min="27" max="29" width="24.41796875" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -46341,7 +46341,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="97" customFormat="1" ht="30">
+    <row r="3" spans="1:50" s="97" customFormat="1">
       <c r="A3" s="29">
         <v>57</v>
       </c>
@@ -46962,7 +46962,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="12" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -47806,27 +47806,27 @@
       <selection activeCell="AA21" sqref="AA21:AC21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="38" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="38" customWidth="1"/>
+    <col min="2" max="2" width="5.41796875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="13.26171875" style="38" customWidth="1"/>
+    <col min="4" max="4" width="8.15625" style="38" customWidth="1"/>
     <col min="5" max="5" width="10" style="38" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="38" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="38" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="38" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="38" customWidth="1"/>
-    <col min="19" max="19" width="49.5703125" style="38" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="38"/>
-    <col min="21" max="21" width="11.42578125" style="97"/>
-    <col min="22" max="22" width="11.42578125" style="38"/>
-    <col min="23" max="23" width="36.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="11.7109375" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="38"/>
-    <col min="27" max="29" width="23.140625" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="38"/>
+    <col min="6" max="6" width="1.83984375" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="38" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="38" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="38" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" style="38" customWidth="1"/>
+    <col min="19" max="19" width="49.578125" style="38" customWidth="1"/>
+    <col min="20" max="20" width="11.41796875" style="38"/>
+    <col min="21" max="21" width="11.41796875" style="97"/>
+    <col min="22" max="22" width="11.41796875" style="38"/>
+    <col min="23" max="23" width="36.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="11.68359375" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.41796875" style="38"/>
+    <col min="27" max="29" width="23.15625" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -49024,7 +49024,7 @@
       <c r="AB18" s="89"/>
       <c r="AC18" s="89"/>
     </row>
-    <row r="19" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="19" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A19" s="55" t="s">
         <v>0</v>
       </c>
@@ -49990,26 +49990,26 @@
       <selection activeCell="AA13" sqref="AA13:AC15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="39" customWidth="1"/>
+    <col min="2" max="2" width="5.41796875" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.26171875" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.15625" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.42578125" style="39"/>
-    <col min="21" max="21" width="11.42578125" style="97"/>
-    <col min="22" max="23" width="11.42578125" style="39"/>
+    <col min="6" max="6" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.41796875" style="39"/>
+    <col min="21" max="21" width="11.41796875" style="97"/>
+    <col min="22" max="23" width="11.41796875" style="39"/>
     <col min="24" max="24" width="23" style="97" customWidth="1"/>
-    <col min="25" max="25" width="13.42578125" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="39"/>
-    <col min="27" max="29" width="23.85546875" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="39"/>
+    <col min="25" max="25" width="13.41796875" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.41796875" style="39"/>
+    <col min="27" max="29" width="23.83984375" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -50170,7 +50170,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="97" customFormat="1" ht="30">
+    <row r="3" spans="1:50" s="97" customFormat="1" ht="28.8">
       <c r="A3" s="29">
         <v>59</v>
       </c>
@@ -50468,7 +50468,7 @@
       <c r="AW6"/>
       <c r="AX6"/>
     </row>
-    <row r="7" spans="1:50" s="97" customFormat="1" ht="30">
+    <row r="7" spans="1:50" s="97" customFormat="1">
       <c r="A7" s="29"/>
       <c r="B7" s="28"/>
       <c r="C7" s="34"/>
@@ -50536,7 +50536,7 @@
       <c r="AW7"/>
       <c r="AX7"/>
     </row>
-    <row r="8" spans="1:50" s="97" customFormat="1" ht="30">
+    <row r="8" spans="1:50" s="97" customFormat="1">
       <c r="A8" s="29" t="s">
         <v>0</v>
       </c>
@@ -50610,7 +50610,7 @@
       <c r="AW8"/>
       <c r="AX8"/>
     </row>
-    <row r="9" spans="1:50" s="97" customFormat="1" ht="30">
+    <row r="9" spans="1:50" s="97" customFormat="1" ht="28.8">
       <c r="A9" s="29"/>
       <c r="B9" s="28"/>
       <c r="C9" s="34"/>
@@ -50853,7 +50853,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="13" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -51817,29 +51817,29 @@
       <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="25" customWidth="1"/>
+    <col min="1" max="1" width="3.26171875" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.68359375" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.68359375" style="25" customWidth="1"/>
     <col min="4" max="4" width="6" style="25" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" style="25" customWidth="1"/>
-    <col min="6" max="7" width="8.7109375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="2.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.5703125" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="3.5703125" style="25" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="3.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.42578125" style="25"/>
-    <col min="20" max="20" width="11.42578125" style="25" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="54" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="25"/>
-    <col min="23" max="23" width="36.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="47.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.85546875" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="25"/>
-    <col min="27" max="27" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="5.83984375" style="25" customWidth="1"/>
+    <col min="6" max="7" width="8.68359375" style="25" customWidth="1"/>
+    <col min="8" max="8" width="2.578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.578125" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="3.578125" style="25" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="3.578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.41796875" style="25"/>
+    <col min="20" max="20" width="11.41796875" style="25" customWidth="1"/>
+    <col min="21" max="21" width="11.41796875" style="54" customWidth="1"/>
+    <col min="22" max="22" width="11.41796875" style="25"/>
+    <col min="23" max="23" width="36.26171875" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="47.68359375" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.83984375" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.41796875" style="25"/>
+    <col min="27" max="27" width="22.83984375" customWidth="1"/>
     <col min="28" max="29" width="23" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="25"/>
+    <col min="51" max="16384" width="11.41796875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="71" customFormat="1">
@@ -56715,20 +56715,20 @@
       <selection activeCell="AA7" sqref="AA7:AB9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.7109375" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" style="111" customWidth="1"/>
-    <col min="27" max="29" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.83984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.68359375" customWidth="1"/>
+    <col min="25" max="25" width="13.68359375" style="111" customWidth="1"/>
+    <col min="27" max="29" width="23.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -57349,7 +57349,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:29" s="56" customFormat="1" ht="30">
+    <row r="13" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -58090,25 +58090,25 @@
       <selection activeCell="AA7" sqref="AA7:AB9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="39" customWidth="1"/>
+    <col min="1" max="1" width="3.83984375" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.41796875" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.26171875" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.15625" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.42578125" style="39"/>
-    <col min="21" max="21" width="11.42578125" style="97"/>
-    <col min="22" max="23" width="11.42578125" style="39"/>
-    <col min="24" max="25" width="11.42578125" style="97"/>
-    <col min="26" max="26" width="11.42578125" style="39"/>
-    <col min="27" max="29" width="23.85546875" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="39"/>
+    <col min="6" max="6" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.41796875" style="39"/>
+    <col min="21" max="21" width="11.41796875" style="97"/>
+    <col min="22" max="23" width="11.41796875" style="39"/>
+    <col min="24" max="25" width="11.41796875" style="97"/>
+    <col min="26" max="26" width="11.41796875" style="39"/>
+    <col min="27" max="29" width="23.83984375" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -58918,7 +58918,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:50" s="56" customFormat="1" ht="30">
+    <row r="13" spans="1:50" s="56" customFormat="1" ht="28.8">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -59266,24 +59266,24 @@
       <selection activeCell="AA1" sqref="AA1:AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.7109375" style="39" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.42578125" style="39"/>
-    <col min="21" max="21" width="11.42578125" style="97"/>
-    <col min="22" max="22" width="12.85546875" style="39" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" style="39"/>
-    <col min="24" max="24" width="12.85546875" style="97" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="39"/>
-    <col min="27" max="29" width="23.5703125" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="39"/>
+    <col min="2" max="4" width="10.68359375" style="39" customWidth="1"/>
+    <col min="5" max="5" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.41796875" style="39"/>
+    <col min="21" max="21" width="11.41796875" style="97"/>
+    <col min="22" max="22" width="12.83984375" style="39" customWidth="1"/>
+    <col min="23" max="23" width="11.41796875" style="39"/>
+    <col min="24" max="24" width="12.83984375" style="97" customWidth="1"/>
+    <col min="25" max="25" width="12.15625" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.41796875" style="39"/>
+    <col min="27" max="29" width="23.578125" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -60364,17 +60364,17 @@
   <sheetPr codeName="Hoja34"/>
   <dimension ref="A1:AX17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.42578125" style="111"/>
-    <col min="26" max="26" width="11.28515625" customWidth="1"/>
-    <col min="27" max="29" width="22.5703125" customWidth="1"/>
+    <col min="25" max="25" width="11.41796875" style="111"/>
+    <col min="26" max="26" width="11.26171875" customWidth="1"/>
+    <col min="27" max="29" width="22.578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -61468,13 +61468,13 @@
       <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="15.85546875" customWidth="1"/>
-    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.42578125" style="111"/>
+    <col min="19" max="19" width="15.83984375" customWidth="1"/>
+    <col min="20" max="20" width="15.26171875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.41796875" style="111"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -61983,23 +61983,23 @@
       <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="7" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="7" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="11.42578125" style="7"/>
-    <col min="21" max="21" width="11.42578125" style="69"/>
-    <col min="22" max="22" width="11.42578125" style="7"/>
-    <col min="23" max="23" width="37.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="54.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" style="7" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="7"/>
-    <col min="27" max="29" width="22.85546875" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="7"/>
+    <col min="1" max="1" width="3.41796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.68359375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="1.83984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="7" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="11.41796875" style="7"/>
+    <col min="21" max="21" width="11.41796875" style="69"/>
+    <col min="22" max="22" width="11.41796875" style="7"/>
+    <col min="23" max="23" width="37.26171875" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="54.578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.41796875" style="7" customWidth="1"/>
+    <col min="26" max="26" width="11.41796875" style="7"/>
+    <col min="27" max="29" width="22.83984375" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -68004,19 +68004,19 @@
       <selection activeCell="AA24" sqref="AA24:AB24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="1.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="10" customWidth="1"/>
-    <col min="23" max="23" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.42578125" style="111"/>
-    <col min="27" max="29" width="22.85546875" customWidth="1"/>
+    <col min="2" max="6" width="10.68359375" customWidth="1"/>
+    <col min="7" max="7" width="1.83984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="1.83984375" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.41796875" customWidth="1"/>
+    <col min="21" max="21" width="11.41796875" style="10" customWidth="1"/>
+    <col min="23" max="23" width="35.83984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.41796875" style="111"/>
+    <col min="27" max="29" width="22.83984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -71101,22 +71101,22 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AA27" sqref="AA27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" customWidth="1"/>
-    <col min="24" max="24" width="8.140625" customWidth="1"/>
-    <col min="25" max="25" width="8.140625" style="111" customWidth="1"/>
-    <col min="27" max="29" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.26171875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.68359375" customWidth="1"/>
+    <col min="6" max="6" width="1.83984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.83984375" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.41796875" customWidth="1"/>
+    <col min="24" max="24" width="8.15625" customWidth="1"/>
+    <col min="25" max="25" width="8.15625" style="111" customWidth="1"/>
+    <col min="27" max="29" width="22.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -72910,7 +72910,7 @@
       <c r="Y27" s="22"/>
       <c r="Z27" s="22"/>
       <c r="AA27" s="89" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="AB27" s="89" t="s">
         <v>445</v>
@@ -72968,9 +72968,7 @@
       </c>
       <c r="Y28" s="22"/>
       <c r="Z28" s="133"/>
-      <c r="AA28" s="89" t="s">
-        <v>452</v>
-      </c>
+      <c r="AA28" s="89"/>
       <c r="AB28" s="89" t="s">
         <v>445</v>
       </c>
@@ -73026,13 +73024,13 @@
       <c r="Y29" s="24"/>
       <c r="Z29" s="24"/>
       <c r="AA29" s="89" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="AB29" s="89" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
       <c r="AC29" s="89" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
     </row>
     <row r="30" spans="1:50" s="56" customFormat="1">
@@ -73080,15 +73078,9 @@
       <c r="X30" s="22"/>
       <c r="Y30" s="22"/>
       <c r="Z30" s="22"/>
-      <c r="AA30" s="89" t="s">
-        <v>454</v>
-      </c>
-      <c r="AB30" s="89" t="s">
-        <v>455</v>
-      </c>
-      <c r="AC30" s="89" t="s">
-        <v>453</v>
-      </c>
+      <c r="AA30" s="89"/>
+      <c r="AB30" s="89"/>
+      <c r="AC30" s="89"/>
     </row>
     <row r="31" spans="1:50" s="56" customFormat="1">
       <c r="A31" s="55" t="s">
@@ -73354,21 +73346,21 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="1.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="11.42578125" style="2"/>
-    <col min="23" max="23" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.42578125" style="2" customWidth="1"/>
-    <col min="25" max="25" width="10.42578125" style="113" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="2"/>
-    <col min="27" max="29" width="22.85546875" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="4.26171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.68359375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="1.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.83984375" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="11.41796875" style="2"/>
+    <col min="23" max="23" width="35.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.41796875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="10.41796875" style="113" customWidth="1"/>
+    <col min="26" max="26" width="11.41796875" style="2"/>
+    <col min="27" max="29" width="22.83984375" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -74779,16 +74771,16 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.7109375" style="38" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.85546875" style="38" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="38" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="18" max="26" width="11.42578125" style="38"/>
-    <col min="27" max="29" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.83984375" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.68359375" style="38" customWidth="1"/>
+    <col min="5" max="5" width="1.83984375" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.83984375" style="38" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="38" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="38" bestFit="1" customWidth="1"/>
+    <col min="18" max="26" width="11.41796875" style="38"/>
+    <col min="27" max="29" width="22.83984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -75629,20 +75621,20 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.7109375" style="56" customWidth="1"/>
-    <col min="7" max="7" width="1.85546875" style="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="1.85546875" style="56" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.7109375" style="56" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="56" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="56"/>
-    <col min="19" max="19" width="30.28515625" style="56" customWidth="1"/>
-    <col min="20" max="21" width="11.42578125" style="56" customWidth="1"/>
-    <col min="22" max="26" width="11.42578125" style="56"/>
-    <col min="27" max="29" width="22.85546875" customWidth="1"/>
-    <col min="51" max="16384" width="11.42578125" style="56"/>
+    <col min="1" max="1" width="3.83984375" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.68359375" style="56" customWidth="1"/>
+    <col min="7" max="7" width="1.83984375" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="1.83984375" style="56" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.68359375" style="56" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.68359375" style="56" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.41796875" style="56"/>
+    <col min="19" max="19" width="30.26171875" style="56" customWidth="1"/>
+    <col min="20" max="21" width="11.41796875" style="56" customWidth="1"/>
+    <col min="22" max="26" width="11.41796875" style="56"/>
+    <col min="27" max="29" width="22.83984375" customWidth="1"/>
+    <col min="51" max="16384" width="11.41796875" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -76087,7 +76079,7 @@
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
     </row>
-    <row r="8" spans="1:50" ht="30">
+    <row r="8" spans="1:50" ht="28.8">
       <c r="B8" s="45" t="s">
         <v>0</v>
       </c>
@@ -76195,7 +76187,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="130" customFormat="1" ht="30">
+    <row r="10" spans="1:50" s="130" customFormat="1" ht="28.8">
       <c r="B10" s="45" t="s">
         <v>0</v>
       </c>
@@ -76310,7 +76302,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" ht="30">
+    <row r="12" spans="1:50" ht="28.8">
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
@@ -76600,7 +76592,7 @@
       <c r="AW17" s="56"/>
       <c r="AX17" s="56"/>
     </row>
-    <row r="18" spans="1:50" ht="30">
+    <row r="18" spans="1:50" ht="28.8">
       <c r="A18" s="55" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
-fixed an issue, where regulated taxonomy v2.1.0 had property keys missplaced for criterion #21. (REMASTERED) (GES-80 Jira issue)
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Documents\NetBeansProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DF1B9A-FB26-4FD3-B969-01380062C794}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30878EA-AF5B-4789-8FB5-F294636C71DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="588" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12443" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12442" uniqueCount="613">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -71102,7 +71102,7 @@
   <dimension ref="A1:AX34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AA27" sqref="AA27"/>
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
@@ -72526,7 +72526,9 @@
       <c r="Z21" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="AA21" s="89"/>
+      <c r="AA21" s="89" t="s">
+        <v>444</v>
+      </c>
       <c r="AB21" s="89"/>
       <c r="AC21" s="89"/>
       <c r="AD21"/>
@@ -72606,9 +72608,7 @@
       <c r="Z22" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="AA22" s="89" t="s">
-        <v>444</v>
-      </c>
+      <c r="AA22" s="89"/>
       <c r="AB22" s="89" t="s">
         <v>445</v>
       </c>
@@ -72670,7 +72670,7 @@
         <v>0</v>
       </c>
       <c r="AA23" s="89" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="AB23" s="89" t="s">
         <v>445</v>
@@ -72732,9 +72732,7 @@
       <c r="Z24" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="AA24" s="89" t="s">
-        <v>451</v>
-      </c>
+      <c r="AA24" s="89"/>
       <c r="AB24" s="89" t="s">
         <v>445</v>
       </c>

</xml_diff>

<commit_message>
-Created new espd.crit.please.give.more.details property key (GES-80 JIRA Issue) -Updated REGULAΤΕD 2.1.0 property taxonomy with the newly added property key (GES-81 JIRA Issue)
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Documents\NetBeansProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria\IdeaProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30878EA-AF5B-4789-8FB5-F294636C71DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD02F83-86BE-4ED4-AB41-773A66EEE84C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="588" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12442" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12442" uniqueCount="614">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1904,6 +1904,9 @@
   <si>
     <t>espd.part2.disworkers.details</t>
   </si>
+  <si>
+    <t>espd.crit.please.give.more.details</t>
+  </si>
 </sst>
 </file>
 
@@ -3194,36 +3197,42 @@
     <cellStyle name="20 % - Akzent4 2" xfId="57" xr:uid="{0CED6BA4-60EF-4640-ACAC-5491EFAA41B6}"/>
     <cellStyle name="20 % - Akzent5 2" xfId="58" xr:uid="{9711E678-D35B-4FDE-A1A2-62A8AD2BA356}"/>
     <cellStyle name="20 % - Akzent6 2" xfId="59" xr:uid="{7CA7835D-FCB7-402D-AC01-33C1572D9E8D}"/>
-    <cellStyle name="20% - Έμφαση1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Έμφαση2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Έμφαση3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Έμφαση4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Έμφαση5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Έμφαση6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent1 2" xfId="60" xr:uid="{F156E56A-1EB1-4208-BC29-CF6B998EA7A3}"/>
     <cellStyle name="40 % - Akzent2 2" xfId="61" xr:uid="{278057DE-C374-4BCB-BFCD-8FC15D932AF8}"/>
     <cellStyle name="40 % - Akzent3 2" xfId="62" xr:uid="{A54EAA7B-E320-4400-9E82-FA6F6AEFE3AC}"/>
     <cellStyle name="40 % - Akzent4 2" xfId="63" xr:uid="{CC5AD9F6-BA87-4F3F-A56B-CDCDACABDA15}"/>
     <cellStyle name="40 % - Akzent5 2" xfId="64" xr:uid="{207787DD-36B8-45D1-8027-AE3F706CF8B6}"/>
     <cellStyle name="40 % - Akzent6 2" xfId="65" xr:uid="{17547E8C-9F29-4A3C-9ED2-715309027EBC}"/>
-    <cellStyle name="40% - Έμφαση1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Έμφαση2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Έμφαση3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Έμφαση4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Έμφαση5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Έμφαση6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent1 2" xfId="66" xr:uid="{40B95E25-5021-4D50-BD78-EF739646E98A}"/>
     <cellStyle name="60 % - Akzent2 2" xfId="67" xr:uid="{6E273BEA-D51E-4B50-8CF4-C2833969CE90}"/>
     <cellStyle name="60 % - Akzent3 2" xfId="68" xr:uid="{D51BC707-3D8B-4DDD-AE79-8DC5AB0B42C5}"/>
     <cellStyle name="60 % - Akzent4 2" xfId="69" xr:uid="{4A56C24B-3685-4CD1-A574-E40817E12F78}"/>
     <cellStyle name="60 % - Akzent5 2" xfId="70" xr:uid="{CCE7CC06-0A99-4475-96EE-A84CB6F4A3A5}"/>
     <cellStyle name="60 % - Akzent6 2" xfId="71" xr:uid="{3289F5EB-86A3-4274-AFFF-FD4F68731930}"/>
-    <cellStyle name="60% - Έμφαση1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Έμφαση2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Έμφαση3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Έμφαση4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Έμφαση5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Έμφαση6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Akzent1 2" xfId="72" xr:uid="{5D4AEBF1-0A7C-4BFB-B180-EAF44EA9B0A0}"/>
     <cellStyle name="Akzent2 2" xfId="73" xr:uid="{85CC1BEF-51DC-4570-B4A5-B17C34C9B97A}"/>
     <cellStyle name="Akzent3 2" xfId="74" xr:uid="{B9E858DA-8B8C-4D0C-B338-C45F23F9086A}"/>
@@ -3231,20 +3240,35 @@
     <cellStyle name="Akzent5 2" xfId="76" xr:uid="{CF7F8E61-0EB1-4992-B9F6-7E1DE473F1D5}"/>
     <cellStyle name="Akzent6 2" xfId="77" xr:uid="{CF8B57BC-427C-49FA-B00F-9FDC4AE226A3}"/>
     <cellStyle name="Ausgabe 2" xfId="78" xr:uid="{A0801910-C56D-41DB-AA5B-D7B9CEA5154B}"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Berechnung 2" xfId="79" xr:uid="{41BDA43A-1ABB-4CE8-B9C1-27E91F26BF6C}"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Eingabe 2" xfId="80" xr:uid="{4E63FB11-C380-4C78-9E5D-ECEC7E1F665D}"/>
     <cellStyle name="Ergebnis 2" xfId="81" xr:uid="{DD805113-7B66-4F6A-AC81-26589BA0D384}"/>
     <cellStyle name="Erklärender Text 2" xfId="82" xr:uid="{A194B96E-6874-44FD-B943-01939BDA0BD2}"/>
     <cellStyle name="Erklärender Text 3" xfId="44" xr:uid="{3688BAA7-06B9-4333-8C0D-984DFDD1B2A1}"/>
     <cellStyle name="Excel Built-in Normal" xfId="50" xr:uid="{56DB3A1F-9D76-48AF-827F-04CDE3DA5590}"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Gut 2" xfId="83" xr:uid="{36A99347-B94D-4690-83AC-8C6CBD65002F}"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hipervínculo" xfId="42" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
     <cellStyle name="Hipervínculo visitado" xfId="103" xr:uid="{9051DEEC-FC84-4591-A8B5-638DE46C05EC}"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Link 2" xfId="46" xr:uid="{74412CD5-81A4-4040-B22F-ED1B046355CD}"/>
     <cellStyle name="Link 2 2" xfId="51" xr:uid="{D14BD33F-0DCB-4F85-85A5-9BB7DDF8AB8C}"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Neutral 2" xfId="84" xr:uid="{1AD55C52-8BBF-476B-B40D-9E1715BBCCDF}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="96" xr:uid="{A0210B32-A716-4DA1-8921-79BD6474A84A}"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Notiz 2" xfId="85" xr:uid="{96F7E845-1C7B-4930-A81D-0C72B5CBD2E5}"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Schlecht 2" xfId="86" xr:uid="{4CC925FC-A91B-432E-96A0-54E0F7C70564}"/>
     <cellStyle name="Standard 2" xfId="45" xr:uid="{4E059FDF-05CD-4388-BF86-76C2B6B0C261}"/>
     <cellStyle name="Standard 2 2" xfId="47" xr:uid="{E963BC3A-6088-4583-83FD-9423FD1ED1E0}"/>
@@ -3268,6 +3292,8 @@
     <cellStyle name="Standard 7" xfId="102" xr:uid="{744AB2FD-CA4D-461B-ABDD-66032D974148}"/>
     <cellStyle name="Standard 7 2" xfId="111" xr:uid="{E5E883CA-4D25-4EE5-AF23-D5DFF53989E9}"/>
     <cellStyle name="Style 1" xfId="52" xr:uid="{DF55E41B-F785-4866-85CE-BBB64E7F0959}"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Überschrift 1 2" xfId="87" xr:uid="{22C91833-F9B6-4CA7-8F5F-BC0057EEF790}"/>
     <cellStyle name="Überschrift 2 2" xfId="88" xr:uid="{CEF7EE81-7675-40F5-B163-07B4049BC735}"/>
     <cellStyle name="Überschrift 3 2" xfId="89" xr:uid="{31D47085-7A55-424D-9C36-8209503C4B54}"/>
@@ -3275,31 +3301,8 @@
     <cellStyle name="Überschrift 5" xfId="91" xr:uid="{77E8198C-A64B-454E-9437-C7F654B906EC}"/>
     <cellStyle name="Verknüpfte Zelle 2" xfId="92" xr:uid="{75D6E79A-C9C3-4688-BF38-48D65D7888B4}"/>
     <cellStyle name="Warnender Text 2" xfId="93" xr:uid="{B95B2F27-4BD2-47FB-BFB4-0373AACBC00D}"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen 2" xfId="94" xr:uid="{CC6AF966-5680-457A-B96D-078ED43C1691}"/>
-    <cellStyle name="Εισαγωγή" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Έλεγχος κελιού" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Έμφαση1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Έμφαση2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Έμφαση3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Έμφαση4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Έμφαση5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Έμφαση6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Έξοδος" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Επεξηγηματικό κείμενο" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Επικεφαλίδα 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Επικεφαλίδα 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Επικεφαλίδα 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Επικεφαλίδα 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Κακό" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Καλό" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Ουδέτερο" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Προειδοποιητικό κείμενο" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Σημείωση" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Συνδεδεμένο κελί" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Σύνολο" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Τίτλος" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Υπολογισμός" xfId="11" builtinId="22" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -5366,7 +5369,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5693,23 +5696,23 @@
       <selection activeCell="AA123" sqref="AA123:AB123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.83984375" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.68359375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="2.83984375" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.83984375" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="3.83984375" style="25" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="3.83984375" style="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="17.15625" style="25" customWidth="1"/>
-    <col min="21" max="21" width="13.83984375" style="54" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="17.15625" style="87" customWidth="1"/>
-    <col min="24" max="25" width="17.15625" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="25" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.6640625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="2.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.88671875" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="3.88671875" style="25" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="3.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="17.109375" style="25" customWidth="1"/>
+    <col min="21" max="21" width="13.88671875" style="54" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="17.109375" style="87" customWidth="1"/>
+    <col min="24" max="25" width="17.109375" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="25" customWidth="1"/>
     <col min="27" max="27" width="24" style="25" customWidth="1"/>
-    <col min="28" max="28" width="22.68359375" style="25" customWidth="1"/>
-    <col min="29" max="29" width="22.83984375" style="25" customWidth="1"/>
-    <col min="30" max="16384" width="11.41796875" style="25"/>
+    <col min="28" max="28" width="22.6640625" style="25" customWidth="1"/>
+    <col min="29" max="29" width="22.88671875" style="25" customWidth="1"/>
+    <col min="30" max="16384" width="11.44140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -6326,7 +6329,7 @@
       <c r="AB10" s="89"/>
       <c r="AC10" s="89"/>
     </row>
-    <row r="11" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="11" spans="1:29" s="56" customFormat="1" ht="27">
       <c r="A11" s="55" t="s">
         <v>0</v>
       </c>
@@ -7206,7 +7209,7 @@
       <c r="AB26" s="163"/>
       <c r="AC26" s="163"/>
     </row>
-    <row r="27" spans="1:29" s="56" customFormat="1">
+    <row r="27" spans="1:29" s="56" customFormat="1" ht="28.8">
       <c r="A27" s="55">
         <v>2</v>
       </c>
@@ -7656,7 +7659,7 @@
       <c r="AB34" s="89"/>
       <c r="AC34" s="89"/>
     </row>
-    <row r="35" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="35" spans="1:29" s="56" customFormat="1" ht="27">
       <c r="A35" s="55" t="s">
         <v>0</v>
       </c>
@@ -8996,7 +8999,7 @@
       <c r="AB58" s="89"/>
       <c r="AC58" s="89"/>
     </row>
-    <row r="59" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="59" spans="1:29" s="56" customFormat="1" ht="27">
       <c r="A59" s="55" t="s">
         <v>0</v>
       </c>
@@ -10336,7 +10339,7 @@
       <c r="AB82" s="89"/>
       <c r="AC82" s="89"/>
     </row>
-    <row r="83" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="83" spans="1:29" s="56" customFormat="1" ht="27">
       <c r="A83" s="55" t="s">
         <v>0</v>
       </c>
@@ -11676,7 +11679,7 @@
       <c r="AB106" s="89"/>
       <c r="AC106" s="89"/>
     </row>
-    <row r="107" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="107" spans="1:29" s="56" customFormat="1" ht="27">
       <c r="A107" s="55" t="s">
         <v>0</v>
       </c>
@@ -13014,7 +13017,7 @@
       <c r="AB130" s="89"/>
       <c r="AC130" s="89"/>
     </row>
-    <row r="131" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="131" spans="1:29" s="56" customFormat="1" ht="27">
       <c r="A131" s="55" t="s">
         <v>0</v>
       </c>
@@ -13917,24 +13920,24 @@
       <selection activeCell="AA15" sqref="AA15:AB15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.68359375" style="2" customWidth="1"/>
-    <col min="3" max="5" width="10.68359375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="12.68359375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" style="2" customWidth="1"/>
     <col min="21" max="21" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="24" width="11.41796875" style="2"/>
-    <col min="25" max="25" width="11.41796875" style="113"/>
-    <col min="26" max="26" width="11.41796875" style="2"/>
-    <col min="27" max="29" width="23.15625" style="2" customWidth="1"/>
-    <col min="30" max="16384" width="11.41796875" style="2"/>
+    <col min="22" max="24" width="11.44140625" style="2"/>
+    <col min="25" max="25" width="11.44140625" style="113"/>
+    <col min="26" max="26" width="11.44140625" style="2"/>
+    <col min="27" max="29" width="23.109375" style="2" customWidth="1"/>
+    <col min="30" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" s="142" customFormat="1">
@@ -16263,13 +16266,13 @@
       <selection activeCell="AB18" sqref="AA18:AB18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.578125" style="111"/>
-    <col min="27" max="29" width="23.578125" customWidth="1"/>
+    <col min="25" max="25" width="11.5546875" style="111"/>
+    <col min="27" max="29" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -18279,23 +18282,23 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="68" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" style="66" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" style="66" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.578125" style="66" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="66" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="66" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="66" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="66" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="66" customWidth="1"/>
-    <col min="19" max="19" width="27.578125" style="66" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" style="66" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="73" customWidth="1"/>
-    <col min="22" max="22" width="11.41796875" style="66" customWidth="1"/>
-    <col min="23" max="26" width="11.41796875" style="66"/>
-    <col min="27" max="29" width="23.41796875" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" style="66" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="66" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.88671875" style="66" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.88671875" style="66" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="66" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="66" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" style="66" customWidth="1"/>
+    <col min="19" max="19" width="27.5546875" style="66" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" style="66" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" style="73" customWidth="1"/>
+    <col min="22" max="22" width="11.44140625" style="66" customWidth="1"/>
+    <col min="23" max="26" width="11.44140625" style="66"/>
+    <col min="27" max="29" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -19187,18 +19190,18 @@
       <selection activeCell="AA6" sqref="AA6:AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.68359375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.578125" style="111"/>
-    <col min="27" max="29" width="23.578125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5546875" style="111"/>
+    <col min="27" max="29" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -20110,25 +20113,25 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" style="7" customWidth="1"/>
-    <col min="3" max="5" width="10.68359375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="7" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="7" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="7" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="7"/>
-    <col min="19" max="19" width="25.15625" style="7" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" style="7" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="69" customWidth="1"/>
-    <col min="22" max="22" width="18.578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.41796875" style="7"/>
-    <col min="24" max="25" width="11.41796875" style="69"/>
-    <col min="26" max="26" width="11.41796875" style="7"/>
-    <col min="27" max="29" width="23.41796875" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="7"/>
+    <col min="2" max="2" width="7.44140625" style="7" customWidth="1"/>
+    <col min="3" max="5" width="10.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" style="7" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="7" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" style="7"/>
+    <col min="19" max="19" width="25.109375" style="7" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" style="7" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" style="69" customWidth="1"/>
+    <col min="22" max="22" width="18.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.44140625" style="7"/>
+    <col min="24" max="25" width="11.44140625" style="69"/>
+    <col min="26" max="26" width="11.44140625" style="7"/>
+    <col min="27" max="29" width="23.44140625" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -21019,17 +21022,17 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="1.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="1.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.578125" style="111"/>
-    <col min="27" max="29" width="23.68359375" customWidth="1"/>
+    <col min="25" max="25" width="11.5546875" style="111"/>
+    <col min="27" max="29" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -21945,21 +21948,21 @@
       <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" style="54" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.578125" style="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.68359375" style="54" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.41796875" style="54"/>
-    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="54" customWidth="1"/>
-    <col min="22" max="26" width="11.41796875" style="54"/>
-    <col min="27" max="29" width="23.41796875" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="54"/>
+    <col min="2" max="2" width="11.109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" style="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.88671875" style="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.88671875" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.6640625" style="54" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.44140625" style="54"/>
+    <col min="20" max="20" width="6.109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" style="54" customWidth="1"/>
+    <col min="22" max="26" width="11.44140625" style="54"/>
+    <col min="27" max="29" width="23.44140625" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -22922,25 +22925,25 @@
       <selection activeCell="AA6" sqref="AA6:AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.41796875" style="80" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83984375" style="15" customWidth="1"/>
-    <col min="3" max="5" width="10.68359375" style="15" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="15" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="15" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.41796875" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.68359375" style="15" customWidth="1"/>
-    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="73" customWidth="1"/>
-    <col min="22" max="22" width="17.15625" style="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.41796875" style="15"/>
-    <col min="24" max="25" width="11.41796875" style="73"/>
-    <col min="26" max="26" width="11.41796875" style="15"/>
-    <col min="27" max="29" width="23.578125" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="15"/>
+    <col min="1" max="1" width="3.44140625" style="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="15" customWidth="1"/>
+    <col min="3" max="5" width="10.6640625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="15" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="15" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" style="15" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" style="73" customWidth="1"/>
+    <col min="22" max="22" width="17.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.44140625" style="15"/>
+    <col min="24" max="25" width="11.44140625" style="73"/>
+    <col min="26" max="26" width="11.44140625" style="15"/>
+    <col min="27" max="29" width="23.5546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -23101,7 +23104,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="28.8">
+    <row r="3" spans="1:50" ht="43.2">
       <c r="A3" s="55">
         <v>34</v>
       </c>
@@ -23903,20 +23906,20 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.15625" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.68359375" style="54" customWidth="1"/>
-    <col min="3" max="5" width="10.68359375" style="54" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="54" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="54" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.41796875" style="54"/>
-    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="11.41796875" style="54"/>
-    <col min="27" max="29" width="23.26171875" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="54"/>
+    <col min="1" max="1" width="3.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="54" customWidth="1"/>
+    <col min="3" max="5" width="10.6640625" style="54" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" style="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="54" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="54" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.44140625" style="54"/>
+    <col min="20" max="20" width="6.109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="11.44140625" style="54"/>
+    <col min="27" max="29" width="23.21875" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -24873,22 +24876,22 @@
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.68359375" style="54" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="54" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="54" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="54"/>
-    <col min="19" max="19" width="41.41796875" style="54" customWidth="1"/>
-    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="54"/>
-    <col min="22" max="22" width="17.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="11.41796875" style="54"/>
-    <col min="27" max="29" width="23.578125" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="54"/>
+    <col min="1" max="1" width="3.88671875" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.6640625" style="54" customWidth="1"/>
+    <col min="5" max="5" width="1.88671875" style="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.88671875" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="54" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="54" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" style="54"/>
+    <col min="19" max="19" width="41.44140625" style="54" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" style="54"/>
+    <col min="22" max="22" width="17.109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="11.44140625" style="54"/>
+    <col min="27" max="29" width="23.5546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -25834,26 +25837,26 @@
       <selection activeCell="AA15" sqref="AA15:AA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.68359375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="10.68359375" style="15" customWidth="1"/>
-    <col min="9" max="9" width="2.68359375" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="16" width="3.68359375" style="15" customWidth="1"/>
-    <col min="17" max="17" width="3.68359375" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="10.6640625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="2.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="16" width="3.6640625" style="15" customWidth="1"/>
+    <col min="17" max="17" width="3.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" style="15" customWidth="1"/>
     <col min="19" max="19" width="23" style="15" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" style="15" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="73" customWidth="1"/>
-    <col min="22" max="22" width="24.15625" style="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.26171875" style="15" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" style="15" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" style="73" customWidth="1"/>
+    <col min="22" max="22" width="24.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.21875" style="15" customWidth="1"/>
     <col min="24" max="24" width="17" style="15" customWidth="1"/>
     <col min="25" max="25" width="22" style="15" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="15"/>
+    <col min="26" max="26" width="11.44140625" style="15"/>
     <col min="27" max="27" width="23" style="15" customWidth="1"/>
-    <col min="28" max="28" width="22.578125" style="15" customWidth="1"/>
+    <col min="28" max="28" width="22.5546875" style="15" customWidth="1"/>
     <col min="29" max="29" width="23" style="15" customWidth="1"/>
-    <col min="30" max="16384" width="11.41796875" style="15"/>
+    <col min="30" max="16384" width="11.44140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -29668,23 +29671,23 @@
       <selection activeCell="AA36" sqref="AA36:AA39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.68359375" style="25" customWidth="1"/>
-    <col min="6" max="6" width="2.83984375" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="2.83984375" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="3.83984375" style="25" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9.68359375" style="25" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.6640625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="2.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="2.88671875" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="3.88671875" style="25" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" style="25" customWidth="1"/>
     <col min="19" max="19" width="37" style="25" customWidth="1"/>
-    <col min="20" max="20" width="8.26171875" style="25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.83984375" style="54" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.41796875" style="87" customWidth="1"/>
-    <col min="23" max="23" width="43.41796875" style="87" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="95.578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.26171875" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="25"/>
-    <col min="27" max="29" width="23.83984375" customWidth="1"/>
+    <col min="20" max="20" width="8.21875" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.88671875" style="54" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.44140625" style="87" customWidth="1"/>
+    <col min="23" max="23" width="43.44140625" style="87" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="95.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.21875" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="25"/>
+    <col min="27" max="29" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -32323,18 +32326,18 @@
       <selection activeCell="AA87" sqref="AA87:AB87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.26171875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.68359375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="10" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="11.41796875" style="10"/>
-    <col min="24" max="24" width="13.68359375" style="10" customWidth="1"/>
-    <col min="25" max="25" width="11.83984375" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="10"/>
+    <col min="1" max="1" width="4.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.6640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="10" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="11.44140625" style="10"/>
+    <col min="24" max="24" width="13.6640625" style="10" customWidth="1"/>
+    <col min="25" max="25" width="11.88671875" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="10"/>
     <col min="27" max="29" width="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -37642,22 +37645,22 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.68359375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="10" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="1.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.88671875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="10" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.83984375" style="10" customWidth="1"/>
-    <col min="20" max="20" width="6.15625" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.41796875" style="10"/>
-    <col min="24" max="25" width="13.83984375" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="10"/>
+    <col min="19" max="19" width="16.88671875" style="10" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11.44140625" style="10"/>
+    <col min="24" max="25" width="13.88671875" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="10"/>
     <col min="27" max="29" width="23" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="10"/>
+    <col min="51" max="16384" width="11.44140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -38504,23 +38507,23 @@
       <selection activeCell="AA43" sqref="AA43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="10.26171875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="10" customWidth="1"/>
     <col min="4" max="4" width="10" style="10" customWidth="1"/>
-    <col min="5" max="6" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.68359375" style="10" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.41796875" style="10"/>
-    <col min="20" max="20" width="9.15625" style="10" customWidth="1"/>
-    <col min="21" max="23" width="11.41796875" style="10"/>
-    <col min="24" max="24" width="17.578125" style="10" customWidth="1"/>
+    <col min="5" max="6" width="1.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.6640625" style="10" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.44140625" style="10"/>
+    <col min="20" max="20" width="9.109375" style="10" customWidth="1"/>
+    <col min="21" max="23" width="11.44140625" style="10"/>
+    <col min="24" max="24" width="17.5546875" style="10" customWidth="1"/>
     <col min="25" max="25" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="10"/>
-    <col min="27" max="29" width="24.68359375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="10"/>
+    <col min="26" max="26" width="11.44140625" style="10"/>
+    <col min="27" max="29" width="24.6640625" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -40920,19 +40923,19 @@
       <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.68359375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="6.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.6640625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14" customWidth="1"/>
     <col min="25" max="25" width="14" style="111" customWidth="1"/>
-    <col min="27" max="29" width="23.15625" customWidth="1"/>
+    <col min="27" max="29" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -41879,23 +41882,23 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.41796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.83984375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11.15625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="11.83984375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.68359375" style="10" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.41796875" style="10"/>
-    <col min="20" max="20" width="6.15625" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.41796875" style="10"/>
-    <col min="24" max="25" width="9.41796875" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="10"/>
-    <col min="27" max="29" width="23.68359375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="10"/>
+    <col min="1" max="1" width="3.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.6640625" style="10" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.44140625" style="10"/>
+    <col min="20" max="20" width="6.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11.44140625" style="10"/>
+    <col min="24" max="25" width="9.44140625" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="10"/>
+    <col min="27" max="29" width="23.6640625" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -43390,22 +43393,22 @@
       <selection activeCell="AB26" sqref="AB26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.41796875" customWidth="1"/>
-    <col min="3" max="3" width="13.26171875" customWidth="1"/>
-    <col min="4" max="4" width="8.15625" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="1.83984375" customWidth="1"/>
-    <col min="9" max="9" width="1.83984375" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" customWidth="1"/>
-    <col min="20" max="20" width="6.15625" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="10.15625" style="10" customWidth="1"/>
-    <col min="27" max="29" width="23.68359375" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="1.88671875" customWidth="1"/>
+    <col min="9" max="9" width="1.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.109375" style="10" customWidth="1"/>
+    <col min="27" max="29" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -45280,7 +45283,7 @@
       <c r="AW32"/>
       <c r="AX32"/>
     </row>
-    <row r="33" spans="1:50" s="10" customFormat="1" ht="43.2">
+    <row r="33" spans="1:50" s="10" customFormat="1" ht="57.6">
       <c r="A33" s="1">
         <v>56</v>
       </c>
@@ -46163,24 +46166,24 @@
       <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.41796875" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.26171875" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.15625" style="39" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
-    <col min="19" max="23" width="11.41796875" style="39"/>
-    <col min="24" max="24" width="46.26171875" style="97" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" style="39" customWidth="1"/>
+    <col min="19" max="23" width="11.44140625" style="39"/>
+    <col min="24" max="24" width="46.21875" style="97" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="39"/>
-    <col min="27" max="29" width="24.41796875" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="39"/>
+    <col min="26" max="26" width="11.44140625" style="39"/>
+    <col min="27" max="29" width="24.44140625" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -47806,27 +47809,27 @@
       <selection activeCell="AA21" sqref="AA21:AC21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.41796875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="13.26171875" style="38" customWidth="1"/>
-    <col min="4" max="4" width="8.15625" style="38" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="38" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" style="38" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="38" customWidth="1"/>
     <col min="5" max="5" width="10" style="38" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="38" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="38" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="38" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="38" customWidth="1"/>
-    <col min="19" max="19" width="49.578125" style="38" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" style="38"/>
-    <col min="21" max="21" width="11.41796875" style="97"/>
-    <col min="22" max="22" width="11.41796875" style="38"/>
-    <col min="23" max="23" width="36.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="11.68359375" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="38"/>
-    <col min="27" max="29" width="23.15625" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="38"/>
+    <col min="6" max="6" width="1.88671875" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="38" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="38" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="38" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" style="38" customWidth="1"/>
+    <col min="19" max="19" width="49.5546875" style="38" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" style="38"/>
+    <col min="21" max="21" width="11.44140625" style="97"/>
+    <col min="22" max="22" width="11.44140625" style="38"/>
+    <col min="23" max="23" width="36.21875" style="38" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="11.6640625" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="38"/>
+    <col min="27" max="29" width="23.109375" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -49990,26 +49993,26 @@
       <selection activeCell="AA13" sqref="AA13:AC15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.41796875" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.26171875" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.15625" style="39" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.41796875" style="39"/>
-    <col min="21" max="21" width="11.41796875" style="97"/>
-    <col min="22" max="23" width="11.41796875" style="39"/>
+    <col min="6" max="6" width="1.88671875" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.44140625" style="39"/>
+    <col min="21" max="21" width="11.44140625" style="97"/>
+    <col min="22" max="23" width="11.44140625" style="39"/>
     <col min="24" max="24" width="23" style="97" customWidth="1"/>
-    <col min="25" max="25" width="13.41796875" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="39"/>
-    <col min="27" max="29" width="23.83984375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="39"/>
+    <col min="25" max="25" width="13.44140625" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="39"/>
+    <col min="27" max="29" width="23.88671875" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -50468,7 +50471,7 @@
       <c r="AW6"/>
       <c r="AX6"/>
     </row>
-    <row r="7" spans="1:50" s="97" customFormat="1">
+    <row r="7" spans="1:50" s="97" customFormat="1" ht="28.8">
       <c r="A7" s="29"/>
       <c r="B7" s="28"/>
       <c r="C7" s="34"/>
@@ -50536,7 +50539,7 @@
       <c r="AW7"/>
       <c r="AX7"/>
     </row>
-    <row r="8" spans="1:50" s="97" customFormat="1">
+    <row r="8" spans="1:50" s="97" customFormat="1" ht="28.8">
       <c r="A8" s="29" t="s">
         <v>0</v>
       </c>
@@ -51817,29 +51820,29 @@
       <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.26171875" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.68359375" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.68359375" style="25" customWidth="1"/>
+    <col min="1" max="1" width="3.21875" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="25" customWidth="1"/>
     <col min="4" max="4" width="6" style="25" customWidth="1"/>
-    <col min="5" max="5" width="5.83984375" style="25" customWidth="1"/>
-    <col min="6" max="7" width="8.68359375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="2.578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.578125" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="3.578125" style="25" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="3.578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.41796875" style="25"/>
-    <col min="20" max="20" width="11.41796875" style="25" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="54" customWidth="1"/>
-    <col min="22" max="22" width="11.41796875" style="25"/>
-    <col min="23" max="23" width="36.26171875" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="47.68359375" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.83984375" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="25"/>
-    <col min="27" max="27" width="22.83984375" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" style="25" customWidth="1"/>
+    <col min="6" max="7" width="8.6640625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="2.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5546875" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="3.5546875" style="25" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="3.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.44140625" style="25"/>
+    <col min="20" max="20" width="11.44140625" style="25" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" style="54" customWidth="1"/>
+    <col min="22" max="22" width="11.44140625" style="25"/>
+    <col min="23" max="23" width="36.21875" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="47.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.88671875" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="25"/>
+    <col min="27" max="27" width="22.88671875" customWidth="1"/>
     <col min="28" max="29" width="23" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="25"/>
+    <col min="51" max="16384" width="11.44140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="71" customFormat="1">
@@ -56715,20 +56718,20 @@
       <selection activeCell="AA7" sqref="AA7:AB9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.68359375" customWidth="1"/>
-    <col min="25" max="25" width="13.68359375" style="111" customWidth="1"/>
-    <col min="27" max="29" width="23.68359375" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" style="111" customWidth="1"/>
+    <col min="27" max="29" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -58090,25 +58093,25 @@
       <selection activeCell="AA7" sqref="AA7:AB9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.41796875" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.26171875" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.15625" style="39" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.41796875" style="39"/>
-    <col min="21" max="21" width="11.41796875" style="97"/>
-    <col min="22" max="23" width="11.41796875" style="39"/>
-    <col min="24" max="25" width="11.41796875" style="97"/>
-    <col min="26" max="26" width="11.41796875" style="39"/>
-    <col min="27" max="29" width="23.83984375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="39"/>
+    <col min="6" max="6" width="1.88671875" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.44140625" style="39"/>
+    <col min="21" max="21" width="11.44140625" style="97"/>
+    <col min="22" max="23" width="11.44140625" style="39"/>
+    <col min="24" max="25" width="11.44140625" style="97"/>
+    <col min="26" max="26" width="11.44140625" style="39"/>
+    <col min="27" max="29" width="23.88671875" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -59266,24 +59269,24 @@
       <selection activeCell="AA1" sqref="AA1:AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.68359375" style="39" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.41796875" style="39"/>
-    <col min="21" max="21" width="11.41796875" style="97"/>
-    <col min="22" max="22" width="12.83984375" style="39" customWidth="1"/>
-    <col min="23" max="23" width="11.41796875" style="39"/>
-    <col min="24" max="24" width="12.83984375" style="97" customWidth="1"/>
-    <col min="25" max="25" width="12.15625" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="39"/>
-    <col min="27" max="29" width="23.578125" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="39"/>
+    <col min="2" max="4" width="10.6640625" style="39" customWidth="1"/>
+    <col min="5" max="5" width="1.88671875" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.88671875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.44140625" style="39"/>
+    <col min="21" max="21" width="11.44140625" style="97"/>
+    <col min="22" max="22" width="12.88671875" style="39" customWidth="1"/>
+    <col min="23" max="23" width="11.44140625" style="39"/>
+    <col min="24" max="24" width="12.88671875" style="97" customWidth="1"/>
+    <col min="25" max="25" width="12.109375" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="39"/>
+    <col min="27" max="29" width="23.5546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -60368,13 +60371,13 @@
       <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.41796875" style="111"/>
-    <col min="26" max="26" width="11.26171875" customWidth="1"/>
-    <col min="27" max="29" width="22.578125" customWidth="1"/>
+    <col min="25" max="25" width="11.44140625" style="111"/>
+    <col min="26" max="26" width="11.21875" customWidth="1"/>
+    <col min="27" max="29" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -61468,13 +61471,13 @@
       <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="15.83984375" customWidth="1"/>
-    <col min="20" max="20" width="15.26171875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.41796875" style="111"/>
+    <col min="19" max="19" width="15.88671875" customWidth="1"/>
+    <col min="20" max="20" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.44140625" style="111"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -61979,27 +61982,27 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:AX98"/>
   <sheetViews>
-    <sheetView topLeftCell="R58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+    <sheetView topLeftCell="X69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA83" sqref="AA83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.41796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.68359375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="7" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="7" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="11.41796875" style="7"/>
-    <col min="21" max="21" width="11.41796875" style="69"/>
-    <col min="22" max="22" width="11.41796875" style="7"/>
-    <col min="23" max="23" width="37.26171875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="54.578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.41796875" style="7" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="7"/>
-    <col min="27" max="29" width="22.83984375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="7"/>
+    <col min="1" max="1" width="3.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="7" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="11.44140625" style="7"/>
+    <col min="21" max="21" width="11.44140625" style="69"/>
+    <col min="22" max="22" width="11.44140625" style="7"/>
+    <col min="23" max="23" width="37.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="54.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.44140625" style="7" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="7"/>
+    <col min="27" max="29" width="22.88671875" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -62523,7 +62526,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="176" t="s">
-        <v>451</v>
+        <v>613</v>
       </c>
       <c r="AB8" s="176" t="s">
         <v>445</v>
@@ -63491,8 +63494,8 @@
       <c r="Z24" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA24" s="176" t="s">
-        <v>451</v>
+      <c r="AA24" t="s">
+        <v>613</v>
       </c>
       <c r="AB24" s="176" t="s">
         <v>445</v>
@@ -64462,8 +64465,8 @@
       <c r="Z40" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA40" s="176" t="s">
-        <v>451</v>
+      <c r="AA40" t="s">
+        <v>613</v>
       </c>
       <c r="AB40" s="176" t="s">
         <v>445</v>
@@ -65433,8 +65436,8 @@
       <c r="Z56" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA56" s="176" t="s">
-        <v>451</v>
+      <c r="AA56" t="s">
+        <v>613</v>
       </c>
       <c r="AB56" s="176" t="s">
         <v>445</v>
@@ -66404,8 +66407,8 @@
       <c r="Z72" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA72" s="176" t="s">
-        <v>451</v>
+      <c r="AA72" t="s">
+        <v>613</v>
       </c>
       <c r="AB72" s="176" t="s">
         <v>445</v>
@@ -67375,8 +67378,8 @@
       <c r="Z88" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA88" s="176" t="s">
-        <v>451</v>
+      <c r="AA88" t="s">
+        <v>613</v>
       </c>
       <c r="AB88" s="176" t="s">
         <v>445</v>
@@ -68000,23 +68003,23 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:AX44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA24" sqref="AA24:AB24"/>
+    <sheetView topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.68359375" customWidth="1"/>
-    <col min="7" max="7" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="1.83984375" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="10" customWidth="1"/>
-    <col min="23" max="23" width="35.83984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.41796875" style="111"/>
-    <col min="27" max="29" width="22.83984375" customWidth="1"/>
+    <col min="2" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="1.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" style="10" customWidth="1"/>
+    <col min="23" max="23" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.44140625" style="111"/>
+    <col min="27" max="29" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -68618,7 +68621,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="89" t="s">
-        <v>451</v>
+        <v>613</v>
       </c>
       <c r="AB8" s="89" t="s">
         <v>445</v>
@@ -70018,7 +70021,7 @@
         <v>0</v>
       </c>
       <c r="AA29" s="89" t="s">
-        <v>451</v>
+        <v>613</v>
       </c>
       <c r="AB29" s="89" t="s">
         <v>445</v>
@@ -71101,22 +71104,22 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AA24" sqref="AA24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.26171875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.68359375" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" customWidth="1"/>
-    <col min="24" max="24" width="8.15625" customWidth="1"/>
-    <col min="25" max="25" width="8.15625" style="111" customWidth="1"/>
-    <col min="27" max="29" width="22.68359375" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" customWidth="1"/>
+    <col min="24" max="24" width="8.109375" customWidth="1"/>
+    <col min="25" max="25" width="8.109375" style="111" customWidth="1"/>
+    <col min="27" max="29" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -71705,7 +71708,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="89" t="s">
-        <v>451</v>
+        <v>613</v>
       </c>
       <c r="AB8" s="89" t="s">
         <v>445</v>
@@ -72670,7 +72673,7 @@
         <v>0</v>
       </c>
       <c r="AA23" s="89" t="s">
-        <v>451</v>
+        <v>613</v>
       </c>
       <c r="AB23" s="89" t="s">
         <v>445</v>
@@ -73340,25 +73343,25 @@
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:AX23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3:AB3"/>
+    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.26171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.68359375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="1.83984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.83984375" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="11.41796875" style="2"/>
-    <col min="23" max="23" width="35.83984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.41796875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="10.41796875" style="113" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="2"/>
-    <col min="27" max="29" width="22.83984375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="2"/>
+    <col min="1" max="1" width="4.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="1.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.88671875" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="11.44140625" style="2"/>
+    <col min="23" max="23" width="35.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.44140625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="10.44140625" style="113" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="2"/>
+    <col min="27" max="29" width="22.88671875" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -73875,8 +73878,8 @@
       <c r="Z8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA8" s="89" t="s">
-        <v>451</v>
+      <c r="AA8" t="s">
+        <v>613</v>
       </c>
       <c r="AB8" s="89" t="s">
         <v>445</v>
@@ -74769,16 +74772,16 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.68359375" style="38" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="38" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="38" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="38" bestFit="1" customWidth="1"/>
-    <col min="18" max="26" width="11.41796875" style="38"/>
-    <col min="27" max="29" width="22.83984375" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.6640625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="1.88671875" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.88671875" style="38" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="38" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="18" max="26" width="11.44140625" style="38"/>
+    <col min="27" max="29" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -75619,20 +75622,20 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.68359375" style="56" customWidth="1"/>
-    <col min="7" max="7" width="1.83984375" style="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="1.83984375" style="56" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="56" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="56" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="56"/>
-    <col min="19" max="19" width="30.26171875" style="56" customWidth="1"/>
-    <col min="20" max="21" width="11.41796875" style="56" customWidth="1"/>
-    <col min="22" max="26" width="11.41796875" style="56"/>
-    <col min="27" max="29" width="22.83984375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="56"/>
+    <col min="1" max="1" width="3.88671875" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.6640625" style="56" customWidth="1"/>
+    <col min="7" max="7" width="1.88671875" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="1.88671875" style="56" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.6640625" style="56" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.6640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" style="56"/>
+    <col min="19" max="19" width="30.21875" style="56" customWidth="1"/>
+    <col min="20" max="21" width="11.44140625" style="56" customWidth="1"/>
+    <col min="22" max="26" width="11.44140625" style="56"/>
+    <col min="27" max="29" width="22.88671875" customWidth="1"/>
+    <col min="51" max="16384" width="11.44140625" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">

</xml_diff>

<commit_message>
-Selection Criteria Part IV: added newly created espd.part4.crit.explain.supply.contracts.environmental.law key to el/en.json files (GES-97 JIRA Issue) -Updated taxonomy 2.1.0 REGULATED
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria\IdeaProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD02F83-86BE-4ED4-AB41-773A66EEE84C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4780D8-6638-4DCE-9CD1-D492202BF290}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="22" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12442" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12442" uniqueCount="616">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1906,6 +1906,12 @@
   </si>
   <si>
     <t>espd.crit.please.give.more.details</t>
+  </si>
+  <si>
+    <t>espd.crit.ratio.type</t>
+  </si>
+  <si>
+    <t>espd.part4.crit.explain.supply.contracts.environmental.law</t>
   </si>
 </sst>
 </file>
@@ -22921,8 +22927,8 @@
   <sheetPr codeName="Hoja17"/>
   <dimension ref="A1:AX15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6:AA7"/>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -23338,7 +23344,7 @@
         <v>0</v>
       </c>
       <c r="AA6" s="159" t="s">
-        <v>538</v>
+        <v>614</v>
       </c>
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
@@ -43389,8 +43395,8 @@
   <sheetPr codeName="Hoja26"/>
   <dimension ref="A1:AX47"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB26" sqref="AB26"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA38" sqref="AA38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -45605,7 +45611,7 @@
       <c r="AB37" s="89"/>
       <c r="AC37" s="89"/>
     </row>
-    <row r="38" spans="1:50" ht="43.2">
+    <row r="38" spans="1:50">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -45655,7 +45661,7 @@
         <v>0</v>
       </c>
       <c r="AA38" s="177" t="s">
-        <v>590</v>
+        <v>615</v>
       </c>
       <c r="AB38" s="89"/>
       <c r="AC38" s="89"/>
@@ -71104,7 +71110,7 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
-Selection Criteria Part IV, Section C hint change: created and added new espd.crit.please.describe property key to en/el.json files. -Updated 2.1.0 REGULATED Taxonomy, replaced espd.crit.please.describe.them key in Selection-Section C criteria (GES-102 JIRA Issue)
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria\IdeaProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4780D8-6638-4DCE-9CD1-D492202BF290}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE686A69-5441-40F2-A8E6-97230CB9AB16}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="22" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="17" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12442" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12442" uniqueCount="617">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1912,6 +1912,9 @@
   </si>
   <si>
     <t>espd.part4.crit.explain.supply.contracts.environmental.law</t>
+  </si>
+  <si>
+    <t>espd.crit.please.describe</t>
   </si>
 </sst>
 </file>
@@ -32328,8 +32331,8 @@
   <sheetPr codeName="Hoja21"/>
   <dimension ref="A1:AC98"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA87" sqref="AA87:AB87"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA42" sqref="AA42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -32666,7 +32669,7 @@
       <c r="AB5" s="89"/>
       <c r="AC5" s="89"/>
     </row>
-    <row r="6" spans="1:29" ht="28.8">
+    <row r="6" spans="1:29">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -32717,8 +32720,8 @@
       <c r="Z6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA6" s="159" t="s">
-        <v>451</v>
+      <c r="AA6" t="s">
+        <v>616</v>
       </c>
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
@@ -33298,7 +33301,7 @@
       <c r="AB17" s="89"/>
       <c r="AC17" s="89"/>
     </row>
-    <row r="18" spans="1:29" ht="28.8">
+    <row r="18" spans="1:29">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -33349,8 +33352,8 @@
       <c r="Z18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA18" s="159" t="s">
-        <v>451</v>
+      <c r="AA18" t="s">
+        <v>616</v>
       </c>
       <c r="AB18" s="89"/>
       <c r="AC18" s="89"/>
@@ -33940,7 +33943,7 @@
       <c r="AB29" s="89"/>
       <c r="AC29" s="89"/>
     </row>
-    <row r="30" spans="1:29" ht="28.8">
+    <row r="30" spans="1:29">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -33991,8 +33994,8 @@
       <c r="Z30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA30" s="159" t="s">
-        <v>451</v>
+      <c r="AA30" t="s">
+        <v>616</v>
       </c>
       <c r="AB30" s="89"/>
       <c r="AC30" s="89"/>
@@ -34582,7 +34585,7 @@
       <c r="AB41" s="89"/>
       <c r="AC41" s="89"/>
     </row>
-    <row r="42" spans="1:29" ht="28.8">
+    <row r="42" spans="1:29">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -34633,8 +34636,8 @@
       <c r="Z42" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA42" s="159" t="s">
-        <v>451</v>
+      <c r="AA42" s="198" t="s">
+        <v>616</v>
       </c>
       <c r="AB42" s="89"/>
       <c r="AC42" s="89"/>
@@ -35224,7 +35227,7 @@
       <c r="AB53" s="89"/>
       <c r="AC53" s="89"/>
     </row>
-    <row r="54" spans="1:29" ht="28.8">
+    <row r="54" spans="1:29">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -35275,8 +35278,8 @@
       <c r="Z54" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA54" s="159" t="s">
-        <v>451</v>
+      <c r="AA54" t="s">
+        <v>616</v>
       </c>
       <c r="AB54" s="89"/>
       <c r="AC54" s="89"/>
@@ -35866,7 +35869,7 @@
       <c r="AB65" s="89"/>
       <c r="AC65" s="89"/>
     </row>
-    <row r="66" spans="1:29" ht="28.8">
+    <row r="66" spans="1:29">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -35917,8 +35920,8 @@
       <c r="Z66" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA66" s="159" t="s">
-        <v>451</v>
+      <c r="AA66" s="198" t="s">
+        <v>616</v>
       </c>
       <c r="AB66" s="89"/>
       <c r="AC66" s="89"/>
@@ -36508,7 +36511,7 @@
       <c r="AB77" s="89"/>
       <c r="AC77" s="89"/>
     </row>
-    <row r="78" spans="1:29" ht="28.8">
+    <row r="78" spans="1:29">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -36559,8 +36562,8 @@
       <c r="Z78" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA78" s="159" t="s">
-        <v>451</v>
+      <c r="AA78" s="198" t="s">
+        <v>616</v>
       </c>
       <c r="AB78" s="89"/>
       <c r="AC78" s="89"/>
@@ -37150,7 +37153,7 @@
       <c r="AB89" s="89"/>
       <c r="AC89" s="89"/>
     </row>
-    <row r="90" spans="1:29" ht="28.8">
+    <row r="90" spans="1:29">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
@@ -37201,8 +37204,8 @@
       <c r="Z90" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AA90" s="159" t="s">
-        <v>451</v>
+      <c r="AA90" s="198" t="s">
+        <v>616</v>
       </c>
       <c r="AB90" s="89"/>
       <c r="AC90" s="89"/>
@@ -37639,6 +37642,7 @@
     <hyperlink ref="T95" r:id="rId8" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1400-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -43395,7 +43399,7 @@
   <sheetPr codeName="Hoja26"/>
   <dimension ref="A1:AX47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AA38" sqref="AA38"/>
     </sheetView>
   </sheetViews>
@@ -45611,7 +45615,7 @@
       <c r="AB37" s="89"/>
       <c r="AC37" s="89"/>
     </row>
-    <row r="38" spans="1:50">
+    <row r="38" spans="1:50" ht="43.2">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
-Criterion 59, translation problem: Corrected property keys at taxonomy REGULATED 2.1.0
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria\IdeaProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE686A69-5441-40F2-A8E6-97230CB9AB16}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB641D2-8364-4EDD-9E44-E7A81089C99A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="17" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="24" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -1860,15 +1860,6 @@
     <t>espd.crit.eo.has.cert.soc</t>
   </si>
   <si>
-    <t>espd.createeo.eo.group.role</t>
-  </si>
-  <si>
-    <t>espd.createeo.other.eo.part</t>
-  </si>
-  <si>
-    <t>espd.createeo.name.part.group</t>
-  </si>
-  <si>
     <t>espd.part2.is.eo.proc.together</t>
   </si>
   <si>
@@ -1915,6 +1906,15 @@
   </si>
   <si>
     <t>espd.crit.please.describe</t>
+  </si>
+  <si>
+    <t>espd.crit.eo.group.role</t>
+  </si>
+  <si>
+    <t>espd.crit.name.part.group</t>
+  </si>
+  <si>
+    <t>espd.crit.other.eo.part</t>
   </si>
 </sst>
 </file>
@@ -23347,7 +23347,7 @@
         <v>0</v>
       </c>
       <c r="AA6" s="159" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
@@ -32331,7 +32331,7 @@
   <sheetPr codeName="Hoja21"/>
   <dimension ref="A1:AC98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AA42" sqref="AA42"/>
     </sheetView>
   </sheetViews>
@@ -32721,7 +32721,7 @@
         <v>0</v>
       </c>
       <c r="AA6" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
@@ -33353,7 +33353,7 @@
         <v>0</v>
       </c>
       <c r="AA18" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AB18" s="89"/>
       <c r="AC18" s="89"/>
@@ -33995,7 +33995,7 @@
         <v>0</v>
       </c>
       <c r="AA30" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AB30" s="89"/>
       <c r="AC30" s="89"/>
@@ -34637,7 +34637,7 @@
         <v>0</v>
       </c>
       <c r="AA42" s="198" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AB42" s="89"/>
       <c r="AC42" s="89"/>
@@ -35279,7 +35279,7 @@
         <v>0</v>
       </c>
       <c r="AA54" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AB54" s="89"/>
       <c r="AC54" s="89"/>
@@ -35921,7 +35921,7 @@
         <v>0</v>
       </c>
       <c r="AA66" s="198" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AB66" s="89"/>
       <c r="AC66" s="89"/>
@@ -36563,7 +36563,7 @@
         <v>0</v>
       </c>
       <c r="AA78" s="198" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AB78" s="89"/>
       <c r="AC78" s="89"/>
@@ -37205,7 +37205,7 @@
         <v>0</v>
       </c>
       <c r="AA90" s="198" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AB90" s="89"/>
       <c r="AC90" s="89"/>
@@ -45665,7 +45665,7 @@
         <v>0</v>
       </c>
       <c r="AA38" s="177" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="AB38" s="89"/>
       <c r="AC38" s="89"/>
@@ -46700,7 +46700,7 @@
       <c r="Y7" s="99"/>
       <c r="Z7" s="100"/>
       <c r="AA7" s="224" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="AB7" s="89"/>
       <c r="AC7" s="62"/>
@@ -46774,7 +46774,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="224" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="AB8" s="89"/>
       <c r="AC8" s="62"/>
@@ -49999,8 +49999,8 @@
   <sheetPr codeName="Hoja29"/>
   <dimension ref="A1:AX142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13:AC15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -50233,7 +50233,7 @@
         <v>0</v>
       </c>
       <c r="AA3" s="158" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="AB3" s="163"/>
       <c r="AC3" s="163"/>
@@ -50481,7 +50481,7 @@
       <c r="AW6"/>
       <c r="AX6"/>
     </row>
-    <row r="7" spans="1:50" s="97" customFormat="1" ht="28.8">
+    <row r="7" spans="1:50" s="97" customFormat="1">
       <c r="A7" s="29"/>
       <c r="B7" s="28"/>
       <c r="C7" s="34"/>
@@ -50522,8 +50522,8 @@
       <c r="Z7" s="147" t="s">
         <v>433</v>
       </c>
-      <c r="AA7" s="159" t="s">
-        <v>598</v>
+      <c r="AA7" t="s">
+        <v>614</v>
       </c>
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
@@ -50549,7 +50549,7 @@
       <c r="AW7"/>
       <c r="AX7"/>
     </row>
-    <row r="8" spans="1:50" s="97" customFormat="1" ht="28.8">
+    <row r="8" spans="1:50" s="97" customFormat="1">
       <c r="A8" s="29" t="s">
         <v>0</v>
       </c>
@@ -50596,8 +50596,8 @@
       <c r="Z8" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="AA8" s="159" t="s">
-        <v>599</v>
+      <c r="AA8" t="s">
+        <v>616</v>
       </c>
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
@@ -50623,7 +50623,7 @@
       <c r="AW8"/>
       <c r="AX8"/>
     </row>
-    <row r="9" spans="1:50" s="97" customFormat="1" ht="28.8">
+    <row r="9" spans="1:50" s="97" customFormat="1">
       <c r="A9" s="29"/>
       <c r="B9" s="28"/>
       <c r="C9" s="34"/>
@@ -50664,8 +50664,8 @@
       <c r="Z9" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="AA9" s="159" t="s">
-        <v>600</v>
+      <c r="AA9" t="s">
+        <v>615</v>
       </c>
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
@@ -56952,7 +56952,7 @@
         <v>0</v>
       </c>
       <c r="AA3" s="163" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="AB3" s="215"/>
       <c r="AC3" s="215"/>
@@ -57142,7 +57142,7 @@
       <c r="Y7" s="127"/>
       <c r="Z7" s="116"/>
       <c r="AA7" s="224" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="AB7" s="224" t="s">
         <v>445</v>
@@ -57189,7 +57189,7 @@
         <v>437</v>
       </c>
       <c r="AA8" s="224" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AB8" s="224" t="s">
         <v>445</v>
@@ -57238,10 +57238,10 @@
         <v>439</v>
       </c>
       <c r="AA9" s="224" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="AB9" s="224" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="AC9" s="89"/>
     </row>
@@ -58332,7 +58332,7 @@
         <v>0</v>
       </c>
       <c r="AA3" s="163" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="AB3" s="163"/>
       <c r="AC3" s="163"/>
@@ -58606,7 +58606,7 @@
       <c r="Y7" s="101"/>
       <c r="Z7" s="28"/>
       <c r="AA7" s="224" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="AB7" s="224" t="s">
         <v>445</v>
@@ -58674,7 +58674,7 @@
         <v>437</v>
       </c>
       <c r="AA8" s="224" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AB8" s="224" t="s">
         <v>445</v>
@@ -58744,10 +58744,10 @@
         <v>439</v>
       </c>
       <c r="AA9" s="224" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="AB9" s="224" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="AC9" s="89"/>
       <c r="AD9"/>
@@ -59507,7 +59507,7 @@
         <v>0</v>
       </c>
       <c r="AA3" s="163" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="AB3" s="163"/>
       <c r="AC3" s="163"/>
@@ -60598,10 +60598,10 @@
         <v>0</v>
       </c>
       <c r="AA3" s="163" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="AB3" s="163" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="AC3" s="163"/>
       <c r="AD3" s="111"/>
@@ -62536,7 +62536,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="176" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AB8" s="176" t="s">
         <v>445</v>
@@ -63505,7 +63505,7 @@
         <v>0</v>
       </c>
       <c r="AA24" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AB24" s="176" t="s">
         <v>445</v>
@@ -64476,7 +64476,7 @@
         <v>0</v>
       </c>
       <c r="AA40" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AB40" s="176" t="s">
         <v>445</v>
@@ -65447,7 +65447,7 @@
         <v>0</v>
       </c>
       <c r="AA56" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AB56" s="176" t="s">
         <v>445</v>
@@ -66418,7 +66418,7 @@
         <v>0</v>
       </c>
       <c r="AA72" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AB72" s="176" t="s">
         <v>445</v>
@@ -67389,7 +67389,7 @@
         <v>0</v>
       </c>
       <c r="AA88" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AB88" s="176" t="s">
         <v>445</v>
@@ -68631,7 +68631,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="89" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AB8" s="89" t="s">
         <v>445</v>
@@ -70031,7 +70031,7 @@
         <v>0</v>
       </c>
       <c r="AA29" s="89" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AB29" s="89" t="s">
         <v>445</v>
@@ -71718,7 +71718,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="89" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AB8" s="89" t="s">
         <v>445</v>
@@ -72683,7 +72683,7 @@
         <v>0</v>
       </c>
       <c r="AA23" s="89" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AB23" s="89" t="s">
         <v>445</v>
@@ -73889,7 +73889,7 @@
         <v>0</v>
       </c>
       <c r="AA8" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="AB8" s="89" t="s">
         <v>445</v>

</xml_diff>

<commit_message>
-Fifth page, text removed: espd.part5.text.eo.declares.that property key removed from taxonomy regulated 2.1.0 (GES-98 JIRA issue)
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria\IdeaProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB641D2-8364-4EDD-9E44-E7A81089C99A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F8D8A3-4EF3-4D03-9A24-F8FD9BB387E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="24" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="30" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12442" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12441" uniqueCount="616">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1876,9 +1876,6 @@
   </si>
   <si>
     <t>espd.part5.title.eo.declares.that</t>
-  </si>
-  <si>
-    <t>espd.part5.text.eo.declares.that</t>
   </si>
   <si>
     <t>espd.crit.entity.id</t>
@@ -23347,7 +23344,7 @@
         <v>0</v>
       </c>
       <c r="AA6" s="159" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
@@ -32721,7 +32718,7 @@
         <v>0</v>
       </c>
       <c r="AA6" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
@@ -33353,7 +33350,7 @@
         <v>0</v>
       </c>
       <c r="AA18" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AB18" s="89"/>
       <c r="AC18" s="89"/>
@@ -33995,7 +33992,7 @@
         <v>0</v>
       </c>
       <c r="AA30" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AB30" s="89"/>
       <c r="AC30" s="89"/>
@@ -34637,7 +34634,7 @@
         <v>0</v>
       </c>
       <c r="AA42" s="198" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AB42" s="89"/>
       <c r="AC42" s="89"/>
@@ -35279,7 +35276,7 @@
         <v>0</v>
       </c>
       <c r="AA54" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AB54" s="89"/>
       <c r="AC54" s="89"/>
@@ -35921,7 +35918,7 @@
         <v>0</v>
       </c>
       <c r="AA66" s="198" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AB66" s="89"/>
       <c r="AC66" s="89"/>
@@ -36563,7 +36560,7 @@
         <v>0</v>
       </c>
       <c r="AA78" s="198" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AB78" s="89"/>
       <c r="AC78" s="89"/>
@@ -37205,7 +37202,7 @@
         <v>0</v>
       </c>
       <c r="AA90" s="198" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AB90" s="89"/>
       <c r="AC90" s="89"/>
@@ -45665,7 +45662,7 @@
         <v>0</v>
       </c>
       <c r="AA38" s="177" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AB38" s="89"/>
       <c r="AC38" s="89"/>
@@ -46700,7 +46697,7 @@
       <c r="Y7" s="99"/>
       <c r="Z7" s="100"/>
       <c r="AA7" s="224" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AB7" s="89"/>
       <c r="AC7" s="62"/>
@@ -46774,7 +46771,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="224" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AB8" s="89"/>
       <c r="AC8" s="62"/>
@@ -49999,7 +49996,7 @@
   <sheetPr codeName="Hoja29"/>
   <dimension ref="A1:AX142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
@@ -50523,7 +50520,7 @@
         <v>433</v>
       </c>
       <c r="AA7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
@@ -50597,7 +50594,7 @@
         <v>0</v>
       </c>
       <c r="AA8" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
@@ -50665,7 +50662,7 @@
         <v>0</v>
       </c>
       <c r="AA9" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
@@ -57189,7 +57186,7 @@
         <v>437</v>
       </c>
       <c r="AA8" s="224" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AB8" s="224" t="s">
         <v>445</v>
@@ -57238,10 +57235,10 @@
         <v>439</v>
       </c>
       <c r="AA9" s="224" t="s">
+        <v>605</v>
+      </c>
+      <c r="AB9" s="224" t="s">
         <v>606</v>
-      </c>
-      <c r="AB9" s="224" t="s">
-        <v>607</v>
       </c>
       <c r="AC9" s="89"/>
     </row>
@@ -58674,7 +58671,7 @@
         <v>437</v>
       </c>
       <c r="AA8" s="224" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AB8" s="224" t="s">
         <v>445</v>
@@ -58744,10 +58741,10 @@
         <v>439</v>
       </c>
       <c r="AA9" s="224" t="s">
+        <v>605</v>
+      </c>
+      <c r="AB9" s="224" t="s">
         <v>606</v>
-      </c>
-      <c r="AB9" s="224" t="s">
-        <v>607</v>
       </c>
       <c r="AC9" s="89"/>
       <c r="AD9"/>
@@ -60377,8 +60374,8 @@
   <sheetPr codeName="Hoja34"/>
   <dimension ref="A1:AX17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
@@ -60600,9 +60597,7 @@
       <c r="AA3" s="163" t="s">
         <v>603</v>
       </c>
-      <c r="AB3" s="163" t="s">
-        <v>604</v>
-      </c>
+      <c r="AB3" s="163"/>
       <c r="AC3" s="163"/>
       <c r="AD3" s="111"/>
       <c r="AE3" s="111"/>
@@ -62536,7 +62531,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="176" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB8" s="176" t="s">
         <v>445</v>
@@ -63505,7 +63500,7 @@
         <v>0</v>
       </c>
       <c r="AA24" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB24" s="176" t="s">
         <v>445</v>
@@ -64476,7 +64471,7 @@
         <v>0</v>
       </c>
       <c r="AA40" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB40" s="176" t="s">
         <v>445</v>
@@ -65447,7 +65442,7 @@
         <v>0</v>
       </c>
       <c r="AA56" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB56" s="176" t="s">
         <v>445</v>
@@ -66418,7 +66413,7 @@
         <v>0</v>
       </c>
       <c r="AA72" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB72" s="176" t="s">
         <v>445</v>
@@ -67389,7 +67384,7 @@
         <v>0</v>
       </c>
       <c r="AA88" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB88" s="176" t="s">
         <v>445</v>
@@ -68631,7 +68626,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="89" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB8" s="89" t="s">
         <v>445</v>
@@ -70031,7 +70026,7 @@
         <v>0</v>
       </c>
       <c r="AA29" s="89" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB29" s="89" t="s">
         <v>445</v>
@@ -71718,7 +71713,7 @@
         <v>0</v>
       </c>
       <c r="AA8" s="89" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB8" s="89" t="s">
         <v>445</v>
@@ -72683,7 +72678,7 @@
         <v>0</v>
       </c>
       <c r="AA23" s="89" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB23" s="89" t="s">
         <v>445</v>
@@ -73889,7 +73884,7 @@
         <v>0</v>
       </c>
       <c r="AA8" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB8" s="89" t="s">
         <v>445</v>

</xml_diff>

<commit_message>
Mandatory fields are not marked (ESPD-109 Jira issue)
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Documents\NetBeansProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NetbeansProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30878EA-AF5B-4789-8FB5-F294636C71DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940751C6-52F8-4AB5-80F6-0BB56AA329D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="588" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="29205" windowHeight="15435" tabRatio="588" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -5693,23 +5693,23 @@
       <selection activeCell="AA123" sqref="AA123:AB123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.83984375" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.68359375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="2.83984375" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.83984375" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="3.83984375" style="25" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="3.83984375" style="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="17.15625" style="25" customWidth="1"/>
-    <col min="21" max="21" width="13.83984375" style="54" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="17.15625" style="87" customWidth="1"/>
-    <col min="24" max="25" width="17.15625" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="25" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.7109375" style="25" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="3.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="17.140625" style="25" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="17.140625" style="87" customWidth="1"/>
+    <col min="24" max="25" width="17.140625" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="25" customWidth="1"/>
     <col min="27" max="27" width="24" style="25" customWidth="1"/>
-    <col min="28" max="28" width="22.68359375" style="25" customWidth="1"/>
-    <col min="29" max="29" width="22.83984375" style="25" customWidth="1"/>
-    <col min="30" max="16384" width="11.41796875" style="25"/>
+    <col min="28" max="28" width="22.7109375" style="25" customWidth="1"/>
+    <col min="29" max="29" width="22.85546875" style="25" customWidth="1"/>
+    <col min="30" max="16384" width="11.42578125" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -5870,7 +5870,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="28.8">
+    <row r="3" spans="1:29" ht="30">
       <c r="A3" s="55">
         <v>1</v>
       </c>
@@ -6155,7 +6155,7 @@
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
     </row>
-    <row r="8" spans="1:29" s="56" customFormat="1">
+    <row r="8" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A8" s="55" t="s">
         <v>0</v>
       </c>
@@ -6326,7 +6326,7 @@
       <c r="AB10" s="89"/>
       <c r="AC10" s="89"/>
     </row>
-    <row r="11" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="11" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A11" s="55" t="s">
         <v>0</v>
       </c>
@@ -6438,7 +6438,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="13" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -6554,7 +6554,7 @@
       <c r="AB14" s="89"/>
       <c r="AC14" s="89"/>
     </row>
-    <row r="15" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="15" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A15" s="55" t="s">
         <v>0</v>
       </c>
@@ -6888,7 +6888,7 @@
       <c r="AB20" s="89"/>
       <c r="AC20" s="89"/>
     </row>
-    <row r="21" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="21" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -7206,7 +7206,7 @@
       <c r="AB26" s="163"/>
       <c r="AC26" s="163"/>
     </row>
-    <row r="27" spans="1:29" s="56" customFormat="1">
+    <row r="27" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A27" s="55">
         <v>2</v>
       </c>
@@ -7485,7 +7485,7 @@
       <c r="AB31" s="89"/>
       <c r="AC31" s="89"/>
     </row>
-    <row r="32" spans="1:29" s="56" customFormat="1">
+    <row r="32" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A32" s="55" t="s">
         <v>0</v>
       </c>
@@ -7656,7 +7656,7 @@
       <c r="AB34" s="89"/>
       <c r="AC34" s="89"/>
     </row>
-    <row r="35" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="35" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A35" s="55" t="s">
         <v>0</v>
       </c>
@@ -7768,7 +7768,7 @@
       <c r="AB36" s="89"/>
       <c r="AC36" s="89"/>
     </row>
-    <row r="37" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="37" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A37" s="55" t="s">
         <v>0</v>
       </c>
@@ -7884,7 +7884,7 @@
       <c r="AB38" s="89"/>
       <c r="AC38" s="89"/>
     </row>
-    <row r="39" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="39" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A39" s="55" t="s">
         <v>0</v>
       </c>
@@ -8218,7 +8218,7 @@
       <c r="AB44" s="89"/>
       <c r="AC44" s="89"/>
     </row>
-    <row r="45" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="45" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A45" s="55" t="s">
         <v>0</v>
       </c>
@@ -8825,7 +8825,7 @@
       <c r="AB55" s="89"/>
       <c r="AC55" s="89"/>
     </row>
-    <row r="56" spans="1:29" s="56" customFormat="1">
+    <row r="56" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A56" s="55" t="s">
         <v>0</v>
       </c>
@@ -8996,7 +8996,7 @@
       <c r="AB58" s="89"/>
       <c r="AC58" s="89"/>
     </row>
-    <row r="59" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="59" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A59" s="55" t="s">
         <v>0</v>
       </c>
@@ -9108,7 +9108,7 @@
       <c r="AB60" s="89"/>
       <c r="AC60" s="89"/>
     </row>
-    <row r="61" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="61" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A61" s="55" t="s">
         <v>0</v>
       </c>
@@ -9224,7 +9224,7 @@
       <c r="AB62" s="89"/>
       <c r="AC62" s="89"/>
     </row>
-    <row r="63" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="63" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A63" s="55" t="s">
         <v>0</v>
       </c>
@@ -9558,7 +9558,7 @@
       <c r="AB68" s="89"/>
       <c r="AC68" s="89"/>
     </row>
-    <row r="69" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="69" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A69" s="55" t="s">
         <v>0</v>
       </c>
@@ -9876,7 +9876,7 @@
       <c r="AB74" s="163"/>
       <c r="AC74" s="163"/>
     </row>
-    <row r="75" spans="1:29" s="56" customFormat="1">
+    <row r="75" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A75" s="55">
         <v>4</v>
       </c>
@@ -10165,7 +10165,7 @@
       <c r="AB79" s="89"/>
       <c r="AC79" s="89"/>
     </row>
-    <row r="80" spans="1:29" s="56" customFormat="1">
+    <row r="80" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A80" s="55" t="s">
         <v>0</v>
       </c>
@@ -10336,7 +10336,7 @@
       <c r="AB82" s="89"/>
       <c r="AC82" s="89"/>
     </row>
-    <row r="83" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="83" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A83" s="55" t="s">
         <v>0</v>
       </c>
@@ -10448,7 +10448,7 @@
       <c r="AB84" s="89"/>
       <c r="AC84" s="89"/>
     </row>
-    <row r="85" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="85" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A85" s="55" t="s">
         <v>0</v>
       </c>
@@ -10564,7 +10564,7 @@
       <c r="AB86" s="89"/>
       <c r="AC86" s="89"/>
     </row>
-    <row r="87" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="87" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A87" s="55" t="s">
         <v>0</v>
       </c>
@@ -10898,7 +10898,7 @@
       <c r="AB92" s="89"/>
       <c r="AC92" s="89"/>
     </row>
-    <row r="93" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="93" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A93" s="55" t="s">
         <v>0</v>
       </c>
@@ -11216,7 +11216,7 @@
       <c r="AB98" s="163"/>
       <c r="AC98" s="163"/>
     </row>
-    <row r="99" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="99" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A99" s="55">
         <v>5</v>
       </c>
@@ -11505,7 +11505,7 @@
       <c r="AB103" s="89"/>
       <c r="AC103" s="89"/>
     </row>
-    <row r="104" spans="1:29" s="56" customFormat="1">
+    <row r="104" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A104" s="55" t="s">
         <v>0</v>
       </c>
@@ -11676,7 +11676,7 @@
       <c r="AB106" s="89"/>
       <c r="AC106" s="89"/>
     </row>
-    <row r="107" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="107" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A107" s="55" t="s">
         <v>0</v>
       </c>
@@ -11788,7 +11788,7 @@
       <c r="AB108" s="89"/>
       <c r="AC108" s="89"/>
     </row>
-    <row r="109" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="109" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A109" s="55" t="s">
         <v>0</v>
       </c>
@@ -11904,7 +11904,7 @@
       <c r="AB110" s="89"/>
       <c r="AC110" s="89"/>
     </row>
-    <row r="111" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="111" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A111" s="55" t="s">
         <v>0</v>
       </c>
@@ -12238,7 +12238,7 @@
       <c r="AB116" s="89"/>
       <c r="AC116" s="89"/>
     </row>
-    <row r="117" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="117" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A117" s="55" t="s">
         <v>0</v>
       </c>
@@ -12556,7 +12556,7 @@
       <c r="AB122" s="163"/>
       <c r="AC122" s="163"/>
     </row>
-    <row r="123" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="123" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A123" s="55">
         <v>6</v>
       </c>
@@ -12843,7 +12843,7 @@
       <c r="AB127" s="89"/>
       <c r="AC127" s="89"/>
     </row>
-    <row r="128" spans="1:29" s="56" customFormat="1">
+    <row r="128" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A128" s="55" t="s">
         <v>0</v>
       </c>
@@ -13014,7 +13014,7 @@
       <c r="AB130" s="89"/>
       <c r="AC130" s="89"/>
     </row>
-    <row r="131" spans="1:29" s="56" customFormat="1" ht="25.5">
+    <row r="131" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A131" s="55" t="s">
         <v>0</v>
       </c>
@@ -13126,7 +13126,7 @@
       <c r="AB132" s="89"/>
       <c r="AC132" s="89"/>
     </row>
-    <row r="133" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="133" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A133" s="55" t="s">
         <v>0</v>
       </c>
@@ -13242,7 +13242,7 @@
       <c r="AB134" s="89"/>
       <c r="AC134" s="89"/>
     </row>
-    <row r="135" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="135" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A135" s="55" t="s">
         <v>0</v>
       </c>
@@ -13576,7 +13576,7 @@
       <c r="AB140" s="89"/>
       <c r="AC140" s="89"/>
     </row>
-    <row r="141" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="141" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A141" s="55" t="s">
         <v>0</v>
       </c>
@@ -13917,24 +13917,24 @@
       <selection activeCell="AA15" sqref="AA15:AB15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.68359375" style="2" customWidth="1"/>
-    <col min="3" max="5" width="10.68359375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="12.68359375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="2" customWidth="1"/>
     <col min="21" max="21" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="24" width="11.41796875" style="2"/>
-    <col min="25" max="25" width="11.41796875" style="113"/>
-    <col min="26" max="26" width="11.41796875" style="2"/>
-    <col min="27" max="29" width="23.15625" style="2" customWidth="1"/>
-    <col min="30" max="16384" width="11.41796875" style="2"/>
+    <col min="22" max="24" width="11.42578125" style="2"/>
+    <col min="25" max="25" width="11.42578125" style="113"/>
+    <col min="26" max="26" width="11.42578125" style="2"/>
+    <col min="27" max="29" width="23.140625" style="2" customWidth="1"/>
+    <col min="30" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" s="142" customFormat="1">
@@ -14115,7 +14115,7 @@
       <c r="AV2" s="203"/>
       <c r="AW2" s="203"/>
     </row>
-    <row r="3" spans="1:55" customFormat="1" ht="43.2">
+    <row r="3" spans="1:55" customFormat="1" ht="60">
       <c r="A3" s="29">
         <v>25</v>
       </c>
@@ -14597,7 +14597,7 @@
       <c r="BB8" s="202"/>
       <c r="BC8" s="202"/>
     </row>
-    <row r="9" spans="1:55" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:55" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -15069,7 +15069,7 @@
       <c r="BB14" s="202"/>
       <c r="BC14" s="202"/>
     </row>
-    <row r="15" spans="1:55" customFormat="1" ht="43.2">
+    <row r="15" spans="1:55" customFormat="1" ht="45">
       <c r="A15" s="29">
         <v>26</v>
       </c>
@@ -15523,7 +15523,7 @@
       <c r="AV20" s="202"/>
       <c r="AW20" s="202"/>
     </row>
-    <row r="21" spans="1:49" s="56" customFormat="1" ht="28.8">
+    <row r="21" spans="1:49" s="56" customFormat="1" ht="30">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -16263,13 +16263,13 @@
       <selection activeCell="AB18" sqref="AA18:AB18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.578125" style="111"/>
-    <col min="27" max="29" width="23.578125" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" style="111"/>
+    <col min="27" max="29" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -16430,7 +16430,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="43.2">
+    <row r="3" spans="1:50" ht="45">
       <c r="A3" s="29">
         <v>27</v>
       </c>
@@ -16722,7 +16722,7 @@
       <c r="AW7"/>
       <c r="AX7"/>
     </row>
-    <row r="8" spans="1:50" s="111" customFormat="1" ht="28.8">
+    <row r="8" spans="1:50" s="111" customFormat="1" ht="30">
       <c r="A8" s="29"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -16976,7 +16976,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="12" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -17294,7 +17294,7 @@
       <c r="AB17" s="163"/>
       <c r="AC17" s="163"/>
     </row>
-    <row r="18" spans="1:50" ht="43.2">
+    <row r="18" spans="1:50" ht="45">
       <c r="A18" s="29">
         <v>28</v>
       </c>
@@ -17647,7 +17647,7 @@
       <c r="AW22"/>
       <c r="AX22"/>
     </row>
-    <row r="23" spans="1:50" s="111" customFormat="1" ht="28.8">
+    <row r="23" spans="1:50" s="111" customFormat="1" ht="30">
       <c r="A23" s="29"/>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
@@ -17922,7 +17922,7 @@
       <c r="AB26" s="89"/>
       <c r="AC26" s="89"/>
     </row>
-    <row r="27" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="27" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A27" s="55" t="s">
         <v>0</v>
       </c>
@@ -18279,23 +18279,23 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="68" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" style="66" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" style="66" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.578125" style="66" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="66" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="66" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="66" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="66" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="66" customWidth="1"/>
-    <col min="19" max="19" width="27.578125" style="66" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" style="66" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="73" customWidth="1"/>
-    <col min="22" max="22" width="11.41796875" style="66" customWidth="1"/>
-    <col min="23" max="26" width="11.41796875" style="66"/>
-    <col min="27" max="29" width="23.41796875" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="66" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="66" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="66" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="66" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="66" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="66" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="66" customWidth="1"/>
+    <col min="19" max="19" width="27.5703125" style="66" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="66" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="73" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" style="66" customWidth="1"/>
+    <col min="23" max="26" width="11.42578125" style="66"/>
+    <col min="27" max="29" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -18456,7 +18456,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="43.2">
+    <row r="3" spans="1:29" ht="45">
       <c r="A3" s="65">
         <v>29</v>
       </c>
@@ -18861,7 +18861,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -19187,18 +19187,18 @@
       <selection activeCell="AA6" sqref="AA6:AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.68359375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.578125" style="111"/>
-    <col min="27" max="29" width="23.578125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" style="111"/>
+    <col min="27" max="29" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -19359,7 +19359,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="43.2">
+    <row r="3" spans="1:50" ht="45">
       <c r="A3" s="4">
         <v>30</v>
       </c>
@@ -19530,7 +19530,7 @@
       <c r="AB5" s="89"/>
       <c r="AC5" s="89"/>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:50" ht="30">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -19591,7 +19591,7 @@
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
     </row>
-    <row r="7" spans="1:50">
+    <row r="7" spans="1:50" ht="30">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -19758,7 +19758,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -20110,25 +20110,25 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" style="7" customWidth="1"/>
-    <col min="3" max="5" width="10.68359375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="7" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="7" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="7" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="7"/>
-    <col min="19" max="19" width="25.15625" style="7" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" style="7" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="69" customWidth="1"/>
-    <col min="22" max="22" width="18.578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.41796875" style="7"/>
-    <col min="24" max="25" width="11.41796875" style="69"/>
-    <col min="26" max="26" width="11.41796875" style="7"/>
-    <col min="27" max="29" width="23.41796875" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="7"/>
+    <col min="2" max="2" width="7.42578125" style="7" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="7" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="7" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="7"/>
+    <col min="19" max="19" width="25.140625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="7" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="69" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="7"/>
+    <col min="24" max="25" width="11.42578125" style="69"/>
+    <col min="26" max="26" width="11.42578125" style="7"/>
+    <col min="27" max="29" width="23.42578125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -20289,7 +20289,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="43.2">
+    <row r="3" spans="1:29" ht="45">
       <c r="A3" s="4">
         <v>31</v>
       </c>
@@ -20460,7 +20460,7 @@
       <c r="AB5" s="89"/>
       <c r="AC5" s="89"/>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" ht="30">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -20521,7 +20521,7 @@
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" ht="30">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -20688,7 +20688,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -21019,17 +21019,17 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="1.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="1.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.578125" style="111"/>
-    <col min="27" max="29" width="23.68359375" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" style="111"/>
+    <col min="27" max="29" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -21190,7 +21190,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="15" customFormat="1" ht="43.2">
+    <row r="3" spans="1:29" s="15" customFormat="1" ht="45">
       <c r="A3" s="65">
         <v>32</v>
       </c>
@@ -21609,7 +21609,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -21945,21 +21945,21 @@
       <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" style="54" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.578125" style="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.68359375" style="54" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.41796875" style="54"/>
-    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="54" customWidth="1"/>
-    <col min="22" max="26" width="11.41796875" style="54"/>
-    <col min="27" max="29" width="23.41796875" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="54"/>
+    <col min="2" max="2" width="11.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="54" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.7109375" style="54" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.42578125" style="54"/>
+    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="54" customWidth="1"/>
+    <col min="22" max="26" width="11.42578125" style="54"/>
+    <col min="27" max="29" width="23.42578125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -22120,7 +22120,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="3" spans="1:50" s="56" customFormat="1" ht="45">
       <c r="A3" s="55">
         <v>33</v>
       </c>
@@ -22575,7 +22575,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -22922,25 +22922,25 @@
       <selection activeCell="AA6" sqref="AA6:AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.41796875" style="80" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83984375" style="15" customWidth="1"/>
-    <col min="3" max="5" width="10.68359375" style="15" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="15" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="15" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.41796875" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.68359375" style="15" customWidth="1"/>
-    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="73" customWidth="1"/>
-    <col min="22" max="22" width="17.15625" style="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.41796875" style="15"/>
-    <col min="24" max="25" width="11.41796875" style="73"/>
-    <col min="26" max="26" width="11.41796875" style="15"/>
-    <col min="27" max="29" width="23.578125" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="15"/>
+    <col min="1" max="1" width="3.42578125" style="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="15" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="15" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="15" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" style="15" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="73" customWidth="1"/>
+    <col min="22" max="22" width="17.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="15"/>
+    <col min="24" max="25" width="11.42578125" style="73"/>
+    <col min="26" max="26" width="11.42578125" style="15"/>
+    <col min="27" max="29" width="23.5703125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -23101,7 +23101,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="28.8">
+    <row r="3" spans="1:50" ht="45">
       <c r="A3" s="55">
         <v>34</v>
       </c>
@@ -23546,7 +23546,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -23903,20 +23903,20 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.15625" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.68359375" style="54" customWidth="1"/>
-    <col min="3" max="5" width="10.68359375" style="54" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="54" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="54" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.41796875" style="54"/>
-    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="11.41796875" style="54"/>
-    <col min="27" max="29" width="23.26171875" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="54"/>
+    <col min="1" max="1" width="3.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="54" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" style="54" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="54" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.42578125" style="54"/>
+    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="11.42578125" style="54"/>
+    <col min="27" max="29" width="23.28515625" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -24077,7 +24077,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="56" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" s="56" customFormat="1" ht="45">
       <c r="A3" s="55">
         <v>35</v>
       </c>
@@ -24516,7 +24516,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -24869,26 +24869,26 @@
   <sheetPr codeName="Hoja19"/>
   <dimension ref="A1:AX14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.68359375" style="54" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="54" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="54" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="54"/>
-    <col min="19" max="19" width="41.41796875" style="54" customWidth="1"/>
-    <col min="20" max="20" width="6.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="54"/>
-    <col min="22" max="22" width="17.15625" style="54" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="11.41796875" style="54"/>
-    <col min="27" max="29" width="23.578125" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="54"/>
+    <col min="1" max="1" width="3.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.7109375" style="54" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="54" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="54"/>
+    <col min="19" max="19" width="41.42578125" style="54" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="54"/>
+    <col min="22" max="22" width="17.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="11.42578125" style="54"/>
+    <col min="27" max="29" width="23.5703125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -25049,7 +25049,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="56" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" s="56" customFormat="1" ht="45">
       <c r="A3" s="55">
         <v>36</v>
       </c>
@@ -25285,7 +25285,7 @@
       <c r="AW5"/>
       <c r="AX5"/>
     </row>
-    <row r="6" spans="1:50" s="56" customFormat="1">
+    <row r="6" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A6" s="55" t="s">
         <v>0</v>
       </c>
@@ -25336,7 +25336,9 @@
       <c r="Z6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AA6" s="159"/>
+      <c r="AA6" s="159" t="s">
+        <v>451</v>
+      </c>
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
       <c r="AD6"/>
@@ -25361,7 +25363,7 @@
       <c r="AW6"/>
       <c r="AX6"/>
     </row>
-    <row r="7" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="7" spans="1:50" s="56" customFormat="1">
       <c r="A7" s="55" t="s">
         <v>0</v>
       </c>
@@ -25410,9 +25412,7 @@
       <c r="Z7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AA7" s="159" t="s">
-        <v>451</v>
-      </c>
+      <c r="AA7" s="159"/>
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
       <c r="AD7"/>
@@ -25486,7 +25486,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -25531,11 +25531,13 @@
       </c>
       <c r="Y9" s="22"/>
       <c r="Z9" s="22"/>
-      <c r="AA9" s="159"/>
+      <c r="AA9" s="159" t="s">
+        <v>452</v>
+      </c>
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:50" s="56" customFormat="1">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -25582,9 +25584,7 @@
       </c>
       <c r="Y10" s="22"/>
       <c r="Z10" s="133"/>
-      <c r="AA10" s="159" t="s">
-        <v>452</v>
-      </c>
+      <c r="AA10" s="159"/>
       <c r="AB10" s="89"/>
       <c r="AC10" s="89"/>
     </row>
@@ -25633,9 +25633,15 @@
       <c r="X11" s="24"/>
       <c r="Y11" s="24"/>
       <c r="Z11" s="24"/>
-      <c r="AA11" s="89"/>
-      <c r="AB11" s="89"/>
-      <c r="AC11" s="89"/>
+      <c r="AA11" s="89" t="s">
+        <v>454</v>
+      </c>
+      <c r="AB11" s="89" t="s">
+        <v>455</v>
+      </c>
+      <c r="AC11" s="89" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="12" spans="1:50" s="56" customFormat="1">
       <c r="A12" s="55" t="s">
@@ -25680,15 +25686,9 @@
       <c r="X12" s="22"/>
       <c r="Y12" s="22"/>
       <c r="Z12" s="22"/>
-      <c r="AA12" s="89" t="s">
-        <v>454</v>
-      </c>
-      <c r="AB12" s="89" t="s">
-        <v>455</v>
-      </c>
-      <c r="AC12" s="89" t="s">
-        <v>453</v>
-      </c>
+      <c r="AA12" s="89"/>
+      <c r="AB12" s="89"/>
+      <c r="AC12" s="89"/>
     </row>
     <row r="13" spans="1:50" s="56" customFormat="1">
       <c r="A13" s="55" t="s">
@@ -25834,26 +25834,26 @@
       <selection activeCell="AA15" sqref="AA15:AA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.68359375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="10.68359375" style="15" customWidth="1"/>
-    <col min="9" max="9" width="2.68359375" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="16" width="3.68359375" style="15" customWidth="1"/>
-    <col min="17" max="17" width="3.68359375" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="10.7109375" style="15" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="16" width="3.7109375" style="15" customWidth="1"/>
+    <col min="17" max="17" width="3.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="15" customWidth="1"/>
     <col min="19" max="19" width="23" style="15" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" style="15" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="73" customWidth="1"/>
-    <col min="22" max="22" width="24.15625" style="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.26171875" style="15" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="15" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="73" customWidth="1"/>
+    <col min="22" max="22" width="24.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" style="15" customWidth="1"/>
     <col min="24" max="24" width="17" style="15" customWidth="1"/>
     <col min="25" max="25" width="22" style="15" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="15"/>
+    <col min="26" max="26" width="11.42578125" style="15"/>
     <col min="27" max="27" width="23" style="15" customWidth="1"/>
-    <col min="28" max="28" width="22.578125" style="15" customWidth="1"/>
+    <col min="28" max="28" width="22.5703125" style="15" customWidth="1"/>
     <col min="29" max="29" width="23" style="15" customWidth="1"/>
-    <col min="30" max="16384" width="11.41796875" style="15"/>
+    <col min="30" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -26014,7 +26014,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="21" customFormat="1" ht="28.8">
+    <row r="3" spans="1:29" s="21" customFormat="1" ht="30">
       <c r="A3" s="58">
         <v>7</v>
       </c>
@@ -29668,23 +29668,23 @@
       <selection activeCell="AA36" sqref="AA36:AA39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.68359375" style="25" customWidth="1"/>
-    <col min="6" max="6" width="2.83984375" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="2.83984375" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="3.83984375" style="25" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9.68359375" style="25" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.7109375" style="25" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="2.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="3.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" style="25" customWidth="1"/>
     <col min="19" max="19" width="37" style="25" customWidth="1"/>
-    <col min="20" max="20" width="8.26171875" style="25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.83984375" style="54" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.41796875" style="87" customWidth="1"/>
-    <col min="23" max="23" width="43.41796875" style="87" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="95.578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.26171875" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="25"/>
-    <col min="27" max="29" width="23.83984375" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="87" customWidth="1"/>
+    <col min="23" max="23" width="43.42578125" style="87" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="95.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.28515625" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="25"/>
+    <col min="27" max="29" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -29845,7 +29845,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="43.2">
+    <row r="3" spans="1:29" ht="60">
       <c r="A3" s="56">
         <v>37</v>
       </c>
@@ -30372,7 +30372,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="12" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -30664,7 +30664,7 @@
       <c r="AB17" s="163"/>
       <c r="AC17" s="163"/>
     </row>
-    <row r="18" spans="1:29" ht="43.2">
+    <row r="18" spans="1:29" ht="60">
       <c r="A18" s="56">
         <v>38</v>
       </c>
@@ -31189,7 +31189,7 @@
       <c r="AB26" s="89"/>
       <c r="AC26" s="89"/>
     </row>
-    <row r="27" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="27" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A27" s="55" t="s">
         <v>0</v>
       </c>
@@ -31481,7 +31481,7 @@
       <c r="AB32" s="163"/>
       <c r="AC32" s="163"/>
     </row>
-    <row r="33" spans="1:29" ht="43.2">
+    <row r="33" spans="1:29" ht="60">
       <c r="A33" s="83">
         <v>39</v>
       </c>
@@ -32008,7 +32008,7 @@
       <c r="AB41" s="89"/>
       <c r="AC41" s="89"/>
     </row>
-    <row r="42" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="42" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A42" s="55" t="s">
         <v>0</v>
       </c>
@@ -32323,18 +32323,18 @@
       <selection activeCell="AA87" sqref="AA87:AB87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.26171875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.68359375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="10" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="11.41796875" style="10"/>
-    <col min="24" max="24" width="13.68359375" style="10" customWidth="1"/>
-    <col min="25" max="25" width="11.83984375" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="10"/>
+    <col min="1" max="1" width="4.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="10" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="11.42578125" style="10"/>
+    <col min="24" max="24" width="13.7109375" style="10" customWidth="1"/>
+    <col min="25" max="25" width="11.85546875" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="10"/>
     <col min="27" max="29" width="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -32496,7 +32496,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="43.2">
+    <row r="3" spans="1:29" ht="45">
       <c r="A3" s="1">
         <v>40</v>
       </c>
@@ -32657,7 +32657,7 @@
       <c r="AB5" s="89"/>
       <c r="AC5" s="89"/>
     </row>
-    <row r="6" spans="1:29" ht="28.8">
+    <row r="6" spans="1:29" ht="30">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -32816,7 +32816,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -33126,7 +33126,7 @@
       <c r="AB14" s="163"/>
       <c r="AC14" s="163"/>
     </row>
-    <row r="15" spans="1:29" ht="43.2">
+    <row r="15" spans="1:29" ht="45">
       <c r="A15" s="1">
         <v>41</v>
       </c>
@@ -33289,7 +33289,7 @@
       <c r="AB17" s="89"/>
       <c r="AC17" s="89"/>
     </row>
-    <row r="18" spans="1:29" ht="28.8">
+    <row r="18" spans="1:29" ht="30">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -33448,7 +33448,7 @@
       <c r="AB20" s="89"/>
       <c r="AC20" s="89"/>
     </row>
-    <row r="21" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="21" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -33766,7 +33766,7 @@
       <c r="AB26" s="163"/>
       <c r="AC26" s="163"/>
     </row>
-    <row r="27" spans="1:29" ht="43.2">
+    <row r="27" spans="1:29" ht="45">
       <c r="A27" s="1">
         <v>42</v>
       </c>
@@ -33931,7 +33931,7 @@
       <c r="AB29" s="89"/>
       <c r="AC29" s="89"/>
     </row>
-    <row r="30" spans="1:29" ht="28.8">
+    <row r="30" spans="1:29" ht="30">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -34090,7 +34090,7 @@
       <c r="AB32" s="89"/>
       <c r="AC32" s="89"/>
     </row>
-    <row r="33" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="33" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A33" s="55" t="s">
         <v>0</v>
       </c>
@@ -34408,7 +34408,7 @@
       <c r="AB38" s="163"/>
       <c r="AC38" s="163"/>
     </row>
-    <row r="39" spans="1:29" ht="43.2">
+    <row r="39" spans="1:29" ht="45">
       <c r="A39" s="1">
         <v>43</v>
       </c>
@@ -34573,7 +34573,7 @@
       <c r="AB41" s="89"/>
       <c r="AC41" s="89"/>
     </row>
-    <row r="42" spans="1:29" ht="28.8">
+    <row r="42" spans="1:29" ht="30">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -34732,7 +34732,7 @@
       <c r="AB44" s="89"/>
       <c r="AC44" s="89"/>
     </row>
-    <row r="45" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="45" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A45" s="55" t="s">
         <v>0</v>
       </c>
@@ -35050,7 +35050,7 @@
       <c r="AB50" s="163"/>
       <c r="AC50" s="163"/>
     </row>
-    <row r="51" spans="1:29" ht="43.2">
+    <row r="51" spans="1:29" ht="45">
       <c r="A51" s="1">
         <v>44</v>
       </c>
@@ -35215,7 +35215,7 @@
       <c r="AB53" s="89"/>
       <c r="AC53" s="89"/>
     </row>
-    <row r="54" spans="1:29" ht="28.8">
+    <row r="54" spans="1:29" ht="30">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -35374,7 +35374,7 @@
       <c r="AB56" s="89"/>
       <c r="AC56" s="89"/>
     </row>
-    <row r="57" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="57" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A57" s="55" t="s">
         <v>0</v>
       </c>
@@ -35692,7 +35692,7 @@
       <c r="AB62" s="163"/>
       <c r="AC62" s="163"/>
     </row>
-    <row r="63" spans="1:29" ht="43.2">
+    <row r="63" spans="1:29" ht="60">
       <c r="A63" s="1">
         <v>45</v>
       </c>
@@ -35857,7 +35857,7 @@
       <c r="AB65" s="89"/>
       <c r="AC65" s="89"/>
     </row>
-    <row r="66" spans="1:29" ht="28.8">
+    <row r="66" spans="1:29" ht="30">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
@@ -36016,7 +36016,7 @@
       <c r="AB68" s="89"/>
       <c r="AC68" s="89"/>
     </row>
-    <row r="69" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="69" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A69" s="55" t="s">
         <v>0</v>
       </c>
@@ -36334,7 +36334,7 @@
       <c r="AB74" s="163"/>
       <c r="AC74" s="163"/>
     </row>
-    <row r="75" spans="1:29" ht="43.2">
+    <row r="75" spans="1:29" ht="60">
       <c r="A75" s="1">
         <v>46</v>
       </c>
@@ -36499,7 +36499,7 @@
       <c r="AB77" s="89"/>
       <c r="AC77" s="89"/>
     </row>
-    <row r="78" spans="1:29" ht="28.8">
+    <row r="78" spans="1:29" ht="30">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -36658,7 +36658,7 @@
       <c r="AB80" s="89"/>
       <c r="AC80" s="89"/>
     </row>
-    <row r="81" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="81" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A81" s="55" t="s">
         <v>0</v>
       </c>
@@ -36976,7 +36976,7 @@
       <c r="AB86" s="199"/>
       <c r="AC86" s="199"/>
     </row>
-    <row r="87" spans="1:29" ht="28.8">
+    <row r="87" spans="1:29" ht="45">
       <c r="A87" s="1">
         <v>47</v>
       </c>
@@ -37141,7 +37141,7 @@
       <c r="AB89" s="89"/>
       <c r="AC89" s="89"/>
     </row>
-    <row r="90" spans="1:29" ht="28.8">
+    <row r="90" spans="1:29" ht="30">
       <c r="A90" s="1" t="s">
         <v>0</v>
       </c>
@@ -37300,7 +37300,7 @@
       <c r="AB92" s="89"/>
       <c r="AC92" s="89"/>
     </row>
-    <row r="93" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="93" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A93" s="55" t="s">
         <v>0</v>
       </c>
@@ -37642,22 +37642,22 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.68359375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="10" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="10" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.83984375" style="10" customWidth="1"/>
-    <col min="20" max="20" width="6.15625" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.41796875" style="10"/>
-    <col min="24" max="25" width="13.83984375" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="10"/>
+    <col min="19" max="19" width="16.85546875" style="10" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11.42578125" style="10"/>
+    <col min="24" max="25" width="13.85546875" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="10"/>
     <col min="27" max="29" width="23" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="10"/>
+    <col min="51" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -37818,7 +37818,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" customFormat="1" ht="45">
       <c r="A3" s="1">
         <v>48</v>
       </c>
@@ -38504,23 +38504,23 @@
       <selection activeCell="AA43" sqref="AA43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="10.26171875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="10" customWidth="1"/>
     <col min="4" max="4" width="10" style="10" customWidth="1"/>
-    <col min="5" max="6" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.68359375" style="10" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.41796875" style="10"/>
-    <col min="20" max="20" width="9.15625" style="10" customWidth="1"/>
-    <col min="21" max="23" width="11.41796875" style="10"/>
-    <col min="24" max="24" width="17.578125" style="10" customWidth="1"/>
+    <col min="5" max="6" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.7109375" style="10" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.42578125" style="10"/>
+    <col min="20" max="20" width="9.140625" style="10" customWidth="1"/>
+    <col min="21" max="23" width="11.42578125" style="10"/>
+    <col min="24" max="24" width="17.5703125" style="10" customWidth="1"/>
     <col min="25" max="25" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="10"/>
-    <col min="27" max="29" width="24.68359375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="10"/>
+    <col min="26" max="26" width="11.42578125" style="10"/>
+    <col min="27" max="29" width="24.7109375" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -38681,7 +38681,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" customFormat="1" ht="43.2">
+    <row r="3" spans="1:29" customFormat="1" ht="45">
       <c r="A3" s="1">
         <v>49</v>
       </c>
@@ -39462,7 +39462,7 @@
       <c r="AB17" s="89"/>
       <c r="AC17" s="89"/>
     </row>
-    <row r="18" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="18" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A18" s="55" t="s">
         <v>0</v>
       </c>
@@ -39791,7 +39791,7 @@
       <c r="AW23"/>
       <c r="AX23"/>
     </row>
-    <row r="24" spans="1:50" customFormat="1" ht="43.2">
+    <row r="24" spans="1:50" customFormat="1" ht="45">
       <c r="A24" s="1">
         <v>50</v>
       </c>
@@ -40572,7 +40572,7 @@
       <c r="AB38" s="89"/>
       <c r="AC38" s="89"/>
     </row>
-    <row r="39" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="39" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A39" s="55" t="s">
         <v>0</v>
       </c>
@@ -40920,19 +40920,19 @@
       <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.68359375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="6.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14" customWidth="1"/>
     <col min="25" max="25" width="14" style="111" customWidth="1"/>
-    <col min="27" max="29" width="23.15625" customWidth="1"/>
+    <col min="27" max="29" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -41093,7 +41093,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="10" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" s="10" customFormat="1" ht="45">
       <c r="A3" s="1">
         <v>51</v>
       </c>
@@ -41531,7 +41531,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -41879,23 +41879,23 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.41796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.83984375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11.15625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="11.83984375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.68359375" style="10" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.41796875" style="10"/>
-    <col min="20" max="20" width="6.15625" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.41796875" style="10"/>
-    <col min="24" max="25" width="9.41796875" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="10"/>
-    <col min="27" max="29" width="23.68359375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="10"/>
+    <col min="1" max="1" width="3.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.7109375" style="10" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.42578125" style="10"/>
+    <col min="20" max="20" width="6.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11.42578125" style="10"/>
+    <col min="24" max="25" width="9.42578125" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="10"/>
+    <col min="27" max="29" width="23.7109375" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -42056,7 +42056,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" customFormat="1" ht="45">
       <c r="A3" s="1">
         <v>52</v>
       </c>
@@ -42388,7 +42388,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -42717,7 +42717,7 @@
       <c r="AW14"/>
       <c r="AX14"/>
     </row>
-    <row r="15" spans="1:50" customFormat="1" ht="43.2">
+    <row r="15" spans="1:50" customFormat="1" ht="45">
       <c r="A15" s="1">
         <v>53</v>
       </c>
@@ -43046,7 +43046,7 @@
       <c r="AB20" s="89"/>
       <c r="AC20" s="89"/>
     </row>
-    <row r="21" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="21" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -43390,22 +43390,22 @@
       <selection activeCell="AB26" sqref="AB26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.41796875" customWidth="1"/>
-    <col min="3" max="3" width="13.26171875" customWidth="1"/>
-    <col min="4" max="4" width="8.15625" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="1.83984375" customWidth="1"/>
-    <col min="9" max="9" width="1.83984375" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" customWidth="1"/>
-    <col min="20" max="20" width="6.15625" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="10.15625" style="10" customWidth="1"/>
-    <col min="27" max="29" width="23.68359375" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="1.85546875" customWidth="1"/>
+    <col min="9" max="9" width="1.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.140625" style="10" customWidth="1"/>
+    <col min="27" max="29" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -43566,7 +43566,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="10" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" s="10" customFormat="1" ht="60">
       <c r="A3" s="1">
         <v>54</v>
       </c>
@@ -43888,7 +43888,7 @@
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
     </row>
-    <row r="8" spans="1:50" ht="43.2">
+    <row r="8" spans="1:50" ht="45">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -44096,7 +44096,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="12" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -44425,7 +44425,7 @@
       <c r="AW17"/>
       <c r="AX17"/>
     </row>
-    <row r="18" spans="1:50" s="10" customFormat="1" ht="43.2">
+    <row r="18" spans="1:50" s="10" customFormat="1" ht="60">
       <c r="A18" s="1">
         <v>55</v>
       </c>
@@ -44745,7 +44745,7 @@
       <c r="AB22" s="89"/>
       <c r="AC22" s="89"/>
     </row>
-    <row r="23" spans="1:50" ht="43.2">
+    <row r="23" spans="1:50" ht="45">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -44951,7 +44951,7 @@
       <c r="AB26" s="89"/>
       <c r="AC26" s="89"/>
     </row>
-    <row r="27" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="27" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A27" s="55" t="s">
         <v>0</v>
       </c>
@@ -45280,7 +45280,7 @@
       <c r="AW32"/>
       <c r="AX32"/>
     </row>
-    <row r="33" spans="1:50" s="10" customFormat="1" ht="43.2">
+    <row r="33" spans="1:50" s="10" customFormat="1" ht="60">
       <c r="A33" s="1">
         <v>56</v>
       </c>
@@ -45602,7 +45602,7 @@
       <c r="AB37" s="89"/>
       <c r="AC37" s="89"/>
     </row>
-    <row r="38" spans="1:50" ht="43.2">
+    <row r="38" spans="1:50" ht="45">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -45810,7 +45810,7 @@
       <c r="AB41" s="89"/>
       <c r="AC41" s="89"/>
     </row>
-    <row r="42" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="42" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A42" s="55" t="s">
         <v>0</v>
       </c>
@@ -46163,24 +46163,24 @@
       <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.41796875" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.26171875" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.15625" style="39" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
-    <col min="19" max="23" width="11.41796875" style="39"/>
-    <col min="24" max="24" width="46.26171875" style="97" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
+    <col min="19" max="23" width="11.42578125" style="39"/>
+    <col min="24" max="24" width="46.28515625" style="97" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="39"/>
-    <col min="27" max="29" width="24.41796875" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="39"/>
+    <col min="26" max="26" width="11.42578125" style="39"/>
+    <col min="27" max="29" width="24.42578125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -46341,7 +46341,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="97" customFormat="1">
+    <row r="3" spans="1:50" s="97" customFormat="1" ht="30">
       <c r="A3" s="29">
         <v>57</v>
       </c>
@@ -46962,7 +46962,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="12" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -47806,27 +47806,27 @@
       <selection activeCell="AA21" sqref="AA21:AC21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.41796875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="13.26171875" style="38" customWidth="1"/>
-    <col min="4" max="4" width="8.15625" style="38" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="38" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="38" customWidth="1"/>
     <col min="5" max="5" width="10" style="38" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="38" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="38" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="38" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="38" customWidth="1"/>
-    <col min="19" max="19" width="49.578125" style="38" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" style="38"/>
-    <col min="21" max="21" width="11.41796875" style="97"/>
-    <col min="22" max="22" width="11.41796875" style="38"/>
-    <col min="23" max="23" width="36.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="11.68359375" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="38"/>
-    <col min="27" max="29" width="23.15625" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="38"/>
+    <col min="6" max="6" width="1.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="38" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="38" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="38" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="38" customWidth="1"/>
+    <col min="19" max="19" width="49.5703125" style="38" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="38"/>
+    <col min="21" max="21" width="11.42578125" style="97"/>
+    <col min="22" max="22" width="11.42578125" style="38"/>
+    <col min="23" max="23" width="36.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="38"/>
+    <col min="27" max="29" width="23.140625" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -49024,7 +49024,7 @@
       <c r="AB18" s="89"/>
       <c r="AC18" s="89"/>
     </row>
-    <row r="19" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="19" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A19" s="55" t="s">
         <v>0</v>
       </c>
@@ -49990,26 +49990,26 @@
       <selection activeCell="AA13" sqref="AA13:AC15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.41796875" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.26171875" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.15625" style="39" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.41796875" style="39"/>
-    <col min="21" max="21" width="11.41796875" style="97"/>
-    <col min="22" max="23" width="11.41796875" style="39"/>
+    <col min="6" max="6" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" style="39"/>
+    <col min="21" max="21" width="11.42578125" style="97"/>
+    <col min="22" max="23" width="11.42578125" style="39"/>
     <col min="24" max="24" width="23" style="97" customWidth="1"/>
-    <col min="25" max="25" width="13.41796875" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="39"/>
-    <col min="27" max="29" width="23.83984375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="39"/>
+    <col min="25" max="25" width="13.42578125" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="39"/>
+    <col min="27" max="29" width="23.85546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -50170,7 +50170,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="97" customFormat="1" ht="28.8">
+    <row r="3" spans="1:50" s="97" customFormat="1" ht="30">
       <c r="A3" s="29">
         <v>59</v>
       </c>
@@ -50468,7 +50468,7 @@
       <c r="AW6"/>
       <c r="AX6"/>
     </row>
-    <row r="7" spans="1:50" s="97" customFormat="1">
+    <row r="7" spans="1:50" s="97" customFormat="1" ht="30">
       <c r="A7" s="29"/>
       <c r="B7" s="28"/>
       <c r="C7" s="34"/>
@@ -50536,7 +50536,7 @@
       <c r="AW7"/>
       <c r="AX7"/>
     </row>
-    <row r="8" spans="1:50" s="97" customFormat="1">
+    <row r="8" spans="1:50" s="97" customFormat="1" ht="30">
       <c r="A8" s="29" t="s">
         <v>0</v>
       </c>
@@ -50610,7 +50610,7 @@
       <c r="AW8"/>
       <c r="AX8"/>
     </row>
-    <row r="9" spans="1:50" s="97" customFormat="1" ht="28.8">
+    <row r="9" spans="1:50" s="97" customFormat="1" ht="30">
       <c r="A9" s="29"/>
       <c r="B9" s="28"/>
       <c r="C9" s="34"/>
@@ -50853,7 +50853,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="13" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -51817,29 +51817,29 @@
       <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.26171875" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.68359375" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.68359375" style="25" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="25" customWidth="1"/>
     <col min="4" max="4" width="6" style="25" customWidth="1"/>
-    <col min="5" max="5" width="5.83984375" style="25" customWidth="1"/>
-    <col min="6" max="7" width="8.68359375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="2.578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.578125" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="3.578125" style="25" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="3.578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.41796875" style="25"/>
-    <col min="20" max="20" width="11.41796875" style="25" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="54" customWidth="1"/>
-    <col min="22" max="22" width="11.41796875" style="25"/>
-    <col min="23" max="23" width="36.26171875" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="47.68359375" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.83984375" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="25"/>
-    <col min="27" max="27" width="22.83984375" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" style="25" customWidth="1"/>
+    <col min="6" max="7" width="8.7109375" style="25" customWidth="1"/>
+    <col min="8" max="8" width="2.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5703125" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="3.5703125" style="25" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="3.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.42578125" style="25"/>
+    <col min="20" max="20" width="11.42578125" style="25" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="54" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" style="25"/>
+    <col min="23" max="23" width="36.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="47.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="25"/>
+    <col min="27" max="27" width="22.85546875" customWidth="1"/>
     <col min="28" max="29" width="23" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="25"/>
+    <col min="51" max="16384" width="11.42578125" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="71" customFormat="1">
@@ -56715,20 +56715,20 @@
       <selection activeCell="AA7" sqref="AA7:AB9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.68359375" customWidth="1"/>
-    <col min="25" max="25" width="13.68359375" style="111" customWidth="1"/>
-    <col min="27" max="29" width="23.68359375" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.7109375" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" style="111" customWidth="1"/>
+    <col min="27" max="29" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -57349,7 +57349,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="13" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -58090,25 +58090,25 @@
       <selection activeCell="AA7" sqref="AA7:AB9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.41796875" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.26171875" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.15625" style="39" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.41796875" style="39"/>
-    <col min="21" max="21" width="11.41796875" style="97"/>
-    <col min="22" max="23" width="11.41796875" style="39"/>
-    <col min="24" max="25" width="11.41796875" style="97"/>
-    <col min="26" max="26" width="11.41796875" style="39"/>
-    <col min="27" max="29" width="23.83984375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="39"/>
+    <col min="6" max="6" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" style="39"/>
+    <col min="21" max="21" width="11.42578125" style="97"/>
+    <col min="22" max="23" width="11.42578125" style="39"/>
+    <col min="24" max="25" width="11.42578125" style="97"/>
+    <col min="26" max="26" width="11.42578125" style="39"/>
+    <col min="27" max="29" width="23.85546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -58918,7 +58918,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="13" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -59266,24 +59266,24 @@
       <selection activeCell="AA1" sqref="AA1:AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.68359375" style="39" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.41796875" style="39"/>
-    <col min="21" max="21" width="11.41796875" style="97"/>
-    <col min="22" max="22" width="12.83984375" style="39" customWidth="1"/>
-    <col min="23" max="23" width="11.41796875" style="39"/>
-    <col min="24" max="24" width="12.83984375" style="97" customWidth="1"/>
-    <col min="25" max="25" width="12.15625" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="39"/>
-    <col min="27" max="29" width="23.578125" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="39"/>
+    <col min="2" max="4" width="10.7109375" style="39" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" style="39"/>
+    <col min="21" max="21" width="11.42578125" style="97"/>
+    <col min="22" max="22" width="12.85546875" style="39" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="39"/>
+    <col min="24" max="24" width="12.85546875" style="97" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="39"/>
+    <col min="27" max="29" width="23.5703125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -60368,13 +60368,13 @@
       <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.41796875" style="111"/>
-    <col min="26" max="26" width="11.26171875" customWidth="1"/>
-    <col min="27" max="29" width="22.578125" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" style="111"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+    <col min="27" max="29" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -61468,13 +61468,13 @@
       <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.68359375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="15.83984375" customWidth="1"/>
-    <col min="20" max="20" width="15.26171875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.41796875" style="111"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" style="111"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -61983,23 +61983,23 @@
       <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.41796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.68359375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" style="7" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="7" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="11.41796875" style="7"/>
-    <col min="21" max="21" width="11.41796875" style="69"/>
-    <col min="22" max="22" width="11.41796875" style="7"/>
-    <col min="23" max="23" width="37.26171875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="54.578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.41796875" style="7" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="7"/>
-    <col min="27" max="29" width="22.83984375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="7"/>
+    <col min="1" max="1" width="3.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="7" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="11.42578125" style="7"/>
+    <col min="21" max="21" width="11.42578125" style="69"/>
+    <col min="22" max="22" width="11.42578125" style="7"/>
+    <col min="23" max="23" width="37.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="54.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" style="7" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="7"/>
+    <col min="27" max="29" width="22.85546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -68004,19 +68004,19 @@
       <selection activeCell="AA24" sqref="AA24:AB24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.68359375" customWidth="1"/>
-    <col min="7" max="7" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="1.83984375" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" customWidth="1"/>
-    <col min="21" max="21" width="11.41796875" style="10" customWidth="1"/>
-    <col min="23" max="23" width="35.83984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.41796875" style="111"/>
-    <col min="27" max="29" width="22.83984375" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="1.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="10" customWidth="1"/>
+    <col min="23" max="23" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" style="111"/>
+    <col min="27" max="29" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -71101,22 +71101,22 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.26171875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.68359375" customWidth="1"/>
-    <col min="6" max="6" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.83984375" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.41796875" customWidth="1"/>
-    <col min="24" max="24" width="8.15625" customWidth="1"/>
-    <col min="25" max="25" width="8.15625" style="111" customWidth="1"/>
-    <col min="27" max="29" width="22.68359375" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="111" customWidth="1"/>
+    <col min="27" max="29" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -73344,21 +73344,21 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.26171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.68359375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="1.83984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.83984375" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="11.41796875" style="2"/>
-    <col min="23" max="23" width="35.83984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.41796875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="10.41796875" style="113" customWidth="1"/>
-    <col min="26" max="26" width="11.41796875" style="2"/>
-    <col min="27" max="29" width="22.83984375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="2"/>
+    <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="11.42578125" style="2"/>
+    <col min="23" max="23" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" style="113" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="2"/>
+    <col min="27" max="29" width="22.85546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -74769,16 +74769,16 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.68359375" style="38" customWidth="1"/>
-    <col min="5" max="5" width="1.83984375" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.83984375" style="38" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="38" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="38" bestFit="1" customWidth="1"/>
-    <col min="18" max="26" width="11.41796875" style="38"/>
-    <col min="27" max="29" width="22.83984375" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.7109375" style="38" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="38" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="38" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="18" max="26" width="11.42578125" style="38"/>
+    <col min="27" max="29" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -75619,20 +75619,20 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.83984375" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.68359375" style="56" customWidth="1"/>
-    <col min="7" max="7" width="1.83984375" style="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="1.83984375" style="56" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.68359375" style="56" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.68359375" style="56" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.41796875" style="56"/>
-    <col min="19" max="19" width="30.26171875" style="56" customWidth="1"/>
-    <col min="20" max="21" width="11.41796875" style="56" customWidth="1"/>
-    <col min="22" max="26" width="11.41796875" style="56"/>
-    <col min="27" max="29" width="22.83984375" customWidth="1"/>
-    <col min="51" max="16384" width="11.41796875" style="56"/>
+    <col min="1" max="1" width="3.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" style="56" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="1.85546875" style="56" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="56" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="56" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="56"/>
+    <col min="19" max="19" width="30.28515625" style="56" customWidth="1"/>
+    <col min="20" max="21" width="11.42578125" style="56" customWidth="1"/>
+    <col min="22" max="26" width="11.42578125" style="56"/>
+    <col min="27" max="29" width="22.85546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -76077,7 +76077,7 @@
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
     </row>
-    <row r="8" spans="1:50" ht="28.8">
+    <row r="8" spans="1:50" ht="30">
       <c r="B8" s="45" t="s">
         <v>0</v>
       </c>
@@ -76185,7 +76185,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="130" customFormat="1" ht="28.8">
+    <row r="10" spans="1:50" s="130" customFormat="1" ht="30">
       <c r="B10" s="45" t="s">
         <v>0</v>
       </c>
@@ -76300,7 +76300,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" ht="28.8">
+    <row r="12" spans="1:50" ht="30">
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
@@ -76590,7 +76590,7 @@
       <c r="AW17" s="56"/>
       <c r="AX17" s="56"/>
     </row>
-    <row r="18" spans="1:50" ht="28.8">
+    <row r="18" spans="1:50" ht="30">
       <c r="A18" s="55" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
-Part IV should be properly displayed in the PDF document v210 regulated (alpha criterion/selection criteria).
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria\IdeaProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NetbeansProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F8D8A3-4EF3-4D03-9A24-F8FD9BB387E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B3D435-42E9-45D4-AC2C-591A126859FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="588" firstSheet="30" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8580" yWindow="135" windowWidth="29205" windowHeight="15435" tabRatio="588" firstSheet="29" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -2377,7 +2377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -2548,6 +2548,148 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2663,7 +2805,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="242">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3195,6 +3337,25 @@
     <xf numFmtId="0" fontId="24" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="112">
     <cellStyle name="20 % - Akzent1 2" xfId="54" xr:uid="{58EA2EC2-B9C9-47AD-9424-4145847963D4}"/>
@@ -3203,42 +3364,36 @@
     <cellStyle name="20 % - Akzent4 2" xfId="57" xr:uid="{0CED6BA4-60EF-4640-ACAC-5491EFAA41B6}"/>
     <cellStyle name="20 % - Akzent5 2" xfId="58" xr:uid="{9711E678-D35B-4FDE-A1A2-62A8AD2BA356}"/>
     <cellStyle name="20 % - Akzent6 2" xfId="59" xr:uid="{7CA7835D-FCB7-402D-AC01-33C1572D9E8D}"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση6" xfId="39" builtinId="50" customBuiltin="1"/>
     <cellStyle name="40 % - Akzent1 2" xfId="60" xr:uid="{F156E56A-1EB1-4208-BC29-CF6B998EA7A3}"/>
     <cellStyle name="40 % - Akzent2 2" xfId="61" xr:uid="{278057DE-C374-4BCB-BFCD-8FC15D932AF8}"/>
     <cellStyle name="40 % - Akzent3 2" xfId="62" xr:uid="{A54EAA7B-E320-4400-9E82-FA6F6AEFE3AC}"/>
     <cellStyle name="40 % - Akzent4 2" xfId="63" xr:uid="{CC5AD9F6-BA87-4F3F-A56B-CDCDACABDA15}"/>
     <cellStyle name="40 % - Akzent5 2" xfId="64" xr:uid="{207787DD-36B8-45D1-8027-AE3F706CF8B6}"/>
     <cellStyle name="40 % - Akzent6 2" xfId="65" xr:uid="{17547E8C-9F29-4A3C-9ED2-715309027EBC}"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση6" xfId="40" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent1 2" xfId="66" xr:uid="{40B95E25-5021-4D50-BD78-EF739646E98A}"/>
     <cellStyle name="60 % - Akzent2 2" xfId="67" xr:uid="{6E273BEA-D51E-4B50-8CF4-C2833969CE90}"/>
     <cellStyle name="60 % - Akzent3 2" xfId="68" xr:uid="{D51BC707-3D8B-4DDD-AE79-8DC5AB0B42C5}"/>
     <cellStyle name="60 % - Akzent4 2" xfId="69" xr:uid="{4A56C24B-3685-4CD1-A574-E40817E12F78}"/>
     <cellStyle name="60 % - Akzent5 2" xfId="70" xr:uid="{CCE7CC06-0A99-4475-96EE-A84CB6F4A3A5}"/>
     <cellStyle name="60 % - Akzent6 2" xfId="71" xr:uid="{3289F5EB-86A3-4274-AFFF-FD4F68731930}"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Akzent1 2" xfId="72" xr:uid="{5D4AEBF1-0A7C-4BFB-B180-EAF44EA9B0A0}"/>
     <cellStyle name="Akzent2 2" xfId="73" xr:uid="{85CC1BEF-51DC-4570-B4A5-B17C34C9B97A}"/>
     <cellStyle name="Akzent3 2" xfId="74" xr:uid="{B9E858DA-8B8C-4D0C-B338-C45F23F9086A}"/>
@@ -3246,35 +3401,20 @@
     <cellStyle name="Akzent5 2" xfId="76" xr:uid="{CF7F8E61-0EB1-4992-B9F6-7E1DE473F1D5}"/>
     <cellStyle name="Akzent6 2" xfId="77" xr:uid="{CF8B57BC-427C-49FA-B00F-9FDC4AE226A3}"/>
     <cellStyle name="Ausgabe 2" xfId="78" xr:uid="{A0801910-C56D-41DB-AA5B-D7B9CEA5154B}"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Berechnung 2" xfId="79" xr:uid="{41BDA43A-1ABB-4CE8-B9C1-27E91F26BF6C}"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Eingabe 2" xfId="80" xr:uid="{4E63FB11-C380-4C78-9E5D-ECEC7E1F665D}"/>
     <cellStyle name="Ergebnis 2" xfId="81" xr:uid="{DD805113-7B66-4F6A-AC81-26589BA0D384}"/>
     <cellStyle name="Erklärender Text 2" xfId="82" xr:uid="{A194B96E-6874-44FD-B943-01939BDA0BD2}"/>
     <cellStyle name="Erklärender Text 3" xfId="44" xr:uid="{3688BAA7-06B9-4333-8C0D-984DFDD1B2A1}"/>
     <cellStyle name="Excel Built-in Normal" xfId="50" xr:uid="{56DB3A1F-9D76-48AF-827F-04CDE3DA5590}"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Gut 2" xfId="83" xr:uid="{36A99347-B94D-4690-83AC-8C6CBD65002F}"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hipervínculo" xfId="42" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
     <cellStyle name="Hipervínculo visitado" xfId="103" xr:uid="{9051DEEC-FC84-4591-A8B5-638DE46C05EC}"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Link 2" xfId="46" xr:uid="{74412CD5-81A4-4040-B22F-ED1B046355CD}"/>
     <cellStyle name="Link 2 2" xfId="51" xr:uid="{D14BD33F-0DCB-4F85-85A5-9BB7DDF8AB8C}"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Neutral 2" xfId="84" xr:uid="{1AD55C52-8BBF-476B-B40D-9E1715BBCCDF}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="96" xr:uid="{A0210B32-A716-4DA1-8921-79BD6474A84A}"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Notiz 2" xfId="85" xr:uid="{96F7E845-1C7B-4930-A81D-0C72B5CBD2E5}"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Schlecht 2" xfId="86" xr:uid="{4CC925FC-A91B-432E-96A0-54E0F7C70564}"/>
     <cellStyle name="Standard 2" xfId="45" xr:uid="{4E059FDF-05CD-4388-BF86-76C2B6B0C261}"/>
     <cellStyle name="Standard 2 2" xfId="47" xr:uid="{E963BC3A-6088-4583-83FD-9423FD1ED1E0}"/>
@@ -3298,8 +3438,6 @@
     <cellStyle name="Standard 7" xfId="102" xr:uid="{744AB2FD-CA4D-461B-ABDD-66032D974148}"/>
     <cellStyle name="Standard 7 2" xfId="111" xr:uid="{E5E883CA-4D25-4EE5-AF23-D5DFF53989E9}"/>
     <cellStyle name="Style 1" xfId="52" xr:uid="{DF55E41B-F785-4866-85CE-BBB64E7F0959}"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Überschrift 1 2" xfId="87" xr:uid="{22C91833-F9B6-4CA7-8F5F-BC0057EEF790}"/>
     <cellStyle name="Überschrift 2 2" xfId="88" xr:uid="{CEF7EE81-7675-40F5-B163-07B4049BC735}"/>
     <cellStyle name="Überschrift 3 2" xfId="89" xr:uid="{31D47085-7A55-424D-9C36-8209503C4B54}"/>
@@ -3307,8 +3445,31 @@
     <cellStyle name="Überschrift 5" xfId="91" xr:uid="{77E8198C-A64B-454E-9437-C7F654B906EC}"/>
     <cellStyle name="Verknüpfte Zelle 2" xfId="92" xr:uid="{75D6E79A-C9C3-4688-BF38-48D65D7888B4}"/>
     <cellStyle name="Warnender Text 2" xfId="93" xr:uid="{B95B2F27-4BD2-47FB-BFB4-0373AACBC00D}"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen 2" xfId="94" xr:uid="{CC6AF966-5680-457A-B96D-078ED43C1691}"/>
+    <cellStyle name="Εισαγωγή" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Έλεγχος κελιού" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Έμφαση1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Έμφαση2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Έμφαση3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Έμφαση4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Έμφαση5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Έμφαση6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Έξοδος" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Επεξηγηματικό κείμενο" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Κακό" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Καλό" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Ουδέτερο" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Προειδοποιητικό κείμενο" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Σημείωση" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Συνδεδεμένο κελί" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Σύνολο" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Τίτλος" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Υπολογισμός" xfId="11" builtinId="22" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -5375,7 +5536,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5702,23 +5863,23 @@
       <selection activeCell="AA123" sqref="AA123:AB123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.6640625" style="25" customWidth="1"/>
-    <col min="8" max="8" width="2.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.88671875" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="3.88671875" style="25" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="3.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="17.109375" style="25" customWidth="1"/>
-    <col min="21" max="21" width="13.88671875" style="54" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="17.109375" style="87" customWidth="1"/>
-    <col min="24" max="25" width="17.109375" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.7109375" style="25" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="3.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="17.140625" style="25" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="17.140625" style="87" customWidth="1"/>
+    <col min="24" max="25" width="17.140625" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="25" customWidth="1"/>
     <col min="27" max="27" width="24" style="25" customWidth="1"/>
-    <col min="28" max="28" width="22.6640625" style="25" customWidth="1"/>
-    <col min="29" max="29" width="22.88671875" style="25" customWidth="1"/>
-    <col min="30" max="16384" width="11.44140625" style="25"/>
+    <col min="28" max="28" width="22.7109375" style="25" customWidth="1"/>
+    <col min="29" max="29" width="22.85546875" style="25" customWidth="1"/>
+    <col min="30" max="16384" width="11.42578125" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -5879,7 +6040,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="28.8">
+    <row r="3" spans="1:29" ht="30">
       <c r="A3" s="55">
         <v>1</v>
       </c>
@@ -6164,7 +6325,7 @@
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
     </row>
-    <row r="8" spans="1:29" s="56" customFormat="1">
+    <row r="8" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A8" s="55" t="s">
         <v>0</v>
       </c>
@@ -6335,7 +6496,7 @@
       <c r="AB10" s="89"/>
       <c r="AC10" s="89"/>
     </row>
-    <row r="11" spans="1:29" s="56" customFormat="1" ht="27">
+    <row r="11" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A11" s="55" t="s">
         <v>0</v>
       </c>
@@ -6447,7 +6608,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="13" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -6563,7 +6724,7 @@
       <c r="AB14" s="89"/>
       <c r="AC14" s="89"/>
     </row>
-    <row r="15" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="15" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A15" s="55" t="s">
         <v>0</v>
       </c>
@@ -6897,7 +7058,7 @@
       <c r="AB20" s="89"/>
       <c r="AC20" s="89"/>
     </row>
-    <row r="21" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="21" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -7215,7 +7376,7 @@
       <c r="AB26" s="163"/>
       <c r="AC26" s="163"/>
     </row>
-    <row r="27" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="27" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A27" s="55">
         <v>2</v>
       </c>
@@ -7494,7 +7655,7 @@
       <c r="AB31" s="89"/>
       <c r="AC31" s="89"/>
     </row>
-    <row r="32" spans="1:29" s="56" customFormat="1">
+    <row r="32" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A32" s="55" t="s">
         <v>0</v>
       </c>
@@ -7665,7 +7826,7 @@
       <c r="AB34" s="89"/>
       <c r="AC34" s="89"/>
     </row>
-    <row r="35" spans="1:29" s="56" customFormat="1" ht="27">
+    <row r="35" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A35" s="55" t="s">
         <v>0</v>
       </c>
@@ -7777,7 +7938,7 @@
       <c r="AB36" s="89"/>
       <c r="AC36" s="89"/>
     </row>
-    <row r="37" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="37" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A37" s="55" t="s">
         <v>0</v>
       </c>
@@ -7893,7 +8054,7 @@
       <c r="AB38" s="89"/>
       <c r="AC38" s="89"/>
     </row>
-    <row r="39" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="39" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A39" s="55" t="s">
         <v>0</v>
       </c>
@@ -8227,7 +8388,7 @@
       <c r="AB44" s="89"/>
       <c r="AC44" s="89"/>
     </row>
-    <row r="45" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="45" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A45" s="55" t="s">
         <v>0</v>
       </c>
@@ -8834,7 +8995,7 @@
       <c r="AB55" s="89"/>
       <c r="AC55" s="89"/>
     </row>
-    <row r="56" spans="1:29" s="56" customFormat="1">
+    <row r="56" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A56" s="55" t="s">
         <v>0</v>
       </c>
@@ -9005,7 +9166,7 @@
       <c r="AB58" s="89"/>
       <c r="AC58" s="89"/>
     </row>
-    <row r="59" spans="1:29" s="56" customFormat="1" ht="27">
+    <row r="59" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A59" s="55" t="s">
         <v>0</v>
       </c>
@@ -9117,7 +9278,7 @@
       <c r="AB60" s="89"/>
       <c r="AC60" s="89"/>
     </row>
-    <row r="61" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="61" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A61" s="55" t="s">
         <v>0</v>
       </c>
@@ -9233,7 +9394,7 @@
       <c r="AB62" s="89"/>
       <c r="AC62" s="89"/>
     </row>
-    <row r="63" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="63" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A63" s="55" t="s">
         <v>0</v>
       </c>
@@ -9567,7 +9728,7 @@
       <c r="AB68" s="89"/>
       <c r="AC68" s="89"/>
     </row>
-    <row r="69" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="69" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A69" s="55" t="s">
         <v>0</v>
       </c>
@@ -9885,7 +10046,7 @@
       <c r="AB74" s="163"/>
       <c r="AC74" s="163"/>
     </row>
-    <row r="75" spans="1:29" s="56" customFormat="1">
+    <row r="75" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A75" s="55">
         <v>4</v>
       </c>
@@ -10174,7 +10335,7 @@
       <c r="AB79" s="89"/>
       <c r="AC79" s="89"/>
     </row>
-    <row r="80" spans="1:29" s="56" customFormat="1">
+    <row r="80" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A80" s="55" t="s">
         <v>0</v>
       </c>
@@ -10345,7 +10506,7 @@
       <c r="AB82" s="89"/>
       <c r="AC82" s="89"/>
     </row>
-    <row r="83" spans="1:29" s="56" customFormat="1" ht="27">
+    <row r="83" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A83" s="55" t="s">
         <v>0</v>
       </c>
@@ -10457,7 +10618,7 @@
       <c r="AB84" s="89"/>
       <c r="AC84" s="89"/>
     </row>
-    <row r="85" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="85" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A85" s="55" t="s">
         <v>0</v>
       </c>
@@ -10573,7 +10734,7 @@
       <c r="AB86" s="89"/>
       <c r="AC86" s="89"/>
     </row>
-    <row r="87" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="87" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A87" s="55" t="s">
         <v>0</v>
       </c>
@@ -10907,7 +11068,7 @@
       <c r="AB92" s="89"/>
       <c r="AC92" s="89"/>
     </row>
-    <row r="93" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="93" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A93" s="55" t="s">
         <v>0</v>
       </c>
@@ -11225,7 +11386,7 @@
       <c r="AB98" s="163"/>
       <c r="AC98" s="163"/>
     </row>
-    <row r="99" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="99" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A99" s="55">
         <v>5</v>
       </c>
@@ -11514,7 +11675,7 @@
       <c r="AB103" s="89"/>
       <c r="AC103" s="89"/>
     </row>
-    <row r="104" spans="1:29" s="56" customFormat="1">
+    <row r="104" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A104" s="55" t="s">
         <v>0</v>
       </c>
@@ -11685,7 +11846,7 @@
       <c r="AB106" s="89"/>
       <c r="AC106" s="89"/>
     </row>
-    <row r="107" spans="1:29" s="56" customFormat="1" ht="27">
+    <row r="107" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A107" s="55" t="s">
         <v>0</v>
       </c>
@@ -11797,7 +11958,7 @@
       <c r="AB108" s="89"/>
       <c r="AC108" s="89"/>
     </row>
-    <row r="109" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="109" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A109" s="55" t="s">
         <v>0</v>
       </c>
@@ -11913,7 +12074,7 @@
       <c r="AB110" s="89"/>
       <c r="AC110" s="89"/>
     </row>
-    <row r="111" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="111" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A111" s="55" t="s">
         <v>0</v>
       </c>
@@ -12247,7 +12408,7 @@
       <c r="AB116" s="89"/>
       <c r="AC116" s="89"/>
     </row>
-    <row r="117" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="117" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A117" s="55" t="s">
         <v>0</v>
       </c>
@@ -12565,7 +12726,7 @@
       <c r="AB122" s="163"/>
       <c r="AC122" s="163"/>
     </row>
-    <row r="123" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="123" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A123" s="55">
         <v>6</v>
       </c>
@@ -12852,7 +13013,7 @@
       <c r="AB127" s="89"/>
       <c r="AC127" s="89"/>
     </row>
-    <row r="128" spans="1:29" s="56" customFormat="1">
+    <row r="128" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A128" s="55" t="s">
         <v>0</v>
       </c>
@@ -13023,7 +13184,7 @@
       <c r="AB130" s="89"/>
       <c r="AC130" s="89"/>
     </row>
-    <row r="131" spans="1:29" s="56" customFormat="1" ht="27">
+    <row r="131" spans="1:29" s="56" customFormat="1" ht="26.25">
       <c r="A131" s="55" t="s">
         <v>0</v>
       </c>
@@ -13135,7 +13296,7 @@
       <c r="AB132" s="89"/>
       <c r="AC132" s="89"/>
     </row>
-    <row r="133" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="133" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A133" s="55" t="s">
         <v>0</v>
       </c>
@@ -13251,7 +13412,7 @@
       <c r="AB134" s="89"/>
       <c r="AC134" s="89"/>
     </row>
-    <row r="135" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="135" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A135" s="55" t="s">
         <v>0</v>
       </c>
@@ -13585,7 +13746,7 @@
       <c r="AB140" s="89"/>
       <c r="AC140" s="89"/>
     </row>
-    <row r="141" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="141" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A141" s="55" t="s">
         <v>0</v>
       </c>
@@ -13926,24 +14087,24 @@
       <selection activeCell="AA15" sqref="AA15:AB15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="2" customWidth="1"/>
-    <col min="3" max="5" width="10.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="12.6640625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="2" customWidth="1"/>
     <col min="21" max="21" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="24" width="11.44140625" style="2"/>
-    <col min="25" max="25" width="11.44140625" style="113"/>
-    <col min="26" max="26" width="11.44140625" style="2"/>
-    <col min="27" max="29" width="23.109375" style="2" customWidth="1"/>
-    <col min="30" max="16384" width="11.44140625" style="2"/>
+    <col min="22" max="24" width="11.42578125" style="2"/>
+    <col min="25" max="25" width="11.42578125" style="113"/>
+    <col min="26" max="26" width="11.42578125" style="2"/>
+    <col min="27" max="29" width="23.140625" style="2" customWidth="1"/>
+    <col min="30" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" s="142" customFormat="1">
@@ -14124,7 +14285,7 @@
       <c r="AV2" s="203"/>
       <c r="AW2" s="203"/>
     </row>
-    <row r="3" spans="1:55" customFormat="1" ht="43.2">
+    <row r="3" spans="1:55" customFormat="1" ht="60">
       <c r="A3" s="29">
         <v>25</v>
       </c>
@@ -14606,7 +14767,7 @@
       <c r="BB8" s="202"/>
       <c r="BC8" s="202"/>
     </row>
-    <row r="9" spans="1:55" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:55" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -15078,7 +15239,7 @@
       <c r="BB14" s="202"/>
       <c r="BC14" s="202"/>
     </row>
-    <row r="15" spans="1:55" customFormat="1" ht="43.2">
+    <row r="15" spans="1:55" customFormat="1" ht="45">
       <c r="A15" s="29">
         <v>26</v>
       </c>
@@ -15532,7 +15693,7 @@
       <c r="AV20" s="202"/>
       <c r="AW20" s="202"/>
     </row>
-    <row r="21" spans="1:49" s="56" customFormat="1" ht="28.8">
+    <row r="21" spans="1:49" s="56" customFormat="1" ht="30">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -16272,13 +16433,13 @@
       <selection activeCell="AB18" sqref="AA18:AB18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5546875" style="111"/>
-    <col min="27" max="29" width="23.5546875" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" style="111"/>
+    <col min="27" max="29" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -16439,7 +16600,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="43.2">
+    <row r="3" spans="1:50" ht="45">
       <c r="A3" s="29">
         <v>27</v>
       </c>
@@ -16731,7 +16892,7 @@
       <c r="AW7"/>
       <c r="AX7"/>
     </row>
-    <row r="8" spans="1:50" s="111" customFormat="1" ht="28.8">
+    <row r="8" spans="1:50" s="111" customFormat="1" ht="30">
       <c r="A8" s="29"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
@@ -16985,7 +17146,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="12" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -17303,7 +17464,7 @@
       <c r="AB17" s="163"/>
       <c r="AC17" s="163"/>
     </row>
-    <row r="18" spans="1:50" ht="43.2">
+    <row r="18" spans="1:50" ht="45">
       <c r="A18" s="29">
         <v>28</v>
       </c>
@@ -17656,7 +17817,7 @@
       <c r="AW22"/>
       <c r="AX22"/>
     </row>
-    <row r="23" spans="1:50" s="111" customFormat="1" ht="28.8">
+    <row r="23" spans="1:50" s="111" customFormat="1" ht="30">
       <c r="A23" s="29"/>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
@@ -17931,7 +18092,7 @@
       <c r="AB26" s="89"/>
       <c r="AC26" s="89"/>
     </row>
-    <row r="27" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="27" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A27" s="55" t="s">
         <v>0</v>
       </c>
@@ -18288,23 +18449,23 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="68" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="66" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" style="66" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="66" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" style="66" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.88671875" style="66" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="66" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="66" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="66" customWidth="1"/>
-    <col min="19" max="19" width="27.5546875" style="66" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" style="66" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" style="73" customWidth="1"/>
-    <col min="22" max="22" width="11.44140625" style="66" customWidth="1"/>
-    <col min="23" max="26" width="11.44140625" style="66"/>
-    <col min="27" max="29" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="66" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="66" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="66" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="66" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="66" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="66" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="66" customWidth="1"/>
+    <col min="19" max="19" width="27.5703125" style="66" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="66" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="73" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" style="66" customWidth="1"/>
+    <col min="23" max="26" width="11.42578125" style="66"/>
+    <col min="27" max="29" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -18465,7 +18626,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="43.2">
+    <row r="3" spans="1:29" ht="45">
       <c r="A3" s="65">
         <v>29</v>
       </c>
@@ -18870,7 +19031,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -19196,18 +19357,18 @@
       <selection activeCell="AA6" sqref="AA6:AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="17" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5546875" style="111"/>
-    <col min="27" max="29" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" style="111"/>
+    <col min="27" max="29" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -19368,7 +19529,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="43.2">
+    <row r="3" spans="1:50" ht="45">
       <c r="A3" s="4">
         <v>30</v>
       </c>
@@ -19539,7 +19700,7 @@
       <c r="AB5" s="89"/>
       <c r="AC5" s="89"/>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:50" ht="30">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -19600,7 +19761,7 @@
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
     </row>
-    <row r="7" spans="1:50">
+    <row r="7" spans="1:50" ht="30">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -19767,7 +19928,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -20119,25 +20280,25 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="7" customWidth="1"/>
-    <col min="3" max="5" width="10.6640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" style="7" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="7" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="7" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="7"/>
-    <col min="19" max="19" width="25.109375" style="7" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" style="7" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" style="69" customWidth="1"/>
-    <col min="22" max="22" width="18.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.44140625" style="7"/>
-    <col min="24" max="25" width="11.44140625" style="69"/>
-    <col min="26" max="26" width="11.44140625" style="7"/>
-    <col min="27" max="29" width="23.44140625" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="7"/>
+    <col min="2" max="2" width="7.42578125" style="7" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="7" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="7" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="7"/>
+    <col min="19" max="19" width="25.140625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="7" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="69" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="7"/>
+    <col min="24" max="25" width="11.42578125" style="69"/>
+    <col min="26" max="26" width="11.42578125" style="7"/>
+    <col min="27" max="29" width="23.42578125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -20298,7 +20459,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="43.2">
+    <row r="3" spans="1:29" ht="45">
       <c r="A3" s="4">
         <v>31</v>
       </c>
@@ -20469,7 +20630,7 @@
       <c r="AB5" s="89"/>
       <c r="AC5" s="89"/>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" ht="30">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -20530,7 +20691,7 @@
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" ht="30">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -20697,7 +20858,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -21028,17 +21189,17 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="1.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="1.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5546875" style="111"/>
-    <col min="27" max="29" width="23.6640625" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" style="111"/>
+    <col min="27" max="29" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -21199,7 +21360,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="15" customFormat="1" ht="43.2">
+    <row r="3" spans="1:29" s="15" customFormat="1" ht="45">
       <c r="A3" s="65">
         <v>32</v>
       </c>
@@ -21618,7 +21779,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -21954,21 +22115,21 @@
       <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" style="54" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" style="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.88671875" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.6640625" style="54" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.44140625" style="54"/>
-    <col min="20" max="20" width="6.109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" style="54" customWidth="1"/>
-    <col min="22" max="26" width="11.44140625" style="54"/>
-    <col min="27" max="29" width="23.44140625" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="54"/>
+    <col min="2" max="2" width="11.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="54" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.7109375" style="54" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.42578125" style="54"/>
+    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="54" customWidth="1"/>
+    <col min="22" max="26" width="11.42578125" style="54"/>
+    <col min="27" max="29" width="23.42578125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -22129,7 +22290,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="3" spans="1:50" s="56" customFormat="1" ht="45">
       <c r="A3" s="55">
         <v>33</v>
       </c>
@@ -22584,7 +22745,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -22931,25 +23092,25 @@
       <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="80" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" style="15" customWidth="1"/>
-    <col min="3" max="5" width="10.6640625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="15" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="15" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.44140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" style="15" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" style="73" customWidth="1"/>
-    <col min="22" max="22" width="17.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.44140625" style="15"/>
-    <col min="24" max="25" width="11.44140625" style="73"/>
-    <col min="26" max="26" width="11.44140625" style="15"/>
-    <col min="27" max="29" width="23.5546875" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="15"/>
+    <col min="1" max="1" width="3.42578125" style="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="15" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="15" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="15" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" style="15" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="73" customWidth="1"/>
+    <col min="22" max="22" width="17.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="15"/>
+    <col min="24" max="25" width="11.42578125" style="73"/>
+    <col min="26" max="26" width="11.42578125" style="15"/>
+    <col min="27" max="29" width="23.5703125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -23110,7 +23271,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="43.2">
+    <row r="3" spans="1:50" ht="45">
       <c r="A3" s="55">
         <v>34</v>
       </c>
@@ -23555,7 +23716,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -23912,20 +24073,20 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" style="54" customWidth="1"/>
-    <col min="3" max="5" width="10.6640625" style="54" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" style="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="54" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="54" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.44140625" style="54"/>
-    <col min="20" max="20" width="6.109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="11.44140625" style="54"/>
-    <col min="27" max="29" width="23.21875" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="54"/>
+    <col min="1" max="1" width="3.140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="54" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" style="54" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="54" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.42578125" style="54"/>
+    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="11.42578125" style="54"/>
+    <col min="27" max="29" width="23.28515625" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -24086,7 +24247,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="56" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" s="56" customFormat="1" ht="45">
       <c r="A3" s="55">
         <v>35</v>
       </c>
@@ -24525,7 +24686,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -24879,25 +25040,25 @@
   <dimension ref="A1:AX14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.6640625" style="54" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" style="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.88671875" style="54" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="54" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="54" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="54"/>
-    <col min="19" max="19" width="41.44140625" style="54" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" style="54"/>
-    <col min="22" max="22" width="17.109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="11.44140625" style="54"/>
-    <col min="27" max="29" width="23.5546875" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="54"/>
+    <col min="1" max="1" width="3.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.7109375" style="54" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="54" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="54" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="54"/>
+    <col min="19" max="19" width="41.42578125" style="54" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="54"/>
+    <col min="22" max="22" width="17.140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="11.42578125" style="54"/>
+    <col min="27" max="29" width="23.5703125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -25058,7 +25219,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="56" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" s="56" customFormat="1" ht="45">
       <c r="A3" s="55">
         <v>36</v>
       </c>
@@ -25294,7 +25455,7 @@
       <c r="AW5"/>
       <c r="AX5"/>
     </row>
-    <row r="6" spans="1:50" s="56" customFormat="1">
+    <row r="6" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A6" s="55" t="s">
         <v>0</v>
       </c>
@@ -25345,7 +25506,9 @@
       <c r="Z6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AA6" s="159"/>
+      <c r="AA6" s="159" t="s">
+        <v>451</v>
+      </c>
       <c r="AB6" s="89"/>
       <c r="AC6" s="89"/>
       <c r="AD6"/>
@@ -25370,7 +25533,7 @@
       <c r="AW6"/>
       <c r="AX6"/>
     </row>
-    <row r="7" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="7" spans="1:50" s="56" customFormat="1">
       <c r="A7" s="55" t="s">
         <v>0</v>
       </c>
@@ -25419,9 +25582,7 @@
       <c r="Z7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AA7" s="159" t="s">
-        <v>451</v>
-      </c>
+      <c r="AA7" s="159"/>
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
       <c r="AD7"/>
@@ -25495,7 +25656,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -25540,11 +25701,13 @@
       </c>
       <c r="Y9" s="22"/>
       <c r="Z9" s="22"/>
-      <c r="AA9" s="159"/>
+      <c r="AA9" s="159" t="s">
+        <v>452</v>
+      </c>
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="10" spans="1:50" s="56" customFormat="1">
       <c r="A10" s="55" t="s">
         <v>0</v>
       </c>
@@ -25591,9 +25754,7 @@
       </c>
       <c r="Y10" s="22"/>
       <c r="Z10" s="133"/>
-      <c r="AA10" s="159" t="s">
-        <v>452</v>
-      </c>
+      <c r="AA10" s="89"/>
       <c r="AB10" s="89"/>
       <c r="AC10" s="89"/>
     </row>
@@ -25642,9 +25803,15 @@
       <c r="X11" s="24"/>
       <c r="Y11" s="24"/>
       <c r="Z11" s="24"/>
-      <c r="AA11" s="89"/>
-      <c r="AB11" s="89"/>
-      <c r="AC11" s="89"/>
+      <c r="AA11" s="89" t="s">
+        <v>454</v>
+      </c>
+      <c r="AB11" s="89" t="s">
+        <v>455</v>
+      </c>
+      <c r="AC11" s="89" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="12" spans="1:50" s="56" customFormat="1">
       <c r="A12" s="55" t="s">
@@ -25689,15 +25856,9 @@
       <c r="X12" s="22"/>
       <c r="Y12" s="22"/>
       <c r="Z12" s="22"/>
-      <c r="AA12" s="89" t="s">
-        <v>454</v>
-      </c>
-      <c r="AB12" s="89" t="s">
-        <v>455</v>
-      </c>
-      <c r="AC12" s="89" t="s">
-        <v>453</v>
-      </c>
+      <c r="AA12" s="89"/>
+      <c r="AB12" s="89"/>
+      <c r="AC12" s="89"/>
     </row>
     <row r="13" spans="1:50" s="56" customFormat="1">
       <c r="A13" s="55" t="s">
@@ -25843,26 +26004,26 @@
       <selection activeCell="AA15" sqref="AA15:AA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="10.6640625" style="15" customWidth="1"/>
-    <col min="9" max="9" width="2.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="16" width="3.6640625" style="15" customWidth="1"/>
-    <col min="17" max="17" width="3.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="10.7109375" style="15" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="16" width="3.7109375" style="15" customWidth="1"/>
+    <col min="17" max="17" width="3.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="15" customWidth="1"/>
     <col min="19" max="19" width="23" style="15" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" style="15" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" style="73" customWidth="1"/>
-    <col min="22" max="22" width="24.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.21875" style="15" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="15" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="73" customWidth="1"/>
+    <col min="22" max="22" width="24.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" style="15" customWidth="1"/>
     <col min="24" max="24" width="17" style="15" customWidth="1"/>
     <col min="25" max="25" width="22" style="15" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="15"/>
+    <col min="26" max="26" width="11.42578125" style="15"/>
     <col min="27" max="27" width="23" style="15" customWidth="1"/>
-    <col min="28" max="28" width="22.5546875" style="15" customWidth="1"/>
+    <col min="28" max="28" width="22.5703125" style="15" customWidth="1"/>
     <col min="29" max="29" width="23" style="15" customWidth="1"/>
-    <col min="30" max="16384" width="11.44140625" style="15"/>
+    <col min="30" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -26023,7 +26184,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="21" customFormat="1" ht="28.8">
+    <row r="3" spans="1:29" s="21" customFormat="1" ht="30">
       <c r="A3" s="58">
         <v>7</v>
       </c>
@@ -29677,23 +29838,23 @@
       <selection activeCell="AA36" sqref="AA36:AA39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.6640625" style="25" customWidth="1"/>
-    <col min="6" max="6" width="2.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="2.88671875" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="3.88671875" style="25" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.7109375" style="25" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="2.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="3.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" style="25" customWidth="1"/>
     <col min="19" max="19" width="37" style="25" customWidth="1"/>
-    <col min="20" max="20" width="8.21875" style="25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.88671875" style="54" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.44140625" style="87" customWidth="1"/>
-    <col min="23" max="23" width="43.44140625" style="87" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="95.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.21875" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="25"/>
-    <col min="27" max="29" width="23.88671875" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="87" customWidth="1"/>
+    <col min="23" max="23" width="43.42578125" style="87" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="95.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.28515625" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="25"/>
+    <col min="27" max="29" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -29854,7 +30015,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="43.2">
+    <row r="3" spans="1:29" ht="60">
       <c r="A3" s="56">
         <v>37</v>
       </c>
@@ -30381,7 +30542,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="12" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -30673,7 +30834,7 @@
       <c r="AB17" s="163"/>
       <c r="AC17" s="163"/>
     </row>
-    <row r="18" spans="1:29" ht="43.2">
+    <row r="18" spans="1:29" ht="60">
       <c r="A18" s="56">
         <v>38</v>
       </c>
@@ -31198,7 +31359,7 @@
       <c r="AB26" s="89"/>
       <c r="AC26" s="89"/>
     </row>
-    <row r="27" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="27" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A27" s="55" t="s">
         <v>0</v>
       </c>
@@ -31490,7 +31651,7 @@
       <c r="AB32" s="163"/>
       <c r="AC32" s="163"/>
     </row>
-    <row r="33" spans="1:29" ht="43.2">
+    <row r="33" spans="1:29" ht="60">
       <c r="A33" s="83">
         <v>39</v>
       </c>
@@ -32017,7 +32178,7 @@
       <c r="AB41" s="89"/>
       <c r="AC41" s="89"/>
     </row>
-    <row r="42" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="42" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A42" s="55" t="s">
         <v>0</v>
       </c>
@@ -32332,18 +32493,18 @@
       <selection activeCell="AA42" sqref="AA42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.21875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.6640625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="10" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="11.44140625" style="10"/>
-    <col min="24" max="24" width="13.6640625" style="10" customWidth="1"/>
-    <col min="25" max="25" width="11.88671875" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="10"/>
+    <col min="1" max="1" width="4.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="10" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="11.42578125" style="10"/>
+    <col min="24" max="24" width="13.7109375" style="10" customWidth="1"/>
+    <col min="25" max="25" width="11.85546875" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="10"/>
     <col min="27" max="29" width="24" customWidth="1"/>
   </cols>
   <sheetData>
@@ -32505,7 +32666,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="43.2">
+    <row r="3" spans="1:29" ht="45">
       <c r="A3" s="1">
         <v>40</v>
       </c>
@@ -32825,7 +32986,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -33135,7 +33296,7 @@
       <c r="AB14" s="163"/>
       <c r="AC14" s="163"/>
     </row>
-    <row r="15" spans="1:29" ht="43.2">
+    <row r="15" spans="1:29" ht="45">
       <c r="A15" s="1">
         <v>41</v>
       </c>
@@ -33457,7 +33618,7 @@
       <c r="AB20" s="89"/>
       <c r="AC20" s="89"/>
     </row>
-    <row r="21" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="21" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -33775,7 +33936,7 @@
       <c r="AB26" s="163"/>
       <c r="AC26" s="163"/>
     </row>
-    <row r="27" spans="1:29" ht="43.2">
+    <row r="27" spans="1:29" ht="45">
       <c r="A27" s="1">
         <v>42</v>
       </c>
@@ -34099,7 +34260,7 @@
       <c r="AB32" s="89"/>
       <c r="AC32" s="89"/>
     </row>
-    <row r="33" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="33" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A33" s="55" t="s">
         <v>0</v>
       </c>
@@ -34417,7 +34578,7 @@
       <c r="AB38" s="163"/>
       <c r="AC38" s="163"/>
     </row>
-    <row r="39" spans="1:29" ht="43.2">
+    <row r="39" spans="1:29" ht="45">
       <c r="A39" s="1">
         <v>43</v>
       </c>
@@ -34741,7 +34902,7 @@
       <c r="AB44" s="89"/>
       <c r="AC44" s="89"/>
     </row>
-    <row r="45" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="45" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A45" s="55" t="s">
         <v>0</v>
       </c>
@@ -35059,7 +35220,7 @@
       <c r="AB50" s="163"/>
       <c r="AC50" s="163"/>
     </row>
-    <row r="51" spans="1:29" ht="43.2">
+    <row r="51" spans="1:29" ht="45">
       <c r="A51" s="1">
         <v>44</v>
       </c>
@@ -35383,7 +35544,7 @@
       <c r="AB56" s="89"/>
       <c r="AC56" s="89"/>
     </row>
-    <row r="57" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="57" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A57" s="55" t="s">
         <v>0</v>
       </c>
@@ -35701,7 +35862,7 @@
       <c r="AB62" s="163"/>
       <c r="AC62" s="163"/>
     </row>
-    <row r="63" spans="1:29" ht="43.2">
+    <row r="63" spans="1:29" ht="60">
       <c r="A63" s="1">
         <v>45</v>
       </c>
@@ -36025,7 +36186,7 @@
       <c r="AB68" s="89"/>
       <c r="AC68" s="89"/>
     </row>
-    <row r="69" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="69" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A69" s="55" t="s">
         <v>0</v>
       </c>
@@ -36343,7 +36504,7 @@
       <c r="AB74" s="163"/>
       <c r="AC74" s="163"/>
     </row>
-    <row r="75" spans="1:29" ht="43.2">
+    <row r="75" spans="1:29" ht="60">
       <c r="A75" s="1">
         <v>46</v>
       </c>
@@ -36667,7 +36828,7 @@
       <c r="AB80" s="89"/>
       <c r="AC80" s="89"/>
     </row>
-    <row r="81" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="81" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A81" s="55" t="s">
         <v>0</v>
       </c>
@@ -36985,7 +37146,7 @@
       <c r="AB86" s="199"/>
       <c r="AC86" s="199"/>
     </row>
-    <row r="87" spans="1:29" ht="28.8">
+    <row r="87" spans="1:29" ht="45">
       <c r="A87" s="1">
         <v>47</v>
       </c>
@@ -37309,7 +37470,7 @@
       <c r="AB92" s="89"/>
       <c r="AC92" s="89"/>
     </row>
-    <row r="93" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="93" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A93" s="55" t="s">
         <v>0</v>
       </c>
@@ -37652,22 +37813,22 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.6640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.88671875" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="10" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="10" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.88671875" style="10" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.44140625" style="10"/>
-    <col min="24" max="25" width="13.88671875" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="10"/>
+    <col min="19" max="19" width="16.85546875" style="10" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11.42578125" style="10"/>
+    <col min="24" max="25" width="13.85546875" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="10"/>
     <col min="27" max="29" width="23" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="10"/>
+    <col min="51" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -37828,7 +37989,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" customFormat="1" ht="45">
       <c r="A3" s="1">
         <v>48</v>
       </c>
@@ -38514,23 +38675,23 @@
       <selection activeCell="AA43" sqref="AA43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="10" customWidth="1"/>
     <col min="4" max="4" width="10" style="10" customWidth="1"/>
-    <col min="5" max="6" width="1.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.6640625" style="10" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.44140625" style="10"/>
-    <col min="20" max="20" width="9.109375" style="10" customWidth="1"/>
-    <col min="21" max="23" width="11.44140625" style="10"/>
-    <col min="24" max="24" width="17.5546875" style="10" customWidth="1"/>
+    <col min="5" max="6" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.7109375" style="10" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.42578125" style="10"/>
+    <col min="20" max="20" width="9.140625" style="10" customWidth="1"/>
+    <col min="21" max="23" width="11.42578125" style="10"/>
+    <col min="24" max="24" width="17.5703125" style="10" customWidth="1"/>
     <col min="25" max="25" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="10"/>
-    <col min="27" max="29" width="24.6640625" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="10"/>
+    <col min="26" max="26" width="11.42578125" style="10"/>
+    <col min="27" max="29" width="24.7109375" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -38691,7 +38852,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:29" customFormat="1" ht="43.2">
+    <row r="3" spans="1:29" customFormat="1" ht="45">
       <c r="A3" s="1">
         <v>49</v>
       </c>
@@ -39472,7 +39633,7 @@
       <c r="AB17" s="89"/>
       <c r="AC17" s="89"/>
     </row>
-    <row r="18" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="18" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A18" s="55" t="s">
         <v>0</v>
       </c>
@@ -39801,7 +39962,7 @@
       <c r="AW23"/>
       <c r="AX23"/>
     </row>
-    <row r="24" spans="1:50" customFormat="1" ht="43.2">
+    <row r="24" spans="1:50" customFormat="1" ht="45">
       <c r="A24" s="1">
         <v>50</v>
       </c>
@@ -40582,7 +40743,7 @@
       <c r="AB38" s="89"/>
       <c r="AC38" s="89"/>
     </row>
-    <row r="39" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="39" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A39" s="55" t="s">
         <v>0</v>
       </c>
@@ -40930,19 +41091,19 @@
       <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.6640625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14" customWidth="1"/>
     <col min="25" max="25" width="14" style="111" customWidth="1"/>
-    <col min="27" max="29" width="23.109375" customWidth="1"/>
+    <col min="27" max="29" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -41103,7 +41264,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="10" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" s="10" customFormat="1" ht="45">
       <c r="A3" s="1">
         <v>51</v>
       </c>
@@ -41541,7 +41702,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -41889,23 +42050,23 @@
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="17" width="2.6640625" style="10" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="11.44140625" style="10"/>
-    <col min="20" max="20" width="6.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.44140625" style="10"/>
-    <col min="24" max="25" width="9.44140625" style="10" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="10"/>
-    <col min="27" max="29" width="23.6640625" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="10"/>
+    <col min="1" max="1" width="3.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="17" width="2.7109375" style="10" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.42578125" style="10"/>
+    <col min="20" max="20" width="6.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="11.42578125" style="10"/>
+    <col min="24" max="25" width="9.42578125" style="10" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="10"/>
+    <col min="27" max="29" width="23.7109375" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -42066,7 +42227,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" customFormat="1" ht="45">
       <c r="A3" s="1">
         <v>52</v>
       </c>
@@ -42398,7 +42559,7 @@
       <c r="AB8" s="89"/>
       <c r="AC8" s="89"/>
     </row>
-    <row r="9" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="9" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
@@ -42727,7 +42888,7 @@
       <c r="AW14"/>
       <c r="AX14"/>
     </row>
-    <row r="15" spans="1:50" customFormat="1" ht="43.2">
+    <row r="15" spans="1:50" customFormat="1" ht="45">
       <c r="A15" s="1">
         <v>53</v>
       </c>
@@ -43056,7 +43217,7 @@
       <c r="AB20" s="89"/>
       <c r="AC20" s="89"/>
     </row>
-    <row r="21" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="21" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A21" s="55" t="s">
         <v>0</v>
       </c>
@@ -43400,22 +43561,22 @@
       <selection activeCell="AA38" sqref="AA38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="1.88671875" customWidth="1"/>
-    <col min="9" max="9" width="1.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="10.109375" style="10" customWidth="1"/>
-    <col min="27" max="29" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="1.85546875" customWidth="1"/>
+    <col min="9" max="9" width="1.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.140625" style="10" customWidth="1"/>
+    <col min="27" max="29" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -43576,7 +43737,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="10" customFormat="1" ht="43.2">
+    <row r="3" spans="1:50" s="10" customFormat="1" ht="60">
       <c r="A3" s="1">
         <v>54</v>
       </c>
@@ -43898,7 +44059,7 @@
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
     </row>
-    <row r="8" spans="1:50" ht="43.2">
+    <row r="8" spans="1:50" ht="45">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -44106,7 +44267,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="12" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -44435,7 +44596,7 @@
       <c r="AW17"/>
       <c r="AX17"/>
     </row>
-    <row r="18" spans="1:50" s="10" customFormat="1" ht="43.2">
+    <row r="18" spans="1:50" s="10" customFormat="1" ht="60">
       <c r="A18" s="1">
         <v>55</v>
       </c>
@@ -44755,7 +44916,7 @@
       <c r="AB22" s="89"/>
       <c r="AC22" s="89"/>
     </row>
-    <row r="23" spans="1:50" ht="43.2">
+    <row r="23" spans="1:50" ht="45">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -44961,7 +45122,7 @@
       <c r="AB26" s="89"/>
       <c r="AC26" s="89"/>
     </row>
-    <row r="27" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="27" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A27" s="55" t="s">
         <v>0</v>
       </c>
@@ -45290,7 +45451,7 @@
       <c r="AW32"/>
       <c r="AX32"/>
     </row>
-    <row r="33" spans="1:50" s="10" customFormat="1" ht="57.6">
+    <row r="33" spans="1:50" s="10" customFormat="1" ht="60">
       <c r="A33" s="1">
         <v>56</v>
       </c>
@@ -45612,7 +45773,7 @@
       <c r="AB37" s="89"/>
       <c r="AC37" s="89"/>
     </row>
-    <row r="38" spans="1:50" ht="43.2">
+    <row r="38" spans="1:50" ht="45">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -45820,7 +45981,7 @@
       <c r="AB41" s="89"/>
       <c r="AC41" s="89"/>
     </row>
-    <row r="42" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="42" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A42" s="55" t="s">
         <v>0</v>
       </c>
@@ -46173,24 +46334,24 @@
       <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="39" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="39" customWidth="1"/>
-    <col min="19" max="23" width="11.44140625" style="39"/>
-    <col min="24" max="24" width="46.21875" style="97" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
+    <col min="19" max="23" width="11.42578125" style="39"/>
+    <col min="24" max="24" width="46.28515625" style="97" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="39"/>
-    <col min="27" max="29" width="24.44140625" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="39"/>
+    <col min="26" max="26" width="11.42578125" style="39"/>
+    <col min="27" max="29" width="24.42578125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -46351,7 +46512,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="97" customFormat="1">
+    <row r="3" spans="1:50" s="97" customFormat="1" ht="30">
       <c r="A3" s="29">
         <v>57</v>
       </c>
@@ -46972,7 +47133,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="12" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A12" s="55" t="s">
         <v>0</v>
       </c>
@@ -47816,27 +47977,27 @@
       <selection activeCell="AA21" sqref="AA21:AC21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" style="38" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" style="38" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="38" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="38" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="38" customWidth="1"/>
     <col min="5" max="5" width="10" style="38" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="38" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="38" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="38" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="38" customWidth="1"/>
-    <col min="19" max="19" width="49.5546875" style="38" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" style="38"/>
-    <col min="21" max="21" width="11.44140625" style="97"/>
-    <col min="22" max="22" width="11.44140625" style="38"/>
-    <col min="23" max="23" width="36.21875" style="38" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="11.6640625" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="38"/>
-    <col min="27" max="29" width="23.109375" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="38"/>
+    <col min="6" max="6" width="1.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="38" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="38" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="38" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="38" customWidth="1"/>
+    <col min="19" max="19" width="49.5703125" style="38" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="38"/>
+    <col min="21" max="21" width="11.42578125" style="97"/>
+    <col min="22" max="22" width="11.42578125" style="38"/>
+    <col min="23" max="23" width="36.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="11.7109375" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="38"/>
+    <col min="27" max="29" width="23.140625" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -49034,7 +49195,7 @@
       <c r="AB18" s="89"/>
       <c r="AC18" s="89"/>
     </row>
-    <row r="19" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="19" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A19" s="55" t="s">
         <v>0</v>
       </c>
@@ -50000,26 +50161,26 @@
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="39" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.44140625" style="39"/>
-    <col min="21" max="21" width="11.44140625" style="97"/>
-    <col min="22" max="23" width="11.44140625" style="39"/>
+    <col min="6" max="6" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" style="39"/>
+    <col min="21" max="21" width="11.42578125" style="97"/>
+    <col min="22" max="23" width="11.42578125" style="39"/>
     <col min="24" max="24" width="23" style="97" customWidth="1"/>
-    <col min="25" max="25" width="13.44140625" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="39"/>
-    <col min="27" max="29" width="23.88671875" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="39"/>
+    <col min="25" max="25" width="13.42578125" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="39"/>
+    <col min="27" max="29" width="23.85546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -50180,7 +50341,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="97" customFormat="1" ht="28.8">
+    <row r="3" spans="1:50" s="97" customFormat="1" ht="30">
       <c r="A3" s="29">
         <v>59</v>
       </c>
@@ -50863,7 +51024,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="13" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -51827,29 +51988,29 @@
       <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.21875" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="25" customWidth="1"/>
     <col min="4" max="4" width="6" style="25" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" style="25" customWidth="1"/>
-    <col min="6" max="7" width="8.6640625" style="25" customWidth="1"/>
-    <col min="8" max="8" width="2.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.5546875" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="3.5546875" style="25" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="3.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.44140625" style="25"/>
-    <col min="20" max="20" width="11.44140625" style="25" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" style="54" customWidth="1"/>
-    <col min="22" max="22" width="11.44140625" style="25"/>
-    <col min="23" max="23" width="36.21875" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="47.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.88671875" style="25" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="25"/>
-    <col min="27" max="27" width="22.88671875" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" style="25" customWidth="1"/>
+    <col min="6" max="7" width="8.7109375" style="25" customWidth="1"/>
+    <col min="8" max="8" width="2.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5703125" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="3.5703125" style="25" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="3.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.42578125" style="25"/>
+    <col min="20" max="20" width="11.42578125" style="25" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="54" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" style="25"/>
+    <col min="23" max="23" width="36.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="47.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" style="25" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="25"/>
+    <col min="27" max="27" width="22.85546875" customWidth="1"/>
     <col min="28" max="29" width="23" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="25"/>
+    <col min="51" max="16384" width="11.42578125" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="71" customFormat="1">
@@ -56725,20 +56886,20 @@
       <selection activeCell="AA7" sqref="AA7:AB9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.6640625" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" style="111" customWidth="1"/>
-    <col min="27" max="29" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.7109375" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" style="111" customWidth="1"/>
+    <col min="27" max="29" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -57359,7 +57520,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:29" s="56" customFormat="1" ht="28.8">
+    <row r="13" spans="1:29" s="56" customFormat="1" ht="30">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -58100,25 +58261,25 @@
       <selection activeCell="AA7" sqref="AA7:AB9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" style="39" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" style="39" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="39" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="39" customWidth="1"/>
     <col min="5" max="5" width="10" style="39" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.44140625" style="39"/>
-    <col min="21" max="21" width="11.44140625" style="97"/>
-    <col min="22" max="23" width="11.44140625" style="39"/>
-    <col min="24" max="25" width="11.44140625" style="97"/>
-    <col min="26" max="26" width="11.44140625" style="39"/>
-    <col min="27" max="29" width="23.88671875" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="39"/>
+    <col min="6" max="6" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" style="39"/>
+    <col min="21" max="21" width="11.42578125" style="97"/>
+    <col min="22" max="23" width="11.42578125" style="39"/>
+    <col min="24" max="25" width="11.42578125" style="97"/>
+    <col min="26" max="26" width="11.42578125" style="39"/>
+    <col min="27" max="29" width="23.85546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -58928,7 +59089,7 @@
       <c r="AB12" s="89"/>
       <c r="AC12" s="89"/>
     </row>
-    <row r="13" spans="1:50" s="56" customFormat="1" ht="28.8">
+    <row r="13" spans="1:50" s="56" customFormat="1" ht="30">
       <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
@@ -59276,24 +59437,24 @@
       <selection activeCell="AA1" sqref="AA1:AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.6640625" style="39" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" style="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.88671875" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="39" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="39" customWidth="1"/>
-    <col min="19" max="20" width="11.44140625" style="39"/>
-    <col min="21" max="21" width="11.44140625" style="97"/>
-    <col min="22" max="22" width="12.88671875" style="39" customWidth="1"/>
-    <col min="23" max="23" width="11.44140625" style="39"/>
-    <col min="24" max="24" width="12.88671875" style="97" customWidth="1"/>
-    <col min="25" max="25" width="12.109375" style="97" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="39"/>
-    <col min="27" max="29" width="23.5546875" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="39"/>
+    <col min="2" max="4" width="10.7109375" style="39" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="39" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="39" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="39" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" style="39"/>
+    <col min="21" max="21" width="11.42578125" style="97"/>
+    <col min="22" max="22" width="12.85546875" style="39" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="39"/>
+    <col min="24" max="24" width="12.85546875" style="97" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" style="97" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="39"/>
+    <col min="27" max="29" width="23.5703125" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -60374,17 +60535,17 @@
   <sheetPr codeName="Hoja34"/>
   <dimension ref="A1:AX17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.44140625" style="111"/>
-    <col min="26" max="26" width="11.21875" customWidth="1"/>
-    <col min="27" max="29" width="22.5546875" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" style="111"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+    <col min="27" max="29" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -61470,19 +61631,22 @@
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <sheetPr codeName="Hoja35"/>
-  <dimension ref="A1:AX7"/>
+  <dimension ref="A1:AX23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S35" sqref="S35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="15.88671875" customWidth="1"/>
-    <col min="20" max="20" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.44140625" style="111"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" style="111"/>
+    <col min="27" max="27" width="26.5703125" customWidth="1"/>
+    <col min="28" max="28" width="20.85546875" customWidth="1"/>
+    <col min="29" max="29" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -61564,6 +61728,9 @@
       <c r="Z1" s="141">
         <v>26</v>
       </c>
+      <c r="AA1" s="239"/>
+      <c r="AB1" s="241"/>
+      <c r="AC1" s="241"/>
     </row>
     <row r="2" spans="1:50" s="25" customFormat="1">
       <c r="A2" s="55" t="s">
@@ -61624,6 +61791,9 @@
       <c r="Z2" s="14" t="s">
         <v>7</v>
       </c>
+      <c r="AA2" s="240"/>
+      <c r="AB2" s="240"/>
+      <c r="AC2" s="240"/>
     </row>
     <row r="3" spans="1:50" s="97" customFormat="1">
       <c r="A3" s="29">
@@ -61674,9 +61844,9 @@
       <c r="Z3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="AA3" s="111"/>
-      <c r="AB3" s="111"/>
-      <c r="AC3" s="111"/>
+      <c r="AA3" s="229"/>
+      <c r="AB3" s="229"/>
+      <c r="AC3" s="229"/>
       <c r="AD3" s="111"/>
       <c r="AE3" s="111"/>
       <c r="AF3" s="111"/>
@@ -61746,9 +61916,9 @@
       <c r="Z4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="AA4" s="111"/>
-      <c r="AB4" s="111"/>
-      <c r="AC4" s="111"/>
+      <c r="AA4" s="229"/>
+      <c r="AB4" s="229"/>
+      <c r="AC4" s="229"/>
       <c r="AD4" s="111"/>
       <c r="AE4" s="111"/>
       <c r="AF4" s="111"/>
@@ -61818,9 +61988,9 @@
       </c>
       <c r="Y5" s="101"/>
       <c r="Z5" s="145"/>
-      <c r="AA5" s="111"/>
-      <c r="AB5" s="111"/>
-      <c r="AC5" s="111"/>
+      <c r="AA5" s="229"/>
+      <c r="AB5" s="229"/>
+      <c r="AC5" s="229"/>
       <c r="AD5" s="111"/>
       <c r="AE5" s="111"/>
       <c r="AF5" s="111"/>
@@ -61872,9 +62042,9 @@
       <c r="X6" s="99"/>
       <c r="Y6" s="99"/>
       <c r="Z6" s="100"/>
-      <c r="AA6" s="111"/>
-      <c r="AB6" s="111"/>
-      <c r="AC6" s="111"/>
+      <c r="AA6" s="229"/>
+      <c r="AB6" s="229"/>
+      <c r="AC6" s="229"/>
       <c r="AD6" s="111"/>
       <c r="AE6" s="111"/>
       <c r="AF6" s="111"/>
@@ -61952,9 +62122,9 @@
       <c r="Z7" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="AA7" s="111"/>
-      <c r="AB7" s="111"/>
-      <c r="AC7" s="111"/>
+      <c r="AA7" s="229"/>
+      <c r="AB7" s="229"/>
+      <c r="AC7" s="229"/>
       <c r="AD7" s="111"/>
       <c r="AE7" s="111"/>
       <c r="AF7" s="111"/>
@@ -61977,8 +62147,90 @@
       <c r="AW7" s="111"/>
       <c r="AX7" s="111"/>
     </row>
+    <row r="8" spans="1:50">
+      <c r="AA8" s="236"/>
+      <c r="AB8" s="229"/>
+      <c r="AC8" s="229"/>
+      <c r="AD8" s="228"/>
+    </row>
+    <row r="9" spans="1:50">
+      <c r="AA9" s="236"/>
+      <c r="AB9" s="229"/>
+      <c r="AC9" s="231"/>
+    </row>
+    <row r="10" spans="1:50">
+      <c r="AA10" s="237"/>
+      <c r="AB10" s="230"/>
+      <c r="AC10" s="230"/>
+    </row>
+    <row r="11" spans="1:50">
+      <c r="Z11" s="238"/>
+      <c r="AA11" s="237"/>
+      <c r="AB11" s="231"/>
+      <c r="AC11" s="229"/>
+    </row>
+    <row r="12" spans="1:50">
+      <c r="AA12" s="237"/>
+      <c r="AB12" s="230"/>
+      <c r="AC12" s="229"/>
+    </row>
+    <row r="13" spans="1:50">
+      <c r="AA13" s="237"/>
+      <c r="AB13" s="230"/>
+      <c r="AC13" s="230"/>
+    </row>
+    <row r="14" spans="1:50">
+      <c r="Z14" s="225"/>
+      <c r="AA14" s="237"/>
+      <c r="AB14" s="230"/>
+      <c r="AC14" s="230"/>
+    </row>
+    <row r="15" spans="1:50">
+      <c r="AA15" s="237"/>
+      <c r="AB15" s="229"/>
+      <c r="AC15" s="230"/>
+      <c r="AD15" s="228"/>
+    </row>
+    <row r="16" spans="1:50">
+      <c r="AA16" s="237"/>
+      <c r="AB16" s="230"/>
+      <c r="AC16" s="230"/>
+      <c r="AD16" s="227"/>
+    </row>
+    <row r="17" spans="25:29">
+      <c r="Y17" s="228"/>
+      <c r="AA17" s="236"/>
+      <c r="AB17" s="230"/>
+      <c r="AC17" s="231"/>
+    </row>
+    <row r="18" spans="25:29">
+      <c r="AA18" s="233"/>
+      <c r="AB18" s="226"/>
+      <c r="AC18" s="226"/>
+    </row>
+    <row r="19" spans="25:29">
+      <c r="AA19" s="232"/>
+      <c r="AB19" s="234"/>
+    </row>
+    <row r="20" spans="25:29">
+      <c r="Z20" s="235"/>
+      <c r="AB20" s="228"/>
+    </row>
+    <row r="21" spans="25:29">
+      <c r="Y21" s="235"/>
+      <c r="AA21" s="228"/>
+    </row>
+    <row r="22" spans="25:29">
+      <c r="Y22" s="225"/>
+      <c r="AA22" s="228"/>
+      <c r="AB22" s="228"/>
+    </row>
+    <row r="23" spans="25:29">
+      <c r="Z23" s="235"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -61991,23 +62243,23 @@
       <selection activeCell="AA83" sqref="AA83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.6640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" style="7" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="7" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="11.44140625" style="7"/>
-    <col min="21" max="21" width="11.44140625" style="69"/>
-    <col min="22" max="22" width="11.44140625" style="7"/>
-    <col min="23" max="23" width="37.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="54.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.44140625" style="7" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="7"/>
-    <col min="27" max="29" width="22.88671875" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="7"/>
+    <col min="1" max="1" width="3.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="7" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="11.42578125" style="7"/>
+    <col min="21" max="21" width="11.42578125" style="69"/>
+    <col min="22" max="22" width="11.42578125" style="7"/>
+    <col min="23" max="23" width="37.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="54.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" style="7" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="7"/>
+    <col min="27" max="29" width="22.85546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="71" customFormat="1">
@@ -68012,19 +68264,19 @@
       <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="1.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="1.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" style="10" customWidth="1"/>
-    <col min="23" max="23" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.44140625" style="111"/>
-    <col min="27" max="29" width="22.88671875" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="1.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="10" customWidth="1"/>
+    <col min="23" max="23" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" style="111"/>
+    <col min="27" max="29" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -71113,18 +71365,18 @@
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="1.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" customWidth="1"/>
-    <col min="24" max="24" width="8.109375" customWidth="1"/>
-    <col min="25" max="25" width="8.109375" style="111" customWidth="1"/>
-    <col min="27" max="29" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" style="111" customWidth="1"/>
+    <col min="27" max="29" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -73352,21 +73604,21 @@
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="1.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="11.44140625" style="2"/>
-    <col min="23" max="23" width="35.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.44140625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="10.44140625" style="113" customWidth="1"/>
-    <col min="26" max="26" width="11.44140625" style="2"/>
-    <col min="27" max="29" width="22.88671875" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="2"/>
+    <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="11.42578125" style="2"/>
+    <col min="23" max="23" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" style="113" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="2"/>
+    <col min="27" max="29" width="22.85546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -74777,16 +75029,16 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.6640625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="1.88671875" style="38" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="38" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="18" max="26" width="11.44140625" style="38"/>
-    <col min="27" max="29" width="22.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.7109375" style="38" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="1.85546875" style="38" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="38" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="18" max="26" width="11.42578125" style="38"/>
+    <col min="27" max="29" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="142" customFormat="1">
@@ -75627,20 +75879,20 @@
       <selection activeCell="AA3" sqref="AA3:AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.6640625" style="56" customWidth="1"/>
-    <col min="7" max="7" width="1.88671875" style="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="1.88671875" style="56" hidden="1" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="56" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="56" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" style="56"/>
-    <col min="19" max="19" width="30.21875" style="56" customWidth="1"/>
-    <col min="20" max="21" width="11.44140625" style="56" customWidth="1"/>
-    <col min="22" max="26" width="11.44140625" style="56"/>
-    <col min="27" max="29" width="22.88671875" customWidth="1"/>
-    <col min="51" max="16384" width="11.44140625" style="56"/>
+    <col min="1" max="1" width="3.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" style="56" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="1.85546875" style="56" hidden="1" customWidth="1"/>
+    <col min="10" max="16" width="2.7109375" style="56" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="56" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="56"/>
+    <col min="19" max="19" width="30.28515625" style="56" customWidth="1"/>
+    <col min="20" max="21" width="11.42578125" style="56" customWidth="1"/>
+    <col min="22" max="26" width="11.42578125" style="56"/>
+    <col min="27" max="29" width="22.85546875" customWidth="1"/>
+    <col min="51" max="16384" width="11.42578125" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" s="142" customFormat="1">
@@ -76085,7 +76337,7 @@
       <c r="AB7" s="89"/>
       <c r="AC7" s="89"/>
     </row>
-    <row r="8" spans="1:50" ht="28.8">
+    <row r="8" spans="1:50" ht="30">
       <c r="B8" s="45" t="s">
         <v>0</v>
       </c>
@@ -76193,7 +76445,7 @@
       <c r="AB9" s="89"/>
       <c r="AC9" s="89"/>
     </row>
-    <row r="10" spans="1:50" s="130" customFormat="1" ht="28.8">
+    <row r="10" spans="1:50" s="130" customFormat="1" ht="30">
       <c r="B10" s="45" t="s">
         <v>0</v>
       </c>
@@ -76308,7 +76560,7 @@
       <c r="AB11" s="89"/>
       <c r="AC11" s="89"/>
     </row>
-    <row r="12" spans="1:50" ht="28.8">
+    <row r="12" spans="1:50" ht="30">
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
@@ -76598,7 +76850,7 @@
       <c r="AW17" s="56"/>
       <c r="AX17" s="56"/>
     </row>
-    <row r="18" spans="1:50" ht="28.8">
+    <row r="18" spans="1:50" ht="30">
       <c r="A18" s="55" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
-fixed an issue, where missing criterion property keys has been added in v210 Regulated taxonomy in OTHER.EO criteria. Related keys added in ESPD_en.json/xml and in ESPD_el.json/xml. -fixed an issue, where description property keys were in wrong column for OTHER.EO criteria. Moved from pk1 to pk2 column and now pk1 column = name, pk2 column = description like the oher criteria. -fixed an issue, where NullPointerException would be thrown during PDF v1 export process.
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0_Property_0.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NetbeansProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B3D435-42E9-45D4-AC2C-591A126859FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067CFE38-02BF-43CC-9410-3FBE16CAEA86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="135" windowWidth="29205" windowHeight="15435" tabRatio="588" firstSheet="29" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="285" yWindow="180" windowWidth="29205" windowHeight="15435" tabRatio="588" firstSheet="30" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12441" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12448" uniqueCount="623">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1912,6 +1912,27 @@
   </si>
   <si>
     <t>espd.crit.other.eo.part</t>
+  </si>
+  <si>
+    <t>espd.part2.if.proc.reserved.main</t>
+  </si>
+  <si>
+    <t>espd.part2.eo.approved.cert.main</t>
+  </si>
+  <si>
+    <t>espd.part2.is.eo.proc.together.main</t>
+  </si>
+  <si>
+    <t>espd.part2.eo.rely.other.entities.main</t>
+  </si>
+  <si>
+    <t>espd.part2.information.subcontractors.main</t>
+  </si>
+  <si>
+    <t>espd.part2.lots.concerned.main</t>
+  </si>
+  <si>
+    <t>espd.part5.title.eo.declares.that.main</t>
   </si>
 </sst>
 </file>
@@ -42047,7 +42068,7 @@
   <dimension ref="A1:AX26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -43557,8 +43578,8 @@
   <sheetPr codeName="Hoja26"/>
   <dimension ref="A1:AX47"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA38" sqref="AA38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -46331,7 +46352,7 @@
   <dimension ref="A1:AX141"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -46562,9 +46583,11 @@
         <v>0</v>
       </c>
       <c r="AA3" s="178" t="s">
+        <v>616</v>
+      </c>
+      <c r="AB3" s="178" t="s">
         <v>591</v>
       </c>
-      <c r="AB3" s="172"/>
       <c r="AC3" s="172"/>
       <c r="AD3"/>
       <c r="AE3"/>
@@ -47974,7 +47997,7 @@
   <dimension ref="A1:AX148"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AA21" sqref="AA21:AC21"/>
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -48208,9 +48231,11 @@
         <v>0</v>
       </c>
       <c r="AA3" s="163" t="s">
+        <v>617</v>
+      </c>
+      <c r="AB3" s="163" t="s">
         <v>592</v>
       </c>
-      <c r="AB3" s="163"/>
       <c r="AC3" s="163"/>
       <c r="AD3"/>
       <c r="AE3"/>
@@ -50158,7 +50183,7 @@
   <dimension ref="A1:AX142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -50391,9 +50416,11 @@
         <v>0</v>
       </c>
       <c r="AA3" s="158" t="s">
+        <v>618</v>
+      </c>
+      <c r="AB3" s="158" t="s">
         <v>598</v>
       </c>
-      <c r="AB3" s="163"/>
       <c r="AC3" s="163"/>
       <c r="AD3"/>
       <c r="AE3"/>
@@ -56883,7 +56910,7 @@
   <dimension ref="A1:AC38"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7:AB9"/>
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -57110,9 +57137,11 @@
         <v>0</v>
       </c>
       <c r="AA3" s="163" t="s">
+        <v>619</v>
+      </c>
+      <c r="AB3" s="163" t="s">
         <v>600</v>
       </c>
-      <c r="AB3" s="215"/>
       <c r="AC3" s="215"/>
     </row>
     <row r="4" spans="1:29">
@@ -58258,7 +58287,7 @@
   <dimension ref="A1:AX18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7:AB9"/>
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -58490,9 +58519,11 @@
         <v>0</v>
       </c>
       <c r="AA3" s="163" t="s">
+        <v>620</v>
+      </c>
+      <c r="AB3" s="163" t="s">
         <v>601</v>
       </c>
-      <c r="AB3" s="163"/>
       <c r="AC3" s="163"/>
       <c r="AD3"/>
       <c r="AE3"/>
@@ -59434,7 +59465,7 @@
   <dimension ref="A1:AX131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AC2"/>
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -59665,9 +59696,11 @@
         <v>0</v>
       </c>
       <c r="AA3" s="163" t="s">
+        <v>621</v>
+      </c>
+      <c r="AB3" s="163" t="s">
         <v>602</v>
       </c>
-      <c r="AB3" s="163"/>
       <c r="AC3" s="163"/>
       <c r="AD3"/>
       <c r="AE3"/>
@@ -60535,8 +60568,8 @@
   <sheetPr codeName="Hoja34"/>
   <dimension ref="A1:AX17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -60756,9 +60789,11 @@
         <v>0</v>
       </c>
       <c r="AA3" s="163" t="s">
+        <v>622</v>
+      </c>
+      <c r="AB3" s="163" t="s">
         <v>603</v>
       </c>
-      <c r="AB3" s="163"/>
       <c r="AC3" s="163"/>
       <c r="AD3" s="111"/>
       <c r="AE3" s="111"/>
@@ -61633,7 +61668,7 @@
   <sheetPr codeName="Hoja35"/>
   <dimension ref="A1:AX23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>

</xml_diff>